<commit_message>
Aggiunti al file Excel i run del 04/02/2020. Aggiunte tutti i grafici finora prodotti
</commit_message>
<xml_diff>
--- a/Caratterizzazione_THGEM.xlsx
+++ b/Caratterizzazione_THGEM.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peppe\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peppe\Desktop\LaTex\Report_THGEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B017533A-43BC-4A76-94F0-C44D6C9D8244}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EB40F4-7712-4355-A012-220B489DD874}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{ACFC7C87-C28D-4487-B063-88156E979354}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ACFC7C87-C28D-4487-B063-88156E979354}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
     <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="81">
   <si>
     <t>DATA</t>
   </si>
@@ -566,6 +566,57 @@
       </rPr>
       <t>) per scariche su catodo</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">354 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>÷ 363</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">364 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>÷ 378</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">379 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>÷ 396</t>
+    </r>
+  </si>
+  <si>
+    <t>VTG=210     Vdrift=800</t>
+  </si>
+  <si>
+    <t>Vind=80        VTG=210</t>
+  </si>
+  <si>
+    <t>Vind=50        VTG=180</t>
   </si>
 </sst>
 </file>
@@ -735,7 +786,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -773,15 +824,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -798,9 +840,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -840,6 +879,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1158,8 +1206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C87521-6C72-4CB0-A78B-1EAFA58AC3F8}">
   <dimension ref="A1:BI55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1274,7 +1322,7 @@
       <c r="E2" s="13">
         <v>30.2</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="19" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="13">
@@ -1355,7 +1403,7 @@
       <c r="E3" s="13">
         <v>30.4</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="20" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="13">
@@ -1436,7 +1484,7 @@
       <c r="E4" s="13">
         <v>30.4</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="21" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="13">
@@ -1517,7 +1565,7 @@
       <c r="E5" s="13">
         <v>30.4</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="19" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="13">
@@ -1598,7 +1646,7 @@
       <c r="E6" s="13">
         <v>30.4</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="19" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="13">
@@ -1679,7 +1727,7 @@
       <c r="E7" s="13">
         <v>20.5</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="19" t="s">
         <v>11</v>
       </c>
       <c r="G7" s="13">
@@ -1760,7 +1808,7 @@
       <c r="E8" s="13">
         <v>20.5</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="20" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="13">
@@ -1841,7 +1889,7 @@
       <c r="E9" s="13">
         <v>20.5</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="21" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="13">
@@ -1922,7 +1970,7 @@
       <c r="E10" s="13">
         <v>11</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="19" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="13">
@@ -2003,7 +2051,7 @@
       <c r="E11" s="13">
         <v>11</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="19" t="s">
         <v>11</v>
       </c>
       <c r="G11" s="13">
@@ -2084,7 +2132,7 @@
       <c r="E12" s="13">
         <v>11</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="19" t="s">
         <v>11</v>
       </c>
       <c r="G12" s="13">
@@ -2165,7 +2213,7 @@
       <c r="E13" s="13">
         <v>11</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="20" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="13">
@@ -2246,7 +2294,7 @@
       <c r="E14" s="13">
         <v>11</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="21" t="s">
         <v>16</v>
       </c>
       <c r="G14" s="13">
@@ -2327,7 +2375,7 @@
       <c r="E15" s="13">
         <v>11</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="21" t="s">
         <v>16</v>
       </c>
       <c r="G15" s="13">
@@ -2393,31 +2441,31 @@
       <c r="BI15" s="1"/>
     </row>
     <row r="16" spans="1:61" ht="18" x14ac:dyDescent="0.35">
-      <c r="A16" s="26">
+      <c r="A16" s="22">
         <v>43810</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="28">
+      <c r="E16" s="24">
         <v>20.6</v>
       </c>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="28">
+      <c r="G16" s="24">
         <v>0</v>
       </c>
-      <c r="H16" s="28">
+      <c r="H16" s="24">
         <v>110</v>
       </c>
-      <c r="I16" s="28" t="s">
+      <c r="I16" s="24" t="s">
         <v>43</v>
       </c>
       <c r="J16" s="2"/>
@@ -2564,7 +2612,7 @@
       <c r="E18" s="13">
         <v>20.6</v>
       </c>
-      <c r="F18" s="23" t="s">
+      <c r="F18" s="20" t="s">
         <v>13</v>
       </c>
       <c r="G18" s="13">
@@ -2645,7 +2693,7 @@
       <c r="E19" s="13">
         <v>30</v>
       </c>
-      <c r="F19" s="22" t="s">
+      <c r="F19" s="19" t="s">
         <v>11</v>
       </c>
       <c r="G19" s="13">
@@ -2726,7 +2774,7 @@
       <c r="E20" s="13">
         <v>30</v>
       </c>
-      <c r="F20" s="25" t="s">
+      <c r="F20" s="21" t="s">
         <v>16</v>
       </c>
       <c r="G20" s="13">
@@ -2807,7 +2855,7 @@
       <c r="E21" s="13">
         <v>30</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="F21" s="20" t="s">
         <v>13</v>
       </c>
       <c r="G21" s="13">
@@ -2888,7 +2936,7 @@
       <c r="E22" s="13">
         <v>30</v>
       </c>
-      <c r="F22" s="25" t="s">
+      <c r="F22" s="21" t="s">
         <v>16</v>
       </c>
       <c r="G22" s="13">
@@ -2969,7 +3017,7 @@
       <c r="E23" s="13">
         <v>42</v>
       </c>
-      <c r="F23" s="22" t="s">
+      <c r="F23" s="19" t="s">
         <v>11</v>
       </c>
       <c r="G23" s="13">
@@ -3050,7 +3098,7 @@
       <c r="E24" s="13">
         <v>42</v>
       </c>
-      <c r="F24" s="23" t="s">
+      <c r="F24" s="20" t="s">
         <v>13</v>
       </c>
       <c r="G24" s="13">
@@ -3131,7 +3179,7 @@
       <c r="E25" s="13">
         <v>31.9</v>
       </c>
-      <c r="F25" s="23" t="s">
+      <c r="F25" s="20" t="s">
         <v>13</v>
       </c>
       <c r="G25" s="13">
@@ -3212,7 +3260,7 @@
       <c r="E26" s="13">
         <v>21.7</v>
       </c>
-      <c r="F26" s="23" t="s">
+      <c r="F26" s="20" t="s">
         <v>13</v>
       </c>
       <c r="G26" s="13">
@@ -3277,32 +3325,32 @@
       <c r="BH26" s="1"/>
       <c r="BI26" s="1"/>
     </row>
-    <row r="27" spans="1:61" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="19">
+    <row r="27" spans="1:61" ht="18" x14ac:dyDescent="0.35">
+      <c r="A27" s="14">
         <v>43837</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D27" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="21">
+      <c r="E27" s="13">
         <v>10.4</v>
       </c>
-      <c r="F27" s="24" t="s">
+      <c r="F27" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="21">
+      <c r="G27" s="13">
         <v>140</v>
       </c>
-      <c r="H27" s="21">
+      <c r="H27" s="13">
         <v>205</v>
       </c>
-      <c r="I27" s="21" t="s">
+      <c r="I27" s="13" t="s">
         <v>65</v>
       </c>
       <c r="J27" s="2"/>
@@ -3358,17 +3406,35 @@
       <c r="BH27" s="1"/>
       <c r="BI27" s="1"/>
     </row>
-    <row r="28" spans="1:61" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="15"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="18"/>
+    <row r="28" spans="1:61" ht="18" x14ac:dyDescent="0.35">
+      <c r="A28" s="14">
+        <v>43865</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" s="13">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="13">
+        <v>100</v>
+      </c>
+      <c r="H28" s="13">
+        <v>1000</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="J28" s="15"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
@@ -3422,16 +3488,34 @@
       <c r="BI28" s="1"/>
     </row>
     <row r="29" spans="1:61" ht="18" x14ac:dyDescent="0.35">
-      <c r="A29" s="15"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="18"/>
+      <c r="A29" s="14">
+        <v>43865</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="13">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="13">
+        <v>0</v>
+      </c>
+      <c r="H29" s="13">
+        <v>140</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="J29" s="15"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
@@ -3484,16 +3568,34 @@
       <c r="BH29" s="1"/>
       <c r="BI29" s="1"/>
     </row>
-    <row r="30" spans="1:61" ht="18" x14ac:dyDescent="0.35">
-      <c r="A30" s="3"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
+    <row r="30" spans="1:61" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="16">
+        <v>43865</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" s="18">
+        <v>10</v>
+      </c>
+      <c r="F30" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" s="18">
+        <v>0</v>
+      </c>
+      <c r="H30" s="18">
+        <v>800</v>
+      </c>
+      <c r="I30" s="18" t="s">
+        <v>80</v>
+      </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
@@ -3547,7 +3649,7 @@
       <c r="BH30" s="1"/>
       <c r="BI30" s="1"/>
     </row>
-    <row r="31" spans="1:61" ht="18" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:61" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="5"/>
       <c r="C31" s="2"/>
@@ -5133,8 +5235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838DA34D-F765-43A5-B43B-778E7D45A2A4}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5169,7 +5271,7 @@
     </row>
     <row r="2" spans="1:15" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A2" s="2"/>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="26" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="2"/>
@@ -5179,7 +5281,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="30" t="s">
+      <c r="J2" s="26" t="s">
         <v>72</v>
       </c>
       <c r="K2" s="2"/>
@@ -5206,477 +5308,519 @@
     <row r="4" spans="1:15" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="29" t="s">
         <v>73</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="33" t="s">
+      <c r="K4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="33" t="s">
+      <c r="L4" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="M4" s="33" t="s">
+      <c r="M4" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="N4" s="33" t="s">
+      <c r="N4" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="O4" s="33" t="s">
+      <c r="O4" s="29" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="28">
         <v>30</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="32">
+      <c r="E5" s="28">
         <v>220</v>
       </c>
-      <c r="F5" s="32">
+      <c r="F5" s="28">
         <v>1000</v>
       </c>
-      <c r="G5" s="32"/>
+      <c r="G5" s="28"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="34" t="s">
+      <c r="J5" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="K5" s="32">
+      <c r="K5" s="28">
         <v>20</v>
       </c>
-      <c r="L5" s="32" t="s">
+      <c r="L5" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="M5" s="32">
+      <c r="M5" s="28">
         <v>220</v>
       </c>
-      <c r="N5" s="32">
+      <c r="N5" s="28">
         <v>800</v>
       </c>
-      <c r="O5" s="37"/>
+      <c r="O5" s="33"/>
     </row>
     <row r="6" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31">
+      <c r="B6" s="27"/>
+      <c r="C6" s="27">
         <v>30</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="27">
         <v>200</v>
       </c>
-      <c r="F6" s="31">
+      <c r="F6" s="27">
         <v>1000</v>
       </c>
-      <c r="G6" s="31"/>
+      <c r="G6" s="27"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31">
+      <c r="J6" s="27"/>
+      <c r="K6" s="27">
         <v>30</v>
       </c>
-      <c r="L6" s="31" t="s">
+      <c r="L6" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="M6" s="31">
+      <c r="M6" s="27">
         <v>240</v>
       </c>
-      <c r="N6" s="31">
+      <c r="N6" s="27">
         <v>800</v>
       </c>
-      <c r="O6" s="36"/>
-    </row>
-    <row r="7" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O6" s="32"/>
+    </row>
+    <row r="7" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31">
+      <c r="B7" s="27"/>
+      <c r="C7" s="27">
         <v>30</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="27">
         <v>230</v>
       </c>
-      <c r="F7" s="31">
+      <c r="F7" s="27">
         <v>1000</v>
       </c>
-      <c r="G7" s="31"/>
+      <c r="G7" s="27"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31">
+      <c r="J7" s="27"/>
+      <c r="K7" s="27">
         <v>40</v>
       </c>
-      <c r="L7" s="31" t="s">
+      <c r="L7" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="M7" s="31">
+      <c r="M7" s="27">
         <v>260</v>
       </c>
-      <c r="N7" s="31">
+      <c r="N7" s="27">
         <v>700</v>
       </c>
-      <c r="O7" s="36"/>
-    </row>
-    <row r="8" spans="1:15" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="O7" s="32"/>
+    </row>
+    <row r="8" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31">
+      <c r="B8" s="27"/>
+      <c r="C8" s="27">
         <v>20</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="27">
         <v>200</v>
       </c>
-      <c r="F8" s="31">
+      <c r="F8" s="27">
         <v>1000</v>
       </c>
-      <c r="G8" s="31"/>
+      <c r="G8" s="27"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" s="32">
+      <c r="J8" s="34"/>
+      <c r="K8" s="36">
         <v>20</v>
       </c>
-      <c r="L8" s="32">
-        <v>50</v>
-      </c>
-      <c r="M8" s="32" t="s">
+      <c r="L8" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="N8" s="32">
+      <c r="M8" s="36">
+        <v>210</v>
+      </c>
+      <c r="N8" s="36">
         <v>800</v>
       </c>
-      <c r="O8" s="37"/>
-    </row>
-    <row r="9" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="O8" s="34"/>
+    </row>
+    <row r="9" spans="1:15" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31">
+      <c r="B9" s="27"/>
+      <c r="C9" s="27">
         <v>11</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="31">
+      <c r="E9" s="27">
         <v>180</v>
       </c>
-      <c r="F9" s="31">
+      <c r="F9" s="27">
         <v>800</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G9" s="35" t="s">
         <v>74</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31">
-        <v>30</v>
-      </c>
-      <c r="L9" s="31">
-        <v>70</v>
-      </c>
-      <c r="M9" s="31" t="s">
+      <c r="J9" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" s="28">
+        <v>20</v>
+      </c>
+      <c r="L9" s="28">
+        <v>50</v>
+      </c>
+      <c r="M9" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="N9" s="31">
+      <c r="N9" s="28">
         <v>800</v>
       </c>
-      <c r="O9" s="36"/>
+      <c r="O9" s="33"/>
     </row>
     <row r="10" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31">
+      <c r="B10" s="27"/>
+      <c r="C10" s="27">
         <v>11</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E10" s="27">
         <v>170</v>
       </c>
-      <c r="F10" s="31">
+      <c r="F10" s="27">
         <v>800</v>
       </c>
-      <c r="G10" s="39" t="s">
+      <c r="G10" s="35" t="s">
         <v>74</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31">
-        <v>40</v>
-      </c>
-      <c r="L10" s="31">
-        <v>80</v>
-      </c>
-      <c r="M10" s="31" t="s">
+      <c r="J10" s="27"/>
+      <c r="K10" s="27">
+        <v>30</v>
+      </c>
+      <c r="L10" s="27">
+        <v>70</v>
+      </c>
+      <c r="M10" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="N10" s="31">
-        <v>700</v>
-      </c>
-      <c r="O10" s="36"/>
+      <c r="N10" s="27">
+        <v>800</v>
+      </c>
+      <c r="O10" s="32"/>
     </row>
     <row r="11" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31">
+      <c r="B11" s="27"/>
+      <c r="C11" s="27">
         <v>11</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="27">
         <v>170</v>
       </c>
-      <c r="F11" s="31">
+      <c r="F11" s="27">
         <v>600</v>
       </c>
-      <c r="G11" s="31"/>
+      <c r="G11" s="27"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31">
-        <v>30</v>
-      </c>
-      <c r="L11" s="31">
-        <v>70</v>
-      </c>
-      <c r="M11" s="31" t="s">
+      <c r="J11" s="27"/>
+      <c r="K11" s="27">
+        <v>40</v>
+      </c>
+      <c r="L11" s="27">
+        <v>80</v>
+      </c>
+      <c r="M11" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="N11" s="31">
-        <v>400</v>
-      </c>
-      <c r="O11" s="36"/>
+      <c r="N11" s="27">
+        <v>700</v>
+      </c>
+      <c r="O11" s="32"/>
     </row>
     <row r="12" spans="1:15" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="28">
         <v>30</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="28">
         <v>120</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="32">
+      <c r="F12" s="28">
         <v>1000</v>
       </c>
-      <c r="G12" s="32"/>
+      <c r="G12" s="28"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="31">
+      <c r="J12" s="27"/>
+      <c r="K12" s="27">
+        <v>30</v>
+      </c>
+      <c r="L12" s="27">
+        <v>70</v>
+      </c>
+      <c r="M12" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="N12" s="27">
+        <v>400</v>
+      </c>
+      <c r="O12" s="32"/>
+    </row>
+    <row r="13" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A13" s="2"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27">
         <v>20</v>
       </c>
-      <c r="L12" s="31">
-        <v>80</v>
-      </c>
-      <c r="M12" s="31" t="s">
+      <c r="D13" s="27">
+        <v>100</v>
+      </c>
+      <c r="E13" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="N12" s="31">
-        <v>300</v>
-      </c>
-      <c r="O12" s="36"/>
-    </row>
-    <row r="13" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="2"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31">
-        <v>20</v>
-      </c>
-      <c r="D13" s="31">
-        <v>100</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="F13" s="31">
+      <c r="F13" s="27">
         <v>1000</v>
       </c>
-      <c r="G13" s="31"/>
+      <c r="G13" s="27"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31">
-        <v>10</v>
-      </c>
-      <c r="L13" s="31">
-        <v>50</v>
-      </c>
-      <c r="M13" s="31" t="s">
+      <c r="J13" s="32"/>
+      <c r="K13" s="27">
+        <v>20</v>
+      </c>
+      <c r="L13" s="27">
+        <v>80</v>
+      </c>
+      <c r="M13" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="N13" s="31">
-        <v>200</v>
-      </c>
-      <c r="O13" s="36"/>
-    </row>
-    <row r="14" spans="1:15" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N13" s="27">
+        <v>300</v>
+      </c>
+      <c r="O13" s="32"/>
+    </row>
+    <row r="14" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31">
+      <c r="B14" s="27"/>
+      <c r="C14" s="27">
         <v>11</v>
       </c>
-      <c r="D14" s="31">
+      <c r="D14" s="27">
         <v>70</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="F14" s="31">
+      <c r="F14" s="27">
         <v>600</v>
       </c>
-      <c r="G14" s="31"/>
+      <c r="G14" s="27"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="34" t="s">
+      <c r="J14" s="27"/>
+      <c r="K14" s="27">
+        <v>10</v>
+      </c>
+      <c r="L14" s="27">
+        <v>50</v>
+      </c>
+      <c r="M14" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="N14" s="27">
+        <v>200</v>
+      </c>
+      <c r="O14" s="32"/>
+    </row>
+    <row r="15" spans="1:15" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2"/>
+      <c r="B15" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="K14" s="32">
+      <c r="C15" s="28">
         <v>30</v>
       </c>
-      <c r="L14" s="32">
-        <v>70</v>
-      </c>
-      <c r="M14" s="32">
-        <v>240</v>
-      </c>
-      <c r="N14" s="32" t="s">
+      <c r="D15" s="28">
+        <v>120</v>
+      </c>
+      <c r="E15" s="28">
+        <v>220</v>
+      </c>
+      <c r="F15" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="O14" s="37"/>
-    </row>
-    <row r="15" spans="1:15" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="2"/>
-      <c r="B15" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="32">
-        <v>30</v>
-      </c>
-      <c r="D15" s="32">
-        <v>120</v>
-      </c>
-      <c r="E15" s="32">
-        <v>220</v>
-      </c>
-      <c r="F15" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15" s="32"/>
+      <c r="G15" s="28"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35">
+      <c r="J15" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" s="28">
         <v>30</v>
       </c>
-      <c r="L15" s="35">
+      <c r="L15" s="28">
         <v>70</v>
       </c>
-      <c r="M15" s="35">
-        <v>230</v>
-      </c>
-      <c r="N15" s="35" t="s">
+      <c r="M15" s="28">
+        <v>240</v>
+      </c>
+      <c r="N15" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="O15" s="38"/>
-    </row>
-    <row r="16" spans="1:15" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="O15" s="33"/>
+    </row>
+    <row r="16" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31">
+      <c r="B16" s="27"/>
+      <c r="C16" s="27">
         <v>20</v>
       </c>
-      <c r="D16" s="31">
+      <c r="D16" s="27">
         <v>100</v>
       </c>
-      <c r="E16" s="31">
+      <c r="E16" s="27">
         <v>205</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="G16" s="31"/>
+      <c r="G16" s="27"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="J16" s="27"/>
+      <c r="K16" s="27">
+        <v>30</v>
+      </c>
+      <c r="L16" s="27">
+        <v>70</v>
+      </c>
+      <c r="M16" s="27">
+        <v>230</v>
+      </c>
+      <c r="N16" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="O16" s="32"/>
+    </row>
+    <row r="17" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31">
+      <c r="B17" s="27"/>
+      <c r="C17" s="27">
         <v>11</v>
       </c>
-      <c r="D17" s="31">
+      <c r="D17" s="27">
         <v>70</v>
       </c>
-      <c r="E17" s="31">
+      <c r="E17" s="27">
         <v>190</v>
       </c>
-      <c r="F17" s="31" t="s">
+      <c r="F17" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="G17" s="31"/>
+      <c r="G17" s="27"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J17" s="32"/>
+      <c r="K17" s="37">
+        <v>20</v>
+      </c>
+      <c r="L17" s="37">
+        <v>80</v>
+      </c>
+      <c r="M17" s="27">
+        <v>210</v>
+      </c>
+      <c r="N17" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="O17" s="32"/>
+    </row>
+    <row r="18" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35">
+      <c r="B18" s="31"/>
+      <c r="C18" s="31">
         <v>11</v>
       </c>
-      <c r="D18" s="35">
+      <c r="D18" s="31">
         <v>70</v>
       </c>
-      <c r="E18" s="35">
+      <c r="E18" s="31">
         <v>170</v>
       </c>
-      <c r="F18" s="35" t="s">
+      <c r="F18" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="G18" s="35"/>
+      <c r="G18" s="31"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:11" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="J18" s="34"/>
+      <c r="K18" s="36">
+        <v>10</v>
+      </c>
+      <c r="L18" s="36">
+        <v>50</v>
+      </c>
+      <c r="M18" s="36">
+        <v>180</v>
+      </c>
+      <c r="N18" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="O18" s="34"/>
+    </row>
+    <row r="19" spans="1:15" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -5689,7 +5833,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -5702,7 +5846,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>

</xml_diff>

<commit_message>
Aggiornato il file Excel con il riassunto di tutti i run
</commit_message>
<xml_diff>
--- a/Caratterizzazione_THGEM.xlsx
+++ b/Caratterizzazione_THGEM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peppe\Desktop\LaTex\Report_THGEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EB40F4-7712-4355-A012-220B489DD874}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EBE993-7B20-43D6-BD52-FDEEE1AB667E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ACFC7C87-C28D-4487-B063-88156E979354}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{ACFC7C87-C28D-4487-B063-88156E979354}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="82">
   <si>
     <t>DATA</t>
   </si>
@@ -617,6 +617,9 @@
   </si>
   <si>
     <t>Vind=50        VTG=180</t>
+  </si>
+  <si>
+    <t>Scan fatto dopo il test col fascio</t>
   </si>
 </sst>
 </file>
@@ -709,7 +712,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -782,11 +785,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -888,6 +900,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1206,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C87521-6C72-4CB0-A78B-1EAFA58AC3F8}">
   <dimension ref="A1:BI55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5235,8 +5250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838DA34D-F765-43A5-B43B-778E7D45A2A4}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5684,24 +5699,24 @@
       </c>
       <c r="O14" s="32"/>
     </row>
-    <row r="15" spans="1:15" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="2"/>
-      <c r="B15" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="28">
-        <v>30</v>
-      </c>
-      <c r="D15" s="28">
-        <v>120</v>
-      </c>
-      <c r="E15" s="28">
-        <v>220</v>
-      </c>
-      <c r="F15" s="28" t="s">
+      <c r="B15" s="34"/>
+      <c r="C15" s="37">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D15" s="37">
+        <v>50</v>
+      </c>
+      <c r="E15" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="G15" s="28"/>
+      <c r="F15" s="37">
+        <v>400</v>
+      </c>
+      <c r="G15" s="39" t="s">
+        <v>81</v>
+      </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="30" t="s">
@@ -5721,22 +5736,24 @@
       </c>
       <c r="O15" s="33"/>
     </row>
-    <row r="16" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27">
-        <v>20</v>
-      </c>
-      <c r="D16" s="27">
-        <v>100</v>
-      </c>
-      <c r="E16" s="27">
-        <v>205</v>
-      </c>
-      <c r="F16" s="27" t="s">
+      <c r="B16" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="28">
+        <v>30</v>
+      </c>
+      <c r="D16" s="28">
+        <v>120</v>
+      </c>
+      <c r="E16" s="28">
+        <v>220</v>
+      </c>
+      <c r="F16" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="G16" s="27"/>
+      <c r="G16" s="28"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="27"/>
@@ -5758,13 +5775,13 @@
       <c r="A17" s="2"/>
       <c r="B17" s="27"/>
       <c r="C17" s="27">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D17" s="27">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="E17" s="27">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="F17" s="27" t="s">
         <v>71</v>
@@ -5789,20 +5806,20 @@
     </row>
     <row r="18" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31">
+      <c r="B18" s="27"/>
+      <c r="C18" s="27">
         <v>11</v>
       </c>
-      <c r="D18" s="31">
+      <c r="D18" s="27">
         <v>70</v>
       </c>
-      <c r="E18" s="31">
-        <v>170</v>
-      </c>
-      <c r="F18" s="31" t="s">
+      <c r="E18" s="27">
+        <v>190</v>
+      </c>
+      <c r="F18" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="G18" s="31"/>
+      <c r="G18" s="27"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="34"/>
@@ -5822,31 +5839,49 @@
     </row>
     <row r="19" spans="1:15" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27">
+        <v>11</v>
+      </c>
+      <c r="D19" s="27">
+        <v>70</v>
+      </c>
+      <c r="E19" s="27">
+        <v>170</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="27"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D20" s="31">
+        <v>50</v>
+      </c>
+      <c r="E20" s="31">
+        <v>160</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="39" t="s">
+        <v>81</v>
+      </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -5861,5 +5896,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modificata la parte dello scan di VTHGEM con la FULL, aggiungendo il test fatto il 20/02/20
</commit_message>
<xml_diff>
--- a/Caratterizzazione_THGEM.xlsx
+++ b/Caratterizzazione_THGEM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peppe\Desktop\LaTex\Report_THGEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E25574-86CD-4A75-9C77-CC5C4454CB88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F1990F-FDCA-4281-9964-4010DFAB0249}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ACFC7C87-C28D-4487-B063-88156E979354}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{ACFC7C87-C28D-4487-B063-88156E979354}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -832,7 +832,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -940,6 +940,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1258,7 +1261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C87521-6C72-4CB0-A78B-1EAFA58AC3F8}">
   <dimension ref="A1:BI55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -5323,8 +5326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838DA34D-F765-43A5-B43B-778E7D45A2A4}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5946,7 +5949,7 @@
       <c r="F20" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="G20" s="39" t="s">
+      <c r="G20" s="41" t="s">
         <v>81</v>
       </c>
       <c r="H20" s="2"/>

</xml_diff>

<commit_message>
Completato il file excel con lo schema dei run del test beam con le FULL THGEM
</commit_message>
<xml_diff>
--- a/Caratterizzazione_THGEM.xlsx
+++ b/Caratterizzazione_THGEM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peppe\Desktop\LaTex\Report_THGEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0AB029-61D3-4F92-896A-1EE186588E02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470C0275-4753-4404-994B-BEFD02913C2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{ACFC7C87-C28D-4487-B063-88156E979354}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="129">
   <si>
     <t>DATA</t>
   </si>
@@ -888,6 +888,30 @@
   </si>
   <si>
     <t>Vind=50    VTG=205    Vdrift=400</t>
+  </si>
+  <si>
+    <t>Single points that can be added to the IBF plot</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>Somma</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Totale parziale</t>
+  </si>
+  <si>
+    <t>Conteggio</t>
+  </si>
+  <si>
+    <t>Ibeam</t>
+  </si>
+  <si>
+    <t>This scan was done varying both Ibeam and target</t>
   </si>
 </sst>
 </file>
@@ -1111,7 +1135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1170,13 +1194,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1261,6 +1279,40 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1686,25 +1738,25 @@
       <c r="B2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="30">
+      <c r="D2" s="28">
         <v>10</v>
       </c>
-      <c r="E2" s="30">
+      <c r="E2" s="28">
         <v>30.2</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="30">
+      <c r="G2" s="28">
         <v>0</v>
       </c>
-      <c r="H2" s="30">
+      <c r="H2" s="28">
         <v>220</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="29" t="s">
         <v>12</v>
       </c>
       <c r="J2" s="2"/>
@@ -1767,25 +1819,25 @@
       <c r="B3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="28">
         <v>10</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="28">
         <v>30.4</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="30">
+      <c r="G3" s="28">
         <v>180</v>
       </c>
-      <c r="H3" s="30">
+      <c r="H3" s="28">
         <v>235</v>
       </c>
-      <c r="I3" s="30" t="s">
+      <c r="I3" s="28" t="s">
         <v>17</v>
       </c>
       <c r="J3" s="2"/>
@@ -1848,25 +1900,25 @@
       <c r="B4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="28">
         <v>10</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="28">
         <v>30.4</v>
       </c>
-      <c r="F4" s="42" t="s">
+      <c r="F4" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="30">
+      <c r="G4" s="28">
         <v>0</v>
       </c>
-      <c r="H4" s="30">
+      <c r="H4" s="28">
         <v>1500</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="I4" s="28" t="s">
         <v>18</v>
       </c>
       <c r="J4" s="2"/>
@@ -1929,25 +1981,25 @@
       <c r="B5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="28">
         <v>10</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="28">
         <v>30.4</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="30">
+      <c r="G5" s="28">
         <v>0</v>
       </c>
-      <c r="H5" s="30">
+      <c r="H5" s="28">
         <v>220</v>
       </c>
-      <c r="I5" s="30" t="s">
+      <c r="I5" s="28" t="s">
         <v>21</v>
       </c>
       <c r="J5" s="2"/>
@@ -2010,25 +2062,25 @@
       <c r="B6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="28">
         <v>10</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="28">
         <v>30.4</v>
       </c>
-      <c r="F6" s="40" t="s">
+      <c r="F6" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="28">
         <v>0</v>
       </c>
-      <c r="H6" s="30">
+      <c r="H6" s="28">
         <v>220</v>
       </c>
-      <c r="I6" s="30" t="s">
+      <c r="I6" s="28" t="s">
         <v>20</v>
       </c>
       <c r="J6" s="2"/>
@@ -2091,25 +2143,25 @@
       <c r="B7" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="28">
         <v>10</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="28">
         <v>20.5</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G7" s="28">
         <v>0</v>
       </c>
-      <c r="H7" s="30">
+      <c r="H7" s="28">
         <v>200</v>
       </c>
-      <c r="I7" s="30" t="s">
+      <c r="I7" s="28" t="s">
         <v>21</v>
       </c>
       <c r="J7" s="2"/>
@@ -2172,25 +2224,25 @@
       <c r="B8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="28">
         <v>10</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="28">
         <v>20.5</v>
       </c>
-      <c r="F8" s="41" t="s">
+      <c r="F8" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="30">
+      <c r="G8" s="28">
         <v>150</v>
       </c>
-      <c r="H8" s="30">
+      <c r="H8" s="28">
         <v>215</v>
       </c>
-      <c r="I8" s="30" t="s">
+      <c r="I8" s="28" t="s">
         <v>25</v>
       </c>
       <c r="J8" s="2"/>
@@ -2253,25 +2305,25 @@
       <c r="B9" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="28">
         <v>10</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="28">
         <v>20.5</v>
       </c>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="30">
+      <c r="G9" s="28">
         <v>100</v>
       </c>
-      <c r="H9" s="30">
+      <c r="H9" s="28">
         <v>1200</v>
       </c>
-      <c r="I9" s="30" t="s">
+      <c r="I9" s="28" t="s">
         <v>27</v>
       </c>
       <c r="J9" s="2"/>
@@ -2334,25 +2386,25 @@
       <c r="B10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="28">
         <v>10</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="28">
         <v>11</v>
       </c>
-      <c r="F10" s="40" t="s">
+      <c r="F10" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="30">
+      <c r="G10" s="28">
         <v>0</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="28">
         <v>60</v>
       </c>
-      <c r="I10" s="30" t="s">
+      <c r="I10" s="28" t="s">
         <v>29</v>
       </c>
       <c r="J10" s="2"/>
@@ -2415,25 +2467,25 @@
       <c r="B11" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11" s="28">
         <v>10</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E11" s="28">
         <v>11</v>
       </c>
-      <c r="F11" s="40" t="s">
+      <c r="F11" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="30">
+      <c r="G11" s="28">
         <v>0</v>
       </c>
-      <c r="H11" s="30">
+      <c r="H11" s="28">
         <v>60</v>
       </c>
-      <c r="I11" s="30" t="s">
+      <c r="I11" s="28" t="s">
         <v>31</v>
       </c>
       <c r="J11" s="2"/>
@@ -2496,25 +2548,25 @@
       <c r="B12" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="28">
         <v>10</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="28">
         <v>11</v>
       </c>
-      <c r="F12" s="40" t="s">
+      <c r="F12" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="30">
+      <c r="G12" s="28">
         <v>0</v>
       </c>
-      <c r="H12" s="30">
+      <c r="H12" s="28">
         <v>150</v>
       </c>
-      <c r="I12" s="30" t="s">
+      <c r="I12" s="28" t="s">
         <v>33</v>
       </c>
       <c r="J12" s="2"/>
@@ -2577,25 +2629,25 @@
       <c r="B13" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="30">
+      <c r="D13" s="28">
         <v>10</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="28">
         <v>11</v>
       </c>
-      <c r="F13" s="41" t="s">
+      <c r="F13" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="30">
+      <c r="G13" s="28">
         <v>130</v>
       </c>
-      <c r="H13" s="30">
+      <c r="H13" s="28">
         <v>210</v>
       </c>
-      <c r="I13" s="30" t="s">
+      <c r="I13" s="28" t="s">
         <v>35</v>
       </c>
       <c r="J13" s="2"/>
@@ -2658,25 +2710,25 @@
       <c r="B14" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="28">
         <v>10</v>
       </c>
-      <c r="E14" s="30">
+      <c r="E14" s="28">
         <v>11</v>
       </c>
-      <c r="F14" s="42" t="s">
+      <c r="F14" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="30">
+      <c r="G14" s="28">
         <v>0</v>
       </c>
-      <c r="H14" s="30">
+      <c r="H14" s="28">
         <v>800</v>
       </c>
-      <c r="I14" s="30" t="s">
+      <c r="I14" s="28" t="s">
         <v>37</v>
       </c>
       <c r="J14" s="2"/>
@@ -2739,25 +2791,25 @@
       <c r="B15" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="30">
+      <c r="D15" s="28">
         <v>10</v>
       </c>
-      <c r="E15" s="30">
+      <c r="E15" s="28">
         <v>11</v>
       </c>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="30">
+      <c r="G15" s="28">
         <v>600</v>
       </c>
-      <c r="H15" s="30">
+      <c r="H15" s="28">
         <v>850</v>
       </c>
-      <c r="I15" s="30" t="s">
+      <c r="I15" s="28" t="s">
         <v>39</v>
       </c>
       <c r="J15" s="2"/>
@@ -2820,25 +2872,25 @@
       <c r="B16" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="30">
+      <c r="D16" s="28">
         <v>10</v>
       </c>
-      <c r="E16" s="30">
+      <c r="E16" s="28">
         <v>9.3000000000000007</v>
       </c>
-      <c r="F16" s="41" t="s">
+      <c r="F16" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="30">
+      <c r="G16" s="28">
         <v>130</v>
       </c>
-      <c r="H16" s="30">
+      <c r="H16" s="28">
         <v>210</v>
       </c>
-      <c r="I16" s="30" t="s">
+      <c r="I16" s="28" t="s">
         <v>88</v>
       </c>
       <c r="J16" s="2"/>
@@ -2901,25 +2953,25 @@
       <c r="B17" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="30">
+      <c r="D17" s="28">
         <v>10</v>
       </c>
-      <c r="E17" s="30">
+      <c r="E17" s="28">
         <v>9.3000000000000007</v>
       </c>
-      <c r="F17" s="42" t="s">
+      <c r="F17" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="30">
+      <c r="G17" s="28">
         <v>200</v>
       </c>
-      <c r="H17" s="30">
+      <c r="H17" s="28">
         <v>600</v>
       </c>
-      <c r="I17" s="30" t="s">
+      <c r="I17" s="28" t="s">
         <v>90</v>
       </c>
       <c r="J17" s="2"/>
@@ -2976,31 +3028,31 @@
       <c r="BI17" s="1"/>
     </row>
     <row r="18" spans="1:61" ht="18" x14ac:dyDescent="0.35">
-      <c r="A18" s="26">
+      <c r="A18" s="24">
         <v>43810</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="43" t="s">
+      <c r="C18" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="43" t="s">
+      <c r="D18" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="43">
+      <c r="E18" s="41">
         <v>20.6</v>
       </c>
-      <c r="F18" s="44" t="s">
+      <c r="F18" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="43">
+      <c r="G18" s="41">
         <v>0</v>
       </c>
-      <c r="H18" s="43">
+      <c r="H18" s="41">
         <v>110</v>
       </c>
-      <c r="I18" s="43" t="s">
+      <c r="I18" s="41" t="s">
         <v>43</v>
       </c>
       <c r="J18" s="2"/>
@@ -3063,21 +3115,21 @@
       <c r="B19" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="30">
+      <c r="E19" s="28">
         <v>20.6</v>
       </c>
-      <c r="F19" s="30" t="s">
+      <c r="F19" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
@@ -3138,25 +3190,25 @@
       <c r="B20" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="28">
         <v>20.6</v>
       </c>
-      <c r="F20" s="41" t="s">
+      <c r="F20" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="30">
+      <c r="G20" s="28">
         <v>180</v>
       </c>
-      <c r="H20" s="30">
+      <c r="H20" s="28">
         <v>225</v>
       </c>
-      <c r="I20" s="30" t="s">
+      <c r="I20" s="28" t="s">
         <v>47</v>
       </c>
       <c r="J20" s="2"/>
@@ -3219,25 +3271,25 @@
       <c r="B21" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="30">
+      <c r="E21" s="28">
         <v>30</v>
       </c>
-      <c r="F21" s="40" t="s">
+      <c r="F21" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="30">
+      <c r="G21" s="28">
         <v>0</v>
       </c>
-      <c r="H21" s="30">
+      <c r="H21" s="28">
         <v>110</v>
       </c>
-      <c r="I21" s="30" t="s">
+      <c r="I21" s="28" t="s">
         <v>49</v>
       </c>
       <c r="J21" s="2"/>
@@ -3300,25 +3352,25 @@
       <c r="B22" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="C22" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="30" t="s">
+      <c r="D22" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="30">
+      <c r="E22" s="28">
         <v>30</v>
       </c>
-      <c r="F22" s="42" t="s">
+      <c r="F22" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="G22" s="30">
+      <c r="G22" s="28">
         <v>0</v>
       </c>
-      <c r="H22" s="30">
+      <c r="H22" s="28">
         <v>1400</v>
       </c>
-      <c r="I22" s="30" t="s">
+      <c r="I22" s="28" t="s">
         <v>51</v>
       </c>
       <c r="J22" s="2"/>
@@ -3381,25 +3433,25 @@
       <c r="B23" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D23" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="30">
+      <c r="E23" s="28">
         <v>30</v>
       </c>
-      <c r="F23" s="41" t="s">
+      <c r="F23" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="30">
+      <c r="G23" s="28">
         <v>180</v>
       </c>
-      <c r="H23" s="30">
+      <c r="H23" s="28">
         <v>240</v>
       </c>
-      <c r="I23" s="30" t="s">
+      <c r="I23" s="28" t="s">
         <v>53</v>
       </c>
       <c r="J23" s="2"/>
@@ -3462,25 +3514,25 @@
       <c r="B24" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="30" t="s">
+      <c r="D24" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="30">
+      <c r="E24" s="28">
         <v>30</v>
       </c>
-      <c r="F24" s="42" t="s">
+      <c r="F24" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="G24" s="30">
+      <c r="G24" s="28">
         <v>0</v>
       </c>
-      <c r="H24" s="30">
+      <c r="H24" s="28">
         <v>1400</v>
       </c>
-      <c r="I24" s="30" t="s">
+      <c r="I24" s="28" t="s">
         <v>55</v>
       </c>
       <c r="J24" s="2"/>
@@ -3543,25 +3595,25 @@
       <c r="B25" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="30" t="s">
+      <c r="D25" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="30">
+      <c r="E25" s="28">
         <v>42</v>
       </c>
-      <c r="F25" s="40" t="s">
+      <c r="F25" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="30">
+      <c r="G25" s="28">
         <v>0</v>
       </c>
-      <c r="H25" s="30">
+      <c r="H25" s="28">
         <v>180</v>
       </c>
-      <c r="I25" s="30" t="s">
+      <c r="I25" s="28" t="s">
         <v>57</v>
       </c>
       <c r="J25" s="2"/>
@@ -3624,25 +3676,25 @@
       <c r="B26" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="30" t="s">
+      <c r="C26" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="30" t="s">
+      <c r="D26" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="30">
+      <c r="E26" s="28">
         <v>42</v>
       </c>
-      <c r="F26" s="41" t="s">
+      <c r="F26" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="30">
+      <c r="G26" s="28">
         <v>220</v>
       </c>
-      <c r="H26" s="30">
+      <c r="H26" s="28">
         <v>270</v>
       </c>
-      <c r="I26" s="30" t="s">
+      <c r="I26" s="28" t="s">
         <v>59</v>
       </c>
       <c r="J26" s="2"/>
@@ -3705,25 +3757,25 @@
       <c r="B27" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="30" t="s">
+      <c r="C27" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="30" t="s">
+      <c r="D27" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="30">
+      <c r="E27" s="28">
         <v>31.9</v>
       </c>
-      <c r="F27" s="41" t="s">
+      <c r="F27" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="30">
+      <c r="G27" s="28">
         <v>170</v>
       </c>
-      <c r="H27" s="30">
+      <c r="H27" s="28">
         <v>245</v>
       </c>
-      <c r="I27" s="30" t="s">
+      <c r="I27" s="28" t="s">
         <v>63</v>
       </c>
       <c r="J27" s="2"/>
@@ -3786,25 +3838,25 @@
       <c r="B28" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="30" t="s">
+      <c r="C28" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="30" t="s">
+      <c r="D28" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="30">
+      <c r="E28" s="28">
         <v>21.7</v>
       </c>
-      <c r="F28" s="41" t="s">
+      <c r="F28" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="30">
+      <c r="G28" s="28">
         <v>120</v>
       </c>
-      <c r="H28" s="30">
+      <c r="H28" s="28">
         <v>220</v>
       </c>
-      <c r="I28" s="30" t="s">
+      <c r="I28" s="28" t="s">
         <v>64</v>
       </c>
       <c r="J28" s="2"/>
@@ -3867,25 +3919,25 @@
       <c r="B29" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D29" s="30" t="s">
+      <c r="D29" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E29" s="30">
+      <c r="E29" s="28">
         <v>10.4</v>
       </c>
-      <c r="F29" s="41" t="s">
+      <c r="F29" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="30">
+      <c r="G29" s="28">
         <v>140</v>
       </c>
-      <c r="H29" s="30">
+      <c r="H29" s="28">
         <v>205</v>
       </c>
-      <c r="I29" s="30" t="s">
+      <c r="I29" s="28" t="s">
         <v>65</v>
       </c>
       <c r="J29" s="2"/>
@@ -3948,25 +4000,25 @@
       <c r="B30" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="30" t="s">
+      <c r="D30" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E30" s="30">
+      <c r="E30" s="28">
         <v>20.100000000000001</v>
       </c>
-      <c r="F30" s="42" t="s">
+      <c r="F30" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="G30" s="30">
+      <c r="G30" s="28">
         <v>100</v>
       </c>
-      <c r="H30" s="30">
+      <c r="H30" s="28">
         <v>1000</v>
       </c>
-      <c r="I30" s="30" t="s">
+      <c r="I30" s="28" t="s">
         <v>92</v>
       </c>
       <c r="J30" s="2"/>
@@ -4029,25 +4081,25 @@
       <c r="B31" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="30" t="s">
+      <c r="D31" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E31" s="30">
+      <c r="E31" s="28">
         <v>20.100000000000001</v>
       </c>
-      <c r="F31" s="40" t="s">
+      <c r="F31" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="G31" s="30">
+      <c r="G31" s="28">
         <v>0</v>
       </c>
-      <c r="H31" s="30">
+      <c r="H31" s="28">
         <v>140</v>
       </c>
-      <c r="I31" s="30" t="s">
+      <c r="I31" s="28" t="s">
         <v>94</v>
       </c>
       <c r="J31" s="2"/>
@@ -4110,25 +4162,25 @@
       <c r="B32" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="34" t="s">
+      <c r="D32" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="32">
         <v>10</v>
       </c>
-      <c r="F32" s="45" t="s">
+      <c r="F32" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="G32" s="34">
+      <c r="G32" s="32">
         <v>0</v>
       </c>
-      <c r="H32" s="34">
+      <c r="H32" s="32">
         <v>800</v>
       </c>
-      <c r="I32" s="34" t="s">
+      <c r="I32" s="32" t="s">
         <v>96</v>
       </c>
       <c r="J32" s="2"/>
@@ -5680,7 +5732,7 @@
     </row>
     <row r="2" spans="1:15" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A2" s="2"/>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="27" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="2"/>
@@ -5690,7 +5742,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="29" t="s">
+      <c r="J2" s="27" t="s">
         <v>72</v>
       </c>
       <c r="K2" s="2"/>
@@ -5717,536 +5769,536 @@
     <row r="4" spans="1:15" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="30" t="s">
         <v>73</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="32" t="s">
+      <c r="K4" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="32" t="s">
+      <c r="L4" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="M4" s="32" t="s">
+      <c r="M4" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="N4" s="32" t="s">
+      <c r="N4" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="O4" s="32" t="s">
+      <c r="O4" s="30" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="29">
         <v>30</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="29">
         <v>220</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="29">
         <v>1000</v>
       </c>
-      <c r="G5" s="31"/>
+      <c r="G5" s="29"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="33" t="s">
+      <c r="J5" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="K5" s="31">
+      <c r="K5" s="29">
         <v>20</v>
       </c>
-      <c r="L5" s="31" t="s">
+      <c r="L5" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="M5" s="31">
+      <c r="M5" s="29">
         <v>220</v>
       </c>
-      <c r="N5" s="31">
+      <c r="N5" s="29">
         <v>800</v>
       </c>
-      <c r="O5" s="36"/>
+      <c r="O5" s="34"/>
     </row>
     <row r="6" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30">
+      <c r="B6" s="28"/>
+      <c r="C6" s="28">
         <v>30</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="28">
         <v>200</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F6" s="28">
         <v>1000</v>
       </c>
-      <c r="G6" s="30"/>
+      <c r="G6" s="28"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30">
+      <c r="J6" s="28"/>
+      <c r="K6" s="28">
         <v>30</v>
       </c>
-      <c r="L6" s="30" t="s">
+      <c r="L6" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="M6" s="30">
+      <c r="M6" s="28">
         <v>240</v>
       </c>
-      <c r="N6" s="30">
+      <c r="N6" s="28">
         <v>800</v>
       </c>
-      <c r="O6" s="35"/>
+      <c r="O6" s="33"/>
     </row>
     <row r="7" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30">
+      <c r="B7" s="28"/>
+      <c r="C7" s="28">
         <v>30</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="28">
         <v>230</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="28">
         <v>1000</v>
       </c>
-      <c r="G7" s="30"/>
+      <c r="G7" s="28"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30">
+      <c r="J7" s="28"/>
+      <c r="K7" s="28">
         <v>40</v>
       </c>
-      <c r="L7" s="30" t="s">
+      <c r="L7" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="M7" s="30">
+      <c r="M7" s="28">
         <v>260</v>
       </c>
-      <c r="N7" s="30">
+      <c r="N7" s="28">
         <v>700</v>
       </c>
-      <c r="O7" s="35"/>
+      <c r="O7" s="33"/>
     </row>
     <row r="8" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30">
+      <c r="B8" s="28"/>
+      <c r="C8" s="28">
         <v>20</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="28">
         <v>200</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="28">
         <v>1000</v>
       </c>
-      <c r="G8" s="30"/>
+      <c r="G8" s="28"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="34">
+      <c r="J8" s="35"/>
+      <c r="K8" s="32">
         <v>20</v>
       </c>
-      <c r="L8" s="34" t="s">
+      <c r="L8" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="M8" s="34">
+      <c r="M8" s="32">
         <v>210</v>
       </c>
-      <c r="N8" s="34">
+      <c r="N8" s="32">
         <v>800</v>
       </c>
-      <c r="O8" s="37"/>
+      <c r="O8" s="35"/>
     </row>
     <row r="9" spans="1:15" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30">
+      <c r="B9" s="28"/>
+      <c r="C9" s="28">
         <v>11</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="28">
         <v>180</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9" s="28">
         <v>800</v>
       </c>
-      <c r="G9" s="38" t="s">
+      <c r="G9" s="36" t="s">
         <v>74</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="33" t="s">
+      <c r="J9" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="31">
+      <c r="K9" s="29">
         <v>20</v>
       </c>
-      <c r="L9" s="31">
+      <c r="L9" s="29">
         <v>50</v>
       </c>
-      <c r="M9" s="31" t="s">
+      <c r="M9" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="N9" s="31">
+      <c r="N9" s="29">
         <v>800</v>
       </c>
-      <c r="O9" s="36"/>
+      <c r="O9" s="34"/>
     </row>
     <row r="10" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30">
+      <c r="B10" s="28"/>
+      <c r="C10" s="28">
         <v>11</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="28">
         <v>170</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="28">
         <v>800</v>
       </c>
-      <c r="G10" s="38" t="s">
+      <c r="G10" s="36" t="s">
         <v>74</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30">
+      <c r="J10" s="28"/>
+      <c r="K10" s="28">
         <v>30</v>
       </c>
-      <c r="L10" s="30">
+      <c r="L10" s="28">
         <v>70</v>
       </c>
-      <c r="M10" s="30" t="s">
+      <c r="M10" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="N10" s="30">
+      <c r="N10" s="28">
         <v>800</v>
       </c>
-      <c r="O10" s="35"/>
+      <c r="O10" s="33"/>
     </row>
     <row r="11" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30">
+      <c r="B11" s="28"/>
+      <c r="C11" s="28">
         <v>11</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E11" s="28">
         <v>170</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F11" s="28">
         <v>600</v>
       </c>
-      <c r="G11" s="30"/>
+      <c r="G11" s="28"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30">
+      <c r="J11" s="28"/>
+      <c r="K11" s="28">
         <v>40</v>
       </c>
-      <c r="L11" s="30">
+      <c r="L11" s="28">
         <v>80</v>
       </c>
-      <c r="M11" s="30" t="s">
+      <c r="M11" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="N11" s="30">
+      <c r="N11" s="28">
         <v>700</v>
       </c>
-      <c r="O11" s="35"/>
+      <c r="O11" s="33"/>
     </row>
     <row r="12" spans="1:15" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="31">
+      <c r="C12" s="29">
         <v>30</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="29">
         <v>120</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="31">
+      <c r="F12" s="29">
         <v>1000</v>
       </c>
-      <c r="G12" s="31"/>
+      <c r="G12" s="29"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30">
+      <c r="J12" s="28"/>
+      <c r="K12" s="28">
         <v>30</v>
       </c>
-      <c r="L12" s="30">
+      <c r="L12" s="28">
         <v>70</v>
       </c>
-      <c r="M12" s="30" t="s">
+      <c r="M12" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="N12" s="30">
+      <c r="N12" s="28">
         <v>400</v>
       </c>
-      <c r="O12" s="35"/>
+      <c r="O12" s="33"/>
     </row>
     <row r="13" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30">
+      <c r="B13" s="28"/>
+      <c r="C13" s="28">
         <v>20</v>
       </c>
-      <c r="D13" s="30">
+      <c r="D13" s="28">
         <v>100</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="28">
         <v>1000</v>
       </c>
-      <c r="G13" s="30"/>
+      <c r="G13" s="28"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="30">
+      <c r="J13" s="33"/>
+      <c r="K13" s="28">
         <v>20</v>
       </c>
-      <c r="L13" s="30">
+      <c r="L13" s="28">
         <v>80</v>
       </c>
-      <c r="M13" s="30" t="s">
+      <c r="M13" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="N13" s="30">
+      <c r="N13" s="28">
         <v>300</v>
       </c>
-      <c r="O13" s="35"/>
+      <c r="O13" s="33"/>
     </row>
     <row r="14" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30">
+      <c r="B14" s="28"/>
+      <c r="C14" s="28">
         <v>11</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="28">
         <v>70</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="F14" s="30">
+      <c r="F14" s="28">
         <v>600</v>
       </c>
-      <c r="G14" s="30"/>
+      <c r="G14" s="28"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30">
+      <c r="J14" s="28"/>
+      <c r="K14" s="28">
         <v>10</v>
       </c>
-      <c r="L14" s="30">
+      <c r="L14" s="28">
         <v>50</v>
       </c>
-      <c r="M14" s="30" t="s">
+      <c r="M14" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="N14" s="30">
+      <c r="N14" s="28">
         <v>200</v>
       </c>
-      <c r="O14" s="35"/>
+      <c r="O14" s="33"/>
     </row>
     <row r="15" spans="1:15" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="2"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="30">
+      <c r="B15" s="35"/>
+      <c r="C15" s="28">
         <v>9.3000000000000007</v>
       </c>
-      <c r="D15" s="30">
+      <c r="D15" s="28">
         <v>50</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="30">
+      <c r="F15" s="28">
         <v>400</v>
       </c>
-      <c r="G15" s="46" t="s">
+      <c r="G15" s="44" t="s">
         <v>97</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="33" t="s">
+      <c r="J15" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="31">
+      <c r="K15" s="29">
         <v>30</v>
       </c>
-      <c r="L15" s="31">
+      <c r="L15" s="29">
         <v>70</v>
       </c>
-      <c r="M15" s="31">
+      <c r="M15" s="29">
         <v>240</v>
       </c>
-      <c r="N15" s="31" t="s">
+      <c r="N15" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="O15" s="36"/>
+      <c r="O15" s="34"/>
     </row>
     <row r="16" spans="1:15" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="31">
+      <c r="C16" s="29">
         <v>30</v>
       </c>
-      <c r="D16" s="31">
+      <c r="D16" s="29">
         <v>120</v>
       </c>
-      <c r="E16" s="31">
+      <c r="E16" s="29">
         <v>220</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="G16" s="31"/>
+      <c r="G16" s="29"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30">
+      <c r="J16" s="28"/>
+      <c r="K16" s="28">
         <v>30</v>
       </c>
-      <c r="L16" s="30">
+      <c r="L16" s="28">
         <v>70</v>
       </c>
-      <c r="M16" s="30">
+      <c r="M16" s="28">
         <v>230</v>
       </c>
-      <c r="N16" s="30" t="s">
+      <c r="N16" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="O16" s="35"/>
+      <c r="O16" s="33"/>
     </row>
     <row r="17" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30">
+      <c r="B17" s="28"/>
+      <c r="C17" s="28">
         <v>20</v>
       </c>
-      <c r="D17" s="30">
+      <c r="D17" s="28">
         <v>100</v>
       </c>
-      <c r="E17" s="30">
+      <c r="E17" s="28">
         <v>205</v>
       </c>
-      <c r="F17" s="30" t="s">
+      <c r="F17" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="G17" s="30"/>
+      <c r="G17" s="28"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="30">
+      <c r="J17" s="33"/>
+      <c r="K17" s="28">
         <v>20</v>
       </c>
-      <c r="L17" s="30">
+      <c r="L17" s="28">
         <v>80</v>
       </c>
-      <c r="M17" s="30">
+      <c r="M17" s="28">
         <v>210</v>
       </c>
-      <c r="N17" s="30" t="s">
+      <c r="N17" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="O17" s="35"/>
+      <c r="O17" s="33"/>
     </row>
     <row r="18" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30">
+      <c r="B18" s="28"/>
+      <c r="C18" s="28">
         <v>11</v>
       </c>
-      <c r="D18" s="30">
+      <c r="D18" s="28">
         <v>70</v>
       </c>
-      <c r="E18" s="30">
+      <c r="E18" s="28">
         <v>190</v>
       </c>
-      <c r="F18" s="30" t="s">
+      <c r="F18" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="G18" s="30"/>
+      <c r="G18" s="28"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="34">
+      <c r="J18" s="35"/>
+      <c r="K18" s="32">
         <v>10</v>
       </c>
-      <c r="L18" s="34">
+      <c r="L18" s="32">
         <v>50</v>
       </c>
-      <c r="M18" s="34">
+      <c r="M18" s="32">
         <v>180</v>
       </c>
-      <c r="N18" s="34" t="s">
+      <c r="N18" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="O18" s="37"/>
+      <c r="O18" s="35"/>
     </row>
     <row r="19" spans="1:15" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30">
+      <c r="B19" s="28"/>
+      <c r="C19" s="28">
         <v>11</v>
       </c>
-      <c r="D19" s="30">
+      <c r="D19" s="28">
         <v>70</v>
       </c>
-      <c r="E19" s="30">
+      <c r="E19" s="28">
         <v>170</v>
       </c>
-      <c r="F19" s="30" t="s">
+      <c r="F19" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="G19" s="30"/>
+      <c r="G19" s="28"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -6254,20 +6306,20 @@
     </row>
     <row r="20" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="2"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34">
+      <c r="B20" s="32"/>
+      <c r="C20" s="32">
         <v>9.3000000000000007</v>
       </c>
-      <c r="D20" s="34">
+      <c r="D20" s="32">
         <v>50</v>
       </c>
-      <c r="E20" s="34">
+      <c r="E20" s="32">
         <v>160</v>
       </c>
-      <c r="F20" s="34" t="s">
+      <c r="F20" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="G20" s="47" t="s">
+      <c r="G20" s="45" t="s">
         <v>97</v>
       </c>
       <c r="H20" s="2"/>
@@ -6297,8 +6349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E260431C-5552-43E0-806B-E171CCC2519A}">
   <dimension ref="A1:BL56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6357,7 +6409,7 @@
       <c r="L1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="M1" s="30" t="s">
         <v>73</v>
       </c>
       <c r="N1" s="2"/>
@@ -6437,7 +6489,7 @@
       <c r="H2" s="13">
         <v>13.5</v>
       </c>
-      <c r="I2" s="48" t="s">
+      <c r="I2" s="46" t="s">
         <v>77</v>
       </c>
       <c r="J2" s="13"/>
@@ -6445,7 +6497,7 @@
       <c r="L2" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="M2" s="39" t="s">
+      <c r="M2" s="37" t="s">
         <v>83</v>
       </c>
       <c r="N2" s="2"/>
@@ -6525,7 +6577,7 @@
       <c r="H3" s="13">
         <v>13.4</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="22" t="s">
         <v>13</v>
       </c>
       <c r="J3" s="13">
@@ -6537,7 +6589,7 @@
       <c r="L3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="39" t="s">
+      <c r="M3" s="37" t="s">
         <v>82</v>
       </c>
       <c r="N3" s="2"/>
@@ -6617,7 +6669,7 @@
       <c r="H4" s="13">
         <v>13.2</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="23" t="s">
         <v>16</v>
       </c>
       <c r="J4" s="13">
@@ -6629,7 +6681,7 @@
       <c r="L4" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="39" t="s">
+      <c r="M4" s="37" t="s">
         <v>85</v>
       </c>
       <c r="N4" s="2"/>
@@ -6709,7 +6761,7 @@
       <c r="H5" s="13">
         <v>8.6</v>
       </c>
-      <c r="I5" s="48" t="s">
+      <c r="I5" s="46" t="s">
         <v>77</v>
       </c>
       <c r="J5" s="13"/>
@@ -6717,7 +6769,7 @@
       <c r="L5" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="M5" s="39" t="s">
+      <c r="M5" s="37" t="s">
         <v>98</v>
       </c>
       <c r="N5" s="2"/>
@@ -6794,10 +6846,10 @@
       <c r="G6" s="13">
         <v>9.6</v>
       </c>
-      <c r="H6" s="49">
+      <c r="H6" s="47">
         <v>9</v>
       </c>
-      <c r="I6" s="48" t="s">
+      <c r="I6" s="46" t="s">
         <v>77</v>
       </c>
       <c r="J6" s="13"/>
@@ -6805,7 +6857,7 @@
       <c r="L6" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="M6" s="39"/>
+      <c r="M6" s="37"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
@@ -6883,7 +6935,7 @@
       <c r="H7" s="13">
         <v>2.5</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="I7" s="23" t="s">
         <v>16</v>
       </c>
       <c r="J7" s="13">
@@ -6895,7 +6947,7 @@
       <c r="L7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="M7" s="39" t="s">
+      <c r="M7" s="37" t="s">
         <v>102</v>
       </c>
       <c r="N7" s="2"/>
@@ -6975,7 +7027,7 @@
       <c r="H8" s="13">
         <v>1.6</v>
       </c>
-      <c r="I8" s="48" t="s">
+      <c r="I8" s="46" t="s">
         <v>77</v>
       </c>
       <c r="J8" s="13"/>
@@ -6983,7 +7035,7 @@
       <c r="L8" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="M8" s="39" t="s">
+      <c r="M8" s="37" t="s">
         <v>101</v>
       </c>
       <c r="N8" s="2"/>
@@ -7063,7 +7115,7 @@
       <c r="H9" s="13">
         <v>1.6</v>
       </c>
-      <c r="I9" s="48" t="s">
+      <c r="I9" s="46" t="s">
         <v>77</v>
       </c>
       <c r="J9" s="13"/>
@@ -7071,7 +7123,7 @@
       <c r="L9" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="M9" s="39" t="s">
+      <c r="M9" s="37" t="s">
         <v>103</v>
       </c>
       <c r="N9" s="2"/>
@@ -7151,7 +7203,7 @@
       <c r="H10" s="13">
         <v>0.2</v>
       </c>
-      <c r="I10" s="48" t="s">
+      <c r="I10" s="46" t="s">
         <v>77</v>
       </c>
       <c r="J10" s="13"/>
@@ -7159,7 +7211,7 @@
       <c r="L10" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="M10" s="39" t="s">
+      <c r="M10" s="37" t="s">
         <v>101</v>
       </c>
       <c r="N10" s="2"/>
@@ -7239,7 +7291,7 @@
       <c r="H11" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="I11" s="48" t="s">
+      <c r="I11" s="46" t="s">
         <v>77</v>
       </c>
       <c r="J11" s="13"/>
@@ -7247,7 +7299,7 @@
       <c r="L11" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="M11" s="39" t="s">
+      <c r="M11" s="37" t="s">
         <v>103</v>
       </c>
       <c r="N11" s="2"/>
@@ -7327,7 +7379,7 @@
       <c r="H12" s="13">
         <v>0.3</v>
       </c>
-      <c r="I12" s="25" t="s">
+      <c r="I12" s="23" t="s">
         <v>16</v>
       </c>
       <c r="J12" s="13">
@@ -7339,7 +7391,7 @@
       <c r="L12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="M12" s="39" t="s">
+      <c r="M12" s="37" t="s">
         <v>107</v>
       </c>
       <c r="N12" s="2"/>
@@ -7419,7 +7471,7 @@
       <c r="H13" s="13">
         <v>0.3</v>
       </c>
-      <c r="I13" s="23" t="s">
+      <c r="I13" s="22" t="s">
         <v>13</v>
       </c>
       <c r="J13" s="13">
@@ -7431,7 +7483,7 @@
       <c r="L13" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="M13" s="39" t="s">
+      <c r="M13" s="37" t="s">
         <v>107</v>
       </c>
       <c r="N13" s="2"/>
@@ -7511,7 +7563,7 @@
       <c r="H14" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="I14" s="48" t="s">
+      <c r="I14" s="46" t="s">
         <v>77</v>
       </c>
       <c r="J14" s="13"/>
@@ -7519,7 +7571,7 @@
       <c r="L14" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="M14" s="39" t="s">
+      <c r="M14" s="37" t="s">
         <v>112</v>
       </c>
       <c r="N14" s="2"/>
@@ -7599,13 +7651,13 @@
       <c r="H15" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="I15" s="48" t="s">
+      <c r="I15" s="46" t="s">
         <v>77</v>
       </c>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
-      <c r="M15" s="50" t="s">
+      <c r="M15" s="48" t="s">
         <v>114</v>
       </c>
       <c r="N15" s="2"/>
@@ -7661,7 +7713,7 @@
       <c r="BL15" s="1"/>
     </row>
     <row r="16" spans="1:64" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="51">
+      <c r="A16" s="49">
         <v>43899</v>
       </c>
       <c r="B16" s="13" t="s">
@@ -7685,7 +7737,7 @@
       <c r="H16" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="I16" s="53" t="s">
+      <c r="I16" s="51" t="s">
         <v>16</v>
       </c>
       <c r="J16" s="13">
@@ -7694,10 +7746,10 @@
       <c r="K16" s="13">
         <v>1000</v>
       </c>
-      <c r="L16" s="54" t="s">
+      <c r="L16" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="M16" s="52" t="s">
+      <c r="M16" s="50" t="s">
         <v>119</v>
       </c>
       <c r="N16" s="2"/>
@@ -7756,32 +7808,32 @@
       <c r="A17" s="14">
         <v>43900</v>
       </c>
-      <c r="B17" s="28">
+      <c r="B17" s="26">
         <v>519</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28">
+      <c r="E17" s="26"/>
+      <c r="F17" s="26">
         <v>280</v>
       </c>
-      <c r="G17" s="28">
+      <c r="G17" s="26">
         <v>9.6</v>
       </c>
-      <c r="H17" s="28"/>
-      <c r="I17" s="48" t="s">
+      <c r="H17" s="26"/>
+      <c r="I17" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
       <c r="L17" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="M17" s="39"/>
+      <c r="M17" s="37"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
@@ -7847,13 +7899,11 @@
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
-      <c r="I18" s="13" t="s">
-        <v>45</v>
-      </c>
+      <c r="I18" s="13"/>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
-      <c r="M18" s="39"/>
+      <c r="M18" s="37"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
@@ -7919,19 +7969,11 @@
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
-      <c r="I19" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="J19" s="13">
-        <v>180</v>
-      </c>
-      <c r="K19" s="13">
-        <v>225</v>
-      </c>
-      <c r="L19" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="M19" s="39"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="37"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
@@ -7997,19 +8039,11 @@
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
-      <c r="I20" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="J20" s="13">
-        <v>0</v>
-      </c>
-      <c r="K20" s="13">
-        <v>110</v>
-      </c>
-      <c r="L20" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="M20" s="39"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="37"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
@@ -8075,19 +8109,11 @@
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
-      <c r="I21" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="J21" s="13">
-        <v>0</v>
-      </c>
-      <c r="K21" s="13">
-        <v>1400</v>
-      </c>
-      <c r="L21" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="M21" s="39"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="37"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
@@ -8153,19 +8179,11 @@
       <c r="F22" s="13"/>
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
-      <c r="I22" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="J22" s="13">
-        <v>180</v>
-      </c>
-      <c r="K22" s="13">
-        <v>240</v>
-      </c>
-      <c r="L22" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="M22" s="39"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="37"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
@@ -8231,19 +8249,11 @@
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
-      <c r="I23" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="J23" s="13">
-        <v>0</v>
-      </c>
-      <c r="K23" s="13">
-        <v>1400</v>
-      </c>
-      <c r="L23" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="M23" s="39"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="37"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
@@ -8309,18 +8319,10 @@
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
-      <c r="I24" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="J24" s="13">
-        <v>0</v>
-      </c>
-      <c r="K24" s="13">
-        <v>180</v>
-      </c>
-      <c r="L24" s="13" t="s">
-        <v>57</v>
-      </c>
+      <c r="I24" s="46"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -8387,18 +8389,10 @@
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
-      <c r="I25" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="J25" s="13">
-        <v>220</v>
-      </c>
-      <c r="K25" s="13">
-        <v>270</v>
-      </c>
-      <c r="L25" s="13" t="s">
-        <v>59</v>
-      </c>
+      <c r="I25" s="46"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
@@ -8465,18 +8459,10 @@
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
-      <c r="I26" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="J26" s="13">
-        <v>170</v>
-      </c>
-      <c r="K26" s="13">
-        <v>245</v>
-      </c>
-      <c r="L26" s="13" t="s">
-        <v>63</v>
-      </c>
+      <c r="I26" s="46"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
@@ -8543,18 +8529,10 @@
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
-      <c r="I27" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="J27" s="13">
-        <v>120</v>
-      </c>
-      <c r="K27" s="13">
-        <v>220</v>
-      </c>
-      <c r="L27" s="13" t="s">
-        <v>64</v>
-      </c>
+      <c r="I27" s="46"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -8621,18 +8599,10 @@
       <c r="F28" s="21"/>
       <c r="G28" s="21"/>
       <c r="H28" s="21"/>
-      <c r="I28" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="J28" s="21">
-        <v>140</v>
-      </c>
-      <c r="K28" s="21">
-        <v>205</v>
-      </c>
-      <c r="L28" s="21" t="s">
-        <v>65</v>
-      </c>
+      <c r="I28" s="60"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -10543,10 +10513,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7293150B-6AD7-4206-AAE6-A798C9E6EC4A}">
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10554,21 +10524,21 @@
     <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5546875" customWidth="1"/>
     <col min="4" max="4" width="14.88671875" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" customWidth="1"/>
-    <col min="7" max="7" width="13.77734375" customWidth="1"/>
-    <col min="8" max="8" width="15.44140625" customWidth="1"/>
-    <col min="9" max="9" width="36.33203125" customWidth="1"/>
-    <col min="11" max="11" width="10.88671875" customWidth="1"/>
-    <col min="12" max="12" width="23.44140625" customWidth="1"/>
-    <col min="13" max="13" width="11.77734375" customWidth="1"/>
-    <col min="14" max="14" width="14.88671875" customWidth="1"/>
-    <col min="15" max="15" width="13.33203125" customWidth="1"/>
-    <col min="16" max="16" width="14.77734375" customWidth="1"/>
-    <col min="17" max="17" width="9" customWidth="1"/>
+    <col min="5" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" customWidth="1"/>
+    <col min="10" max="10" width="92.21875" customWidth="1"/>
+    <col min="12" max="12" width="10.88671875" customWidth="1"/>
+    <col min="13" max="13" width="23.44140625" customWidth="1"/>
+    <col min="14" max="14" width="11.77734375" customWidth="1"/>
+    <col min="15" max="15" width="14.88671875" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" customWidth="1"/>
+    <col min="17" max="17" width="14.77734375" customWidth="1"/>
+    <col min="18" max="18" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -10582,10 +10552,11 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
-    </row>
-    <row r="2" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:14" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A2" s="2"/>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="27" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="2"/>
@@ -10597,15 +10568,9 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-    </row>
-    <row r="3" spans="1:17" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -10618,445 +10583,689 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-    </row>
-    <row r="4" spans="1:17" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:14" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="H4" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="32" t="s">
+      <c r="I4" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="J4" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="N4" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="O4" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="P4" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q4" s="32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:14" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="29">
         <v>20.7</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31">
+      <c r="D5" s="29">
+        <v>400</v>
+      </c>
+      <c r="E5" s="29">
+        <v>9.6</v>
+      </c>
+      <c r="F5" s="29">
+        <v>13.4</v>
+      </c>
+      <c r="G5" s="29">
         <v>100</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="H5" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="H5" s="31">
+      <c r="I5" s="29">
         <v>1000</v>
       </c>
-      <c r="I5" s="31"/>
-      <c r="J5" s="2"/>
+      <c r="J5" s="37" t="s">
+        <v>82</v>
+      </c>
       <c r="K5" s="2"/>
-      <c r="L5" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="M5" s="31">
-        <v>20</v>
-      </c>
-      <c r="N5" s="31" t="s">
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="2"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28">
+        <v>20.7</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" s="28">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="F6" s="28">
+        <v>0.3</v>
+      </c>
+      <c r="G6" s="28">
+        <v>100</v>
+      </c>
+      <c r="H6" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="O5" s="31">
-        <v>220</v>
-      </c>
-      <c r="P5" s="31">
-        <v>800</v>
-      </c>
-      <c r="Q5" s="36"/>
-    </row>
-    <row r="6" spans="1:17" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30">
+      <c r="I6" s="28">
+        <v>1000</v>
+      </c>
+      <c r="J6" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2"/>
+      <c r="B7" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="29">
         <v>20.7</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30">
+      <c r="D7" s="29">
+        <v>400</v>
+      </c>
+      <c r="E7" s="29">
+        <v>9.6</v>
+      </c>
+      <c r="F7" s="29">
+        <v>13.2</v>
+      </c>
+      <c r="G7" s="29">
         <v>100</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="H7" s="29">
+        <v>205</v>
+      </c>
+      <c r="I7" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="H6" s="30">
+      <c r="J7" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="2"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28">
+        <v>20.7</v>
+      </c>
+      <c r="D8" s="28">
+        <v>100</v>
+      </c>
+      <c r="E8" s="28">
+        <v>9.6</v>
+      </c>
+      <c r="F8" s="28">
+        <v>2.5</v>
+      </c>
+      <c r="G8" s="28">
+        <v>100</v>
+      </c>
+      <c r="H8" s="28">
+        <v>205</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="J8" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="2"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28">
+        <v>20.7</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="28">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="F9" s="28">
+        <v>0.3</v>
+      </c>
+      <c r="G9" s="28">
+        <v>100</v>
+      </c>
+      <c r="H9" s="28">
+        <v>205</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="J9" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="2"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54">
+        <v>20.7</v>
+      </c>
+      <c r="D10" s="54">
+        <v>300</v>
+      </c>
+      <c r="E10" s="54">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="F10" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="G10" s="54">
+        <v>100</v>
+      </c>
+      <c r="H10" s="54">
+        <v>205</v>
+      </c>
+      <c r="I10" s="54" t="s">
+        <v>71</v>
+      </c>
+      <c r="J10" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="2"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="55">
+        <v>20.7</v>
+      </c>
+      <c r="D11" s="55">
+        <v>280</v>
+      </c>
+      <c r="E11" s="55">
+        <v>9.6</v>
+      </c>
+      <c r="F11" s="46">
+        <v>8.6</v>
+      </c>
+      <c r="G11" s="55">
+        <v>100</v>
+      </c>
+      <c r="H11" s="55">
+        <v>205</v>
+      </c>
+      <c r="I11" s="55">
+        <v>400</v>
+      </c>
+      <c r="J11" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="2"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="55">
+        <v>20.7</v>
+      </c>
+      <c r="D12" s="55">
+        <v>280</v>
+      </c>
+      <c r="E12" s="55">
+        <v>9.6</v>
+      </c>
+      <c r="F12" s="46">
+        <v>8.6</v>
+      </c>
+      <c r="G12" s="55">
+        <v>100</v>
+      </c>
+      <c r="H12" s="55">
+        <v>205</v>
+      </c>
+      <c r="I12" s="55">
         <v>1000</v>
       </c>
-      <c r="I6" s="30"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30">
-        <v>30</v>
-      </c>
-      <c r="N6" s="30" t="s">
+      <c r="J12" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="A13" s="2"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="57">
+        <v>20.7</v>
+      </c>
+      <c r="D13" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" s="57">
+        <v>9.6</v>
+      </c>
+      <c r="F13" s="58">
+        <v>1.6</v>
+      </c>
+      <c r="G13" s="57">
+        <v>100</v>
+      </c>
+      <c r="H13" s="57">
+        <v>205</v>
+      </c>
+      <c r="I13" s="57">
+        <v>400</v>
+      </c>
+      <c r="J13" s="64" t="s">
+        <v>122</v>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="2"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="55">
+        <v>20.7</v>
+      </c>
+      <c r="D14" s="55" t="s">
+        <v>104</v>
+      </c>
+      <c r="E14" s="55">
+        <v>9.6</v>
+      </c>
+      <c r="F14" s="46">
+        <v>1.6</v>
+      </c>
+      <c r="G14" s="55">
+        <v>100</v>
+      </c>
+      <c r="H14" s="55">
+        <v>205</v>
+      </c>
+      <c r="I14" s="55">
+        <v>1000</v>
+      </c>
+      <c r="J14" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="A15" s="2"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="57">
+        <v>20.7</v>
+      </c>
+      <c r="D15" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="57">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="F15" s="58">
+        <v>0.2</v>
+      </c>
+      <c r="G15" s="57">
+        <v>100</v>
+      </c>
+      <c r="H15" s="57">
+        <v>205</v>
+      </c>
+      <c r="I15" s="57">
+        <v>400</v>
+      </c>
+      <c r="J15" s="64" t="s">
+        <v>122</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="2"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="59">
+        <v>20.7</v>
+      </c>
+      <c r="D16" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="59">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="F16" s="60" t="s">
+        <v>108</v>
+      </c>
+      <c r="G16" s="59">
+        <v>100</v>
+      </c>
+      <c r="H16" s="59">
+        <v>205</v>
+      </c>
+      <c r="I16" s="59">
+        <v>1000</v>
+      </c>
+      <c r="J16" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:14" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2"/>
+      <c r="B17" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" s="29">
+        <v>20.7</v>
+      </c>
+      <c r="D17" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="O6" s="30">
-        <v>240</v>
-      </c>
-      <c r="P6" s="30">
-        <v>800</v>
-      </c>
-      <c r="Q6" s="35"/>
-    </row>
-    <row r="7" spans="1:17" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="2"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30">
+      <c r="E17" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17" s="29">
+        <v>100</v>
+      </c>
+      <c r="H17" s="29">
+        <v>205</v>
+      </c>
+      <c r="I17" s="29">
+        <v>400</v>
+      </c>
+      <c r="J17" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="2"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32">
         <v>20.7</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30">
+      <c r="D18" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" s="32">
         <v>100</v>
       </c>
-      <c r="G7" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="H7" s="30">
-        <v>600</v>
-      </c>
-      <c r="I7" s="30"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30">
-        <v>40</v>
-      </c>
-      <c r="N7" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="O7" s="30">
-        <v>260</v>
-      </c>
-      <c r="P7" s="30">
-        <v>700</v>
-      </c>
-      <c r="Q7" s="35"/>
-    </row>
-    <row r="8" spans="1:17" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="31">
-        <v>20.7</v>
-      </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31">
-        <v>120</v>
-      </c>
-      <c r="G8" s="31">
-        <v>220</v>
-      </c>
-      <c r="H8" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="I8" s="31"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="M8" s="31">
-        <v>20</v>
-      </c>
-      <c r="N8" s="31">
-        <v>50</v>
-      </c>
-      <c r="O8" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="P8" s="31">
-        <v>800</v>
-      </c>
-      <c r="Q8" s="36"/>
-    </row>
-    <row r="9" spans="1:17" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30">
-        <v>20.7</v>
-      </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30">
-        <v>100</v>
-      </c>
-      <c r="G9" s="30">
+      <c r="H18" s="32">
         <v>205</v>
       </c>
-      <c r="H9" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="I9" s="30"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30">
-        <v>30</v>
-      </c>
-      <c r="N9" s="30">
-        <v>70</v>
-      </c>
-      <c r="O9" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="P9" s="30">
-        <v>800</v>
-      </c>
-      <c r="Q9" s="35"/>
-    </row>
-    <row r="10" spans="1:17" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30">
-        <v>20.7</v>
-      </c>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30">
-        <v>70</v>
-      </c>
-      <c r="G10" s="30">
-        <v>190</v>
-      </c>
-      <c r="H10" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="I10" s="30"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30">
-        <v>40</v>
-      </c>
-      <c r="N10" s="30">
-        <v>80</v>
-      </c>
-      <c r="O10" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="P10" s="30">
-        <v>700</v>
-      </c>
-      <c r="Q10" s="35"/>
-    </row>
-    <row r="11" spans="1:17" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="2"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34">
-        <v>20.7</v>
-      </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34">
-        <v>70</v>
-      </c>
-      <c r="G11" s="34">
-        <v>170</v>
-      </c>
-      <c r="H11" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="I11" s="34"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30">
-        <v>30</v>
-      </c>
-      <c r="N11" s="30">
-        <v>70</v>
-      </c>
-      <c r="O11" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="P11" s="30">
-        <v>400</v>
-      </c>
-      <c r="Q11" s="35"/>
-    </row>
-    <row r="12" spans="1:17" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="30">
-        <v>20</v>
-      </c>
-      <c r="N12" s="30">
-        <v>80</v>
-      </c>
-      <c r="O12" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="P12" s="30">
-        <v>300</v>
-      </c>
-      <c r="Q12" s="35"/>
-    </row>
-    <row r="13" spans="1:17" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30">
-        <v>10</v>
-      </c>
-      <c r="N13" s="30">
-        <v>50</v>
-      </c>
-      <c r="O13" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="P13" s="30">
-        <v>200</v>
-      </c>
-      <c r="Q13" s="35"/>
-    </row>
-    <row r="14" spans="1:17" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="M14" s="31">
-        <v>30</v>
-      </c>
-      <c r="N14" s="31">
-        <v>70</v>
-      </c>
-      <c r="O14" s="31">
-        <v>240</v>
-      </c>
-      <c r="P14" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q14" s="36"/>
-    </row>
-    <row r="15" spans="1:17" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34">
-        <v>30</v>
-      </c>
-      <c r="N15" s="34">
-        <v>70</v>
-      </c>
-      <c r="O15" s="34">
-        <v>230</v>
-      </c>
-      <c r="P15" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q15" s="37"/>
-    </row>
-    <row r="16" spans="1:17" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:13" ht="18" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="1:13" ht="18" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
-      <c r="J18" s="2"/>
+      <c r="I18" s="32">
+        <v>1000</v>
+      </c>
+      <c r="J18" s="53" t="s">
+        <v>122</v>
+      </c>
       <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-    </row>
-    <row r="20" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
-    </row>
-    <row r="21" spans="1:13" ht="18" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B21" s="27" t="s">
+        <v>72</v>
+      </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-    </row>
+    </row>
+    <row r="22" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="2"/>
+      <c r="C23" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="I23" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="J23" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="37"/>
+    </row>
+    <row r="25" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="53"/>
+    </row>
+    <row r="26" spans="1:14" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="37"/>
+    </row>
+    <row r="27" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="37"/>
+    </row>
+    <row r="28" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="37"/>
+    </row>
+    <row r="29" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B29" s="54"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="50"/>
+    </row>
+    <row r="30" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="B30" s="56"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="55"/>
+      <c r="I30" s="55"/>
+      <c r="J30" s="61"/>
+    </row>
+    <row r="31" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="33"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="62"/>
+    </row>
+    <row r="32" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="B32" s="56"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="57"/>
+      <c r="I32" s="57"/>
+      <c r="J32" s="61"/>
+    </row>
+    <row r="33" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="33"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="55"/>
+      <c r="I33" s="55"/>
+      <c r="J33" s="62"/>
+    </row>
+    <row r="34" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="B34" s="56"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="57"/>
+      <c r="H34" s="57"/>
+      <c r="I34" s="57"/>
+      <c r="J34" s="61"/>
+    </row>
+    <row r="35" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B35" s="35"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="59"/>
+      <c r="H35" s="59"/>
+      <c r="I35" s="59"/>
+      <c r="J35" s="63"/>
+    </row>
+    <row r="36" spans="2:10" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="37"/>
+    </row>
+    <row r="37" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B37" s="32"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="32"/>
+      <c r="J37" s="53"/>
+    </row>
+    <row r="38" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Aggiunto al file excel anche lo schema dei run del test beam con le ROW THGEM. Tale schema è stato dunque completato.
</commit_message>
<xml_diff>
--- a/Caratterizzazione_THGEM.xlsx
+++ b/Caratterizzazione_THGEM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peppe\Desktop\LaTex\Report_THGEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470C0275-4753-4404-994B-BEFD02913C2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F516AE8-95FC-43B3-A0E7-2A3C4C4B3C05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{ACFC7C87-C28D-4487-B063-88156E979354}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{ACFC7C87-C28D-4487-B063-88156E979354}"/>
   </bookViews>
   <sheets>
     <sheet name="alpha-crono" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="157">
   <si>
     <t>DATA</t>
   </si>
@@ -912,6 +912,124 @@
   </si>
   <si>
     <t>This scan was done varying both Ibeam and target</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">At the beginning, MXFC1=670 pA. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TRIP</t>
+    </r>
+  </si>
+  <si>
+    <t>Vind=50    VTG=200    Vdrift=400</t>
+  </si>
+  <si>
+    <t>Discharge</t>
+  </si>
+  <si>
+    <t>At the beginning MXFC1=900 pA</t>
+  </si>
+  <si>
+    <t>521 ÷ 526</t>
+  </si>
+  <si>
+    <t>Vind=50        VTG=195</t>
+  </si>
+  <si>
+    <t>527 ÷ 534</t>
+  </si>
+  <si>
+    <t>535 ÷ 553</t>
+  </si>
+  <si>
+    <t>Scan analogous to the previous one, but with a lower VTHGEM</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A lot of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>discharges</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>!</t>
+    </r>
+  </si>
+  <si>
+    <t>Vind=50    VTG=195    Vdrift=400</t>
+  </si>
+  <si>
+    <t>At the beginning MXFC1=680 pA</t>
+  </si>
+  <si>
+    <t>556 ÷ 565</t>
+  </si>
+  <si>
+    <t>Vind=50        VTG=190</t>
+  </si>
+  <si>
+    <t>At the beginning MXFC1=250 pA. Little discharges</t>
+  </si>
+  <si>
+    <t>566 ÷ 572</t>
+  </si>
+  <si>
+    <t>At the beginning MXFC1=110 pA</t>
+  </si>
+  <si>
+    <t>573 ÷ 582</t>
+  </si>
+  <si>
+    <t>At the beginning MXFC1=680 pA. Little discharges in the first 6 runs</t>
+  </si>
+  <si>
+    <t>583 ÷ 601</t>
+  </si>
+  <si>
+    <t>At the beginning MXFC1=250 pA. Little discharges in the some runs</t>
+  </si>
+  <si>
+    <t>602 ÷ 610</t>
+  </si>
+  <si>
+    <t>At the beginning and at the end, MXFC1=250 pA</t>
+  </si>
+  <si>
+    <t>Vind=50    VTG=190    Vdrift=400</t>
+  </si>
+  <si>
+    <t>50 ÷ 200 (~160)</t>
+  </si>
+  <si>
+    <t>Vind=50    VTG=190    Vdrift=1000</t>
+  </si>
+  <si>
+    <t>At the beginning MXFC1=680 pA. Single points  that can be added to the IBF plot</t>
+  </si>
+  <si>
+    <t>At the beginning MXFC1=110 pA. Single points  that can be added to the IBF plot</t>
   </si>
 </sst>
 </file>
@@ -1135,7 +1253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1303,16 +1421,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6347,10 +6472,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E260431C-5552-43E0-806B-E171CCC2519A}">
-  <dimension ref="A1:BL56"/>
+  <dimension ref="A1:BL58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView topLeftCell="H10" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6360,7 +6485,7 @@
     <col min="3" max="3" width="12.21875" customWidth="1"/>
     <col min="4" max="4" width="10.21875" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" customWidth="1"/>
     <col min="7" max="7" width="18.5546875" customWidth="1"/>
     <col min="8" max="8" width="15.109375" customWidth="1"/>
     <col min="9" max="9" width="21.21875" customWidth="1"/>
@@ -7817,14 +7942,18 @@
       <c r="D17" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="26"/>
+      <c r="E17" s="26">
+        <v>20.7</v>
+      </c>
       <c r="F17" s="26">
         <v>280</v>
       </c>
       <c r="G17" s="26">
         <v>9.6</v>
       </c>
-      <c r="H17" s="26"/>
+      <c r="H17" s="26" t="s">
+        <v>77</v>
+      </c>
       <c r="I17" s="46" t="s">
         <v>77</v>
       </c>
@@ -7833,7 +7962,9 @@
       <c r="L17" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="M17" s="37"/>
+      <c r="M17" s="37" t="s">
+        <v>129</v>
+      </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
@@ -7887,23 +8018,41 @@
       <c r="BL17" s="1"/>
     </row>
     <row r="18" spans="1:64" ht="18" x14ac:dyDescent="0.35">
-      <c r="A18" s="14"/>
-      <c r="B18" s="12"/>
+      <c r="A18" s="14">
+        <v>43900</v>
+      </c>
+      <c r="B18" s="13">
+        <v>520</v>
+      </c>
       <c r="C18" s="13" t="s">
         <v>41</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
+      <c r="E18" s="13">
+        <v>20.7</v>
+      </c>
+      <c r="F18" s="13">
+        <v>280</v>
+      </c>
+      <c r="G18" s="13">
+        <v>9.6</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>77</v>
+      </c>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="37"/>
+      <c r="L18" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="M18" s="63" t="s">
+        <v>131</v>
+      </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
@@ -7957,23 +8106,45 @@
       <c r="BL18" s="1"/>
     </row>
     <row r="19" spans="1:64" ht="18" x14ac:dyDescent="0.35">
-      <c r="A19" s="14"/>
-      <c r="B19" s="12"/>
+      <c r="A19" s="14">
+        <v>43900</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>133</v>
+      </c>
       <c r="C19" s="13" t="s">
         <v>41</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="37"/>
+      <c r="E19" s="13">
+        <v>20.7</v>
+      </c>
+      <c r="F19" s="13">
+        <v>400</v>
+      </c>
+      <c r="G19" s="13">
+        <v>9.6</v>
+      </c>
+      <c r="H19" s="13">
+        <v>14.9</v>
+      </c>
+      <c r="I19" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" s="13">
+        <v>170</v>
+      </c>
+      <c r="K19" s="13">
+        <v>200</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="M19" s="37" t="s">
+        <v>132</v>
+      </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
@@ -8027,23 +8198,45 @@
       <c r="BL19" s="1"/>
     </row>
     <row r="20" spans="1:64" ht="18" x14ac:dyDescent="0.35">
-      <c r="A20" s="14"/>
-      <c r="B20" s="12"/>
+      <c r="A20" s="14">
+        <v>43900</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>135</v>
+      </c>
       <c r="C20" s="13" t="s">
         <v>41</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="37"/>
+      <c r="E20" s="13">
+        <v>20.7</v>
+      </c>
+      <c r="F20" s="13">
+        <v>400</v>
+      </c>
+      <c r="G20" s="13">
+        <v>9.6</v>
+      </c>
+      <c r="H20" s="13">
+        <v>14.8</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" s="13">
+        <v>30</v>
+      </c>
+      <c r="K20" s="13">
+        <v>600</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="M20" s="37" t="s">
+        <v>138</v>
+      </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
@@ -8097,23 +8290,45 @@
       <c r="BL20" s="1"/>
     </row>
     <row r="21" spans="1:64" ht="18" x14ac:dyDescent="0.35">
-      <c r="A21" s="14"/>
-      <c r="B21" s="12"/>
+      <c r="A21" s="14">
+        <v>43900</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>136</v>
+      </c>
       <c r="C21" s="13" t="s">
         <v>41</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="37"/>
+      <c r="E21" s="13">
+        <v>20.7</v>
+      </c>
+      <c r="F21" s="13">
+        <v>400</v>
+      </c>
+      <c r="G21" s="13">
+        <v>9.6</v>
+      </c>
+      <c r="H21" s="13">
+        <v>14.9</v>
+      </c>
+      <c r="I21" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" s="13">
+        <v>30</v>
+      </c>
+      <c r="K21" s="13">
+        <v>1000</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="M21" s="37" t="s">
+        <v>137</v>
+      </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
@@ -8167,23 +8382,41 @@
       <c r="BL21" s="1"/>
     </row>
     <row r="22" spans="1:64" ht="18" x14ac:dyDescent="0.35">
-      <c r="A22" s="14"/>
-      <c r="B22" s="12"/>
+      <c r="A22" s="14">
+        <v>43900</v>
+      </c>
+      <c r="B22" s="13">
+        <v>554</v>
+      </c>
       <c r="C22" s="13" t="s">
         <v>41</v>
       </c>
       <c r="D22" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="46"/>
+      <c r="E22" s="13">
+        <v>20.7</v>
+      </c>
+      <c r="F22" s="13">
+        <v>280</v>
+      </c>
+      <c r="G22" s="13">
+        <v>9.6</v>
+      </c>
+      <c r="H22" s="13">
+        <v>8.9</v>
+      </c>
+      <c r="I22" s="46" t="s">
+        <v>77</v>
+      </c>
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="37"/>
+      <c r="L22" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="M22" s="37" t="s">
+        <v>140</v>
+      </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
@@ -8237,22 +8470,38 @@
       <c r="BL22" s="1"/>
     </row>
     <row r="23" spans="1:64" ht="18" x14ac:dyDescent="0.35">
-      <c r="A23" s="14"/>
-      <c r="B23" s="12"/>
+      <c r="A23" s="14">
+        <v>43900</v>
+      </c>
+      <c r="B23" s="13">
+        <v>555</v>
+      </c>
       <c r="C23" s="13" t="s">
         <v>41</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="46"/>
+      <c r="E23" s="13">
+        <v>20.7</v>
+      </c>
+      <c r="F23" s="13">
+        <v>280</v>
+      </c>
+      <c r="G23" s="13">
+        <v>9.6</v>
+      </c>
+      <c r="H23" s="13">
+        <v>9.5</v>
+      </c>
+      <c r="I23" s="46" t="s">
+        <v>77</v>
+      </c>
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
+      <c r="L23" s="13" t="s">
+        <v>154</v>
+      </c>
       <c r="M23" s="37"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -8307,23 +8556,45 @@
       <c r="BL23" s="1"/>
     </row>
     <row r="24" spans="1:64" ht="18" x14ac:dyDescent="0.35">
-      <c r="A24" s="14"/>
-      <c r="B24" s="12"/>
+      <c r="A24" s="14">
+        <v>43900</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="C24" s="13" t="s">
         <v>41</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="2"/>
+      <c r="E24" s="13">
+        <v>20.7</v>
+      </c>
+      <c r="F24" s="13">
+        <v>150</v>
+      </c>
+      <c r="G24" s="13">
+        <v>9.6</v>
+      </c>
+      <c r="H24" s="13">
+        <v>3.4</v>
+      </c>
+      <c r="I24" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" s="13">
+        <v>100</v>
+      </c>
+      <c r="K24" s="13">
+        <v>1000</v>
+      </c>
+      <c r="L24" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="M24" s="37" t="s">
+        <v>143</v>
+      </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
@@ -8377,23 +8648,45 @@
       <c r="BL24" s="1"/>
     </row>
     <row r="25" spans="1:64" ht="18" x14ac:dyDescent="0.35">
-      <c r="A25" s="14"/>
-      <c r="B25" s="12"/>
+      <c r="A25" s="14">
+        <v>43900</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>144</v>
+      </c>
       <c r="C25" s="13" t="s">
         <v>41</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="2"/>
+      <c r="E25" s="13">
+        <v>20.7</v>
+      </c>
+      <c r="F25" s="13">
+        <v>60</v>
+      </c>
+      <c r="G25" s="13">
+        <v>9.6</v>
+      </c>
+      <c r="H25" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="I25" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" s="13">
+        <v>400</v>
+      </c>
+      <c r="K25" s="13">
+        <v>1000</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="M25" s="37" t="s">
+        <v>145</v>
+      </c>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
@@ -8447,23 +8740,45 @@
       <c r="BL25" s="1"/>
     </row>
     <row r="26" spans="1:64" ht="18" x14ac:dyDescent="0.35">
-      <c r="A26" s="14"/>
-      <c r="B26" s="12"/>
+      <c r="A26" s="14">
+        <v>43900</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>146</v>
+      </c>
       <c r="C26" s="13" t="s">
         <v>41</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="2"/>
+      <c r="E26" s="13">
+        <v>20.7</v>
+      </c>
+      <c r="F26" s="13">
+        <v>280</v>
+      </c>
+      <c r="G26" s="13">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="H26" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="I26" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" s="13">
+        <v>100</v>
+      </c>
+      <c r="K26" s="13">
+        <v>1000</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="M26" s="37" t="s">
+        <v>147</v>
+      </c>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
@@ -8517,23 +8832,45 @@
       <c r="BL26" s="1"/>
     </row>
     <row r="27" spans="1:64" ht="18" x14ac:dyDescent="0.35">
-      <c r="A27" s="14"/>
-      <c r="B27" s="12"/>
+      <c r="A27" s="14">
+        <v>43900</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>148</v>
+      </c>
       <c r="C27" s="13" t="s">
         <v>41</v>
       </c>
       <c r="D27" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="46"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="2"/>
+      <c r="E27" s="13">
+        <v>20.7</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="G27" s="13">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="H27" s="13">
+        <v>0.4</v>
+      </c>
+      <c r="I27" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J27" s="13">
+        <v>30</v>
+      </c>
+      <c r="K27" s="13">
+        <v>1000</v>
+      </c>
+      <c r="L27" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="M27" s="37" t="s">
+        <v>149</v>
+      </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
@@ -8586,24 +8923,46 @@
       <c r="BK27" s="1"/>
       <c r="BL27" s="1"/>
     </row>
-    <row r="28" spans="1:64" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="19"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="21" t="s">
+    <row r="28" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="A28" s="14">
+        <v>43900</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="C28" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D28" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="60"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
-      <c r="L28" s="21"/>
-      <c r="M28" s="2"/>
+      <c r="E28" s="13">
+        <v>20.7</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="G28" s="13">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="H28" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="I28" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J28" s="13">
+        <v>170</v>
+      </c>
+      <c r="K28" s="13">
+        <v>205</v>
+      </c>
+      <c r="L28" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="M28" s="37" t="s">
+        <v>151</v>
+      </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
@@ -8656,20 +9015,42 @@
       <c r="BK28" s="1"/>
       <c r="BL28" s="1"/>
     </row>
-    <row r="29" spans="1:64" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="15"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
-      <c r="M29" s="18"/>
+    <row r="29" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="A29" s="14">
+        <v>43900</v>
+      </c>
+      <c r="B29" s="13">
+        <v>611</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="13">
+        <v>20.7</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="G29" s="13">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="H29" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="I29" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="M29" s="37" t="s">
+        <v>145</v>
+      </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
@@ -8722,20 +9103,40 @@
       <c r="BK29" s="1"/>
       <c r="BL29" s="1"/>
     </row>
-    <row r="30" spans="1:64" ht="18" x14ac:dyDescent="0.35">
-      <c r="A30" s="15"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="18"/>
+    <row r="30" spans="1:64" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="19">
+        <v>43900</v>
+      </c>
+      <c r="B30" s="21">
+        <v>612</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" s="21">
+        <v>20.7</v>
+      </c>
+      <c r="F30" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="G30" s="21">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="H30" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="I30" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="M30" s="53"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
@@ -8788,20 +9189,20 @@
       <c r="BK30" s="1"/>
       <c r="BL30" s="1"/>
     </row>
-    <row r="31" spans="1:64" ht="18" x14ac:dyDescent="0.35">
-      <c r="A31" s="3"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="2"/>
+    <row r="31" spans="1:64" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="15"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="18"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
@@ -8855,19 +9256,19 @@
       <c r="BL31" s="1"/>
     </row>
     <row r="32" spans="1:64" ht="18" x14ac:dyDescent="0.35">
-      <c r="A32" s="3"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="18"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
@@ -8923,16 +9324,16 @@
     <row r="33" spans="1:64" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="5"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -10504,6 +10905,138 @@
       <c r="BK56" s="1"/>
       <c r="BL56" s="1"/>
     </row>
+    <row r="57" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="A57" s="3"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
+      <c r="O57" s="2"/>
+      <c r="P57" s="2"/>
+      <c r="Q57" s="2"/>
+      <c r="R57" s="2"/>
+      <c r="S57" s="2"/>
+      <c r="T57" s="2"/>
+      <c r="U57" s="2"/>
+      <c r="V57" s="2"/>
+      <c r="W57" s="2"/>
+      <c r="X57" s="2"/>
+      <c r="Y57" s="2"/>
+      <c r="Z57" s="1"/>
+      <c r="AA57" s="1"/>
+      <c r="AB57" s="1"/>
+      <c r="AC57" s="1"/>
+      <c r="AD57" s="1"/>
+      <c r="AE57" s="1"/>
+      <c r="AF57" s="1"/>
+      <c r="AG57" s="1"/>
+      <c r="AH57" s="1"/>
+      <c r="AI57" s="1"/>
+      <c r="AJ57" s="1"/>
+      <c r="AK57" s="1"/>
+      <c r="AL57" s="1"/>
+      <c r="AM57" s="1"/>
+      <c r="AN57" s="1"/>
+      <c r="AO57" s="1"/>
+      <c r="AP57" s="1"/>
+      <c r="AQ57" s="1"/>
+      <c r="AR57" s="1"/>
+      <c r="AS57" s="1"/>
+      <c r="AT57" s="1"/>
+      <c r="AU57" s="1"/>
+      <c r="AV57" s="1"/>
+      <c r="AW57" s="1"/>
+      <c r="AX57" s="1"/>
+      <c r="AY57" s="1"/>
+      <c r="AZ57" s="1"/>
+      <c r="BA57" s="1"/>
+      <c r="BB57" s="1"/>
+      <c r="BC57" s="1"/>
+      <c r="BD57" s="1"/>
+      <c r="BE57" s="1"/>
+      <c r="BF57" s="1"/>
+      <c r="BG57" s="1"/>
+      <c r="BH57" s="1"/>
+      <c r="BI57" s="1"/>
+      <c r="BJ57" s="1"/>
+      <c r="BK57" s="1"/>
+      <c r="BL57" s="1"/>
+    </row>
+    <row r="58" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="A58" s="3"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
+      <c r="O58" s="2"/>
+      <c r="P58" s="2"/>
+      <c r="Q58" s="2"/>
+      <c r="R58" s="2"/>
+      <c r="S58" s="2"/>
+      <c r="T58" s="2"/>
+      <c r="U58" s="2"/>
+      <c r="V58" s="2"/>
+      <c r="W58" s="2"/>
+      <c r="X58" s="2"/>
+      <c r="Y58" s="2"/>
+      <c r="Z58" s="1"/>
+      <c r="AA58" s="1"/>
+      <c r="AB58" s="1"/>
+      <c r="AC58" s="1"/>
+      <c r="AD58" s="1"/>
+      <c r="AE58" s="1"/>
+      <c r="AF58" s="1"/>
+      <c r="AG58" s="1"/>
+      <c r="AH58" s="1"/>
+      <c r="AI58" s="1"/>
+      <c r="AJ58" s="1"/>
+      <c r="AK58" s="1"/>
+      <c r="AL58" s="1"/>
+      <c r="AM58" s="1"/>
+      <c r="AN58" s="1"/>
+      <c r="AO58" s="1"/>
+      <c r="AP58" s="1"/>
+      <c r="AQ58" s="1"/>
+      <c r="AR58" s="1"/>
+      <c r="AS58" s="1"/>
+      <c r="AT58" s="1"/>
+      <c r="AU58" s="1"/>
+      <c r="AV58" s="1"/>
+      <c r="AW58" s="1"/>
+      <c r="AX58" s="1"/>
+      <c r="AY58" s="1"/>
+      <c r="AZ58" s="1"/>
+      <c r="BA58" s="1"/>
+      <c r="BB58" s="1"/>
+      <c r="BC58" s="1"/>
+      <c r="BD58" s="1"/>
+      <c r="BE58" s="1"/>
+      <c r="BF58" s="1"/>
+      <c r="BG58" s="1"/>
+      <c r="BH58" s="1"/>
+      <c r="BI58" s="1"/>
+      <c r="BJ58" s="1"/>
+      <c r="BK58" s="1"/>
+      <c r="BL58" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10515,15 +11048,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7293150B-6AD7-4206-AAE6-A798C9E6EC4A}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="7.5546875" customWidth="1"/>
     <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5546875" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
     <col min="5" max="6" width="20.6640625" customWidth="1"/>
     <col min="7" max="7" width="15.21875" customWidth="1"/>
     <col min="8" max="8" width="13.77734375" customWidth="1"/>
@@ -10822,7 +11356,7 @@
       <c r="I11" s="55">
         <v>400</v>
       </c>
-      <c r="J11" s="64" t="s">
+      <c r="J11" s="62" t="s">
         <v>121</v>
       </c>
       <c r="K11" s="2"/>
@@ -10882,7 +11416,7 @@
       <c r="I13" s="57">
         <v>400</v>
       </c>
-      <c r="J13" s="64" t="s">
+      <c r="J13" s="62" t="s">
         <v>122</v>
       </c>
       <c r="K13" s="2"/>
@@ -10942,7 +11476,7 @@
       <c r="I15" s="57">
         <v>400</v>
       </c>
-      <c r="J15" s="64" t="s">
+      <c r="J15" s="62" t="s">
         <v>122</v>
       </c>
       <c r="K15" s="2"/>
@@ -11109,161 +11643,381 @@
       <c r="B24" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="37"/>
+      <c r="C24" s="29">
+        <v>20.7</v>
+      </c>
+      <c r="D24" s="29">
+        <v>400</v>
+      </c>
+      <c r="E24" s="29">
+        <v>9.6</v>
+      </c>
+      <c r="F24" s="29">
+        <v>14.9</v>
+      </c>
+      <c r="G24" s="29">
+        <v>50</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="I24" s="29">
+        <v>800</v>
+      </c>
+      <c r="J24" s="37" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="25" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="53"/>
+      <c r="C25" s="28">
+        <v>20.7</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="E25" s="28">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="F25" s="28">
+        <v>0.3</v>
+      </c>
+      <c r="G25" s="28">
+        <v>50</v>
+      </c>
+      <c r="H25" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="I25" s="28">
+        <v>800</v>
+      </c>
+      <c r="J25" s="53" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="26" spans="1:14" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B26" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="37"/>
+      <c r="C26" s="29">
+        <v>20.7</v>
+      </c>
+      <c r="D26" s="29">
+        <v>400</v>
+      </c>
+      <c r="E26" s="29">
+        <v>9.6</v>
+      </c>
+      <c r="F26" s="29">
+        <v>14.8</v>
+      </c>
+      <c r="G26" s="29">
+        <v>50</v>
+      </c>
+      <c r="H26" s="29">
+        <v>195</v>
+      </c>
+      <c r="I26" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="J26" s="37" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="27" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="37"/>
+      <c r="C27" s="28">
+        <v>20.7</v>
+      </c>
+      <c r="D27" s="28">
+        <v>400</v>
+      </c>
+      <c r="E27" s="28">
+        <v>9.6</v>
+      </c>
+      <c r="F27" s="28">
+        <v>14.9</v>
+      </c>
+      <c r="G27" s="28">
+        <v>50</v>
+      </c>
+      <c r="H27" s="28">
+        <v>190</v>
+      </c>
+      <c r="I27" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="J27" s="37" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="28" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="37"/>
-    </row>
-    <row r="29" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="54"/>
-      <c r="C29" s="54"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="54"/>
-      <c r="H29" s="54"/>
-      <c r="I29" s="54"/>
-      <c r="J29" s="50"/>
+      <c r="C28" s="28">
+        <v>20.7</v>
+      </c>
+      <c r="D28" s="28">
+        <v>150</v>
+      </c>
+      <c r="E28" s="28">
+        <v>9.6</v>
+      </c>
+      <c r="F28" s="28">
+        <v>3.4</v>
+      </c>
+      <c r="G28" s="28">
+        <v>50</v>
+      </c>
+      <c r="H28" s="28">
+        <v>190</v>
+      </c>
+      <c r="I28" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="J28" s="37" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="B29" s="28"/>
+      <c r="C29" s="28">
+        <v>20.7</v>
+      </c>
+      <c r="D29" s="28">
+        <v>60</v>
+      </c>
+      <c r="E29" s="28">
+        <v>9.6</v>
+      </c>
+      <c r="F29" s="28">
+        <v>1.5</v>
+      </c>
+      <c r="G29" s="28">
+        <v>50</v>
+      </c>
+      <c r="H29" s="28">
+        <v>190</v>
+      </c>
+      <c r="I29" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="J29" s="37" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="30" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="B30" s="56"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="55"/>
-      <c r="J30" s="61"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28">
+        <v>20.7</v>
+      </c>
+      <c r="D30" s="28">
+        <v>280</v>
+      </c>
+      <c r="E30" s="28">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="F30" s="28">
+        <v>0.9</v>
+      </c>
+      <c r="G30" s="28">
+        <v>50</v>
+      </c>
+      <c r="H30" s="28">
+        <v>190</v>
+      </c>
+      <c r="I30" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="J30" s="37" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="31" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="33"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="55"/>
-      <c r="H31" s="55"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="62"/>
+      <c r="B31" s="54"/>
+      <c r="C31" s="54">
+        <v>20.7</v>
+      </c>
+      <c r="D31" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="E31" s="54">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="F31" s="52">
+        <v>0.4</v>
+      </c>
+      <c r="G31" s="54">
+        <v>50</v>
+      </c>
+      <c r="H31" s="54">
+        <v>190</v>
+      </c>
+      <c r="I31" s="54" t="s">
+        <v>71</v>
+      </c>
+      <c r="J31" s="37" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="32" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="B32" s="56"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="57"/>
-      <c r="H32" s="57"/>
-      <c r="I32" s="57"/>
-      <c r="J32" s="61"/>
+      <c r="C32" s="55">
+        <v>20.7</v>
+      </c>
+      <c r="D32" s="55">
+        <v>280</v>
+      </c>
+      <c r="E32" s="55">
+        <v>9.6</v>
+      </c>
+      <c r="F32" s="46">
+        <v>8.9</v>
+      </c>
+      <c r="G32" s="55">
+        <v>50</v>
+      </c>
+      <c r="H32" s="55">
+        <v>190</v>
+      </c>
+      <c r="I32" s="55">
+        <v>400</v>
+      </c>
+      <c r="J32" s="62" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="33" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="33"/>
-      <c r="C33" s="55"/>
-      <c r="D33" s="55"/>
-      <c r="E33" s="55"/>
-      <c r="F33" s="46"/>
-      <c r="G33" s="55"/>
-      <c r="H33" s="55"/>
-      <c r="I33" s="55"/>
-      <c r="J33" s="62"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="65">
+        <v>20.7</v>
+      </c>
+      <c r="D33" s="65">
+        <v>280</v>
+      </c>
+      <c r="E33" s="65">
+        <v>9.6</v>
+      </c>
+      <c r="F33" s="66">
+        <v>9.5</v>
+      </c>
+      <c r="G33" s="65">
+        <v>50</v>
+      </c>
+      <c r="H33" s="65">
+        <v>190</v>
+      </c>
+      <c r="I33" s="65">
+        <v>1000</v>
+      </c>
+      <c r="J33" s="67"/>
     </row>
     <row r="34" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B34" s="56"/>
-      <c r="C34" s="57"/>
-      <c r="D34" s="57"/>
-      <c r="E34" s="57"/>
-      <c r="F34" s="58"/>
-      <c r="G34" s="57"/>
-      <c r="H34" s="57"/>
-      <c r="I34" s="57"/>
-      <c r="J34" s="61"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="55">
+        <v>20.7</v>
+      </c>
+      <c r="D34" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="E34" s="55">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="F34" s="46">
+        <v>0.2</v>
+      </c>
+      <c r="G34" s="55">
+        <v>50</v>
+      </c>
+      <c r="H34" s="55">
+        <v>190</v>
+      </c>
+      <c r="I34" s="55">
+        <v>400</v>
+      </c>
+      <c r="J34" s="37" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="35" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="35"/>
-      <c r="C35" s="59"/>
-      <c r="D35" s="59"/>
-      <c r="E35" s="59"/>
-      <c r="F35" s="60"/>
-      <c r="G35" s="59"/>
-      <c r="H35" s="59"/>
-      <c r="I35" s="59"/>
-      <c r="J35" s="63"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="55">
+        <v>20.7</v>
+      </c>
+      <c r="D35" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="E35" s="55">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="F35" s="46">
+        <v>0.2</v>
+      </c>
+      <c r="G35" s="55">
+        <v>50</v>
+      </c>
+      <c r="H35" s="55">
+        <v>190</v>
+      </c>
+      <c r="I35" s="55">
+        <v>1000</v>
+      </c>
+      <c r="J35" s="61"/>
     </row>
     <row r="36" spans="2:10" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B36" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="29"/>
-      <c r="J36" s="37"/>
+      <c r="C36" s="29">
+        <v>20.7</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="F36" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="G36" s="29">
+        <v>50</v>
+      </c>
+      <c r="H36" s="29">
+        <v>190</v>
+      </c>
+      <c r="I36" s="29">
+        <v>400</v>
+      </c>
+      <c r="J36" s="37" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="37" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="32"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="53"/>
+      <c r="C37" s="32">
+        <v>20.7</v>
+      </c>
+      <c r="D37" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="E37" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F37" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="G37" s="32">
+        <v>50</v>
+      </c>
+      <c r="H37" s="32">
+        <v>190</v>
+      </c>
+      <c r="I37" s="32">
+        <v>1000</v>
+      </c>
+      <c r="J37" s="53" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="38" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>

</xml_diff>

<commit_message>
Corretta la dicitura <Rate> in <Rate_PD>, a sottolineare che quello è il rate misurato dal fotodiodo
</commit_message>
<xml_diff>
--- a/Caratterizzazione_THGEM.xlsx
+++ b/Caratterizzazione_THGEM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peppe\Desktop\LaTex\Report_THGEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F516AE8-95FC-43B3-A0E7-2A3C4C4B3C05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C6500B-6334-43DE-B308-8C71B6906462}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{ACFC7C87-C28D-4487-B063-88156E979354}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="152">
   <si>
     <t>DATA</t>
   </si>
@@ -633,9 +633,6 @@
     <t>Vind=100    VTG=160    Vdrift=1000</t>
   </si>
   <si>
-    <t>&lt;Rate&gt; (Hz)</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">454 </t>
     </r>
@@ -894,18 +891,6 @@
   </si>
   <si>
     <t>"</t>
-  </si>
-  <si>
-    <t>Somma</t>
-  </si>
-  <si>
-    <t>Media</t>
-  </si>
-  <si>
-    <t>Totale parziale</t>
-  </si>
-  <si>
-    <t>Conteggio</t>
   </si>
   <si>
     <t>Ibeam</t>
@@ -978,9 +963,6 @@
     </r>
   </si>
   <si>
-    <t>Vind=50    VTG=195    Vdrift=400</t>
-  </si>
-  <si>
     <t>At the beginning MXFC1=680 pA</t>
   </si>
   <si>
@@ -1030,6 +1012,9 @@
   </si>
   <si>
     <t>At the beginning MXFC1=110 pA. Single points  that can be added to the IBF plot</t>
+  </si>
+  <si>
+    <t>&lt;Rate_PD&gt; (Hz)</t>
   </si>
 </sst>
 </file>
@@ -2995,7 +2980,7 @@
         <v>43881</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C16" s="28" t="s">
         <v>10</v>
@@ -3016,7 +3001,7 @@
         <v>210</v>
       </c>
       <c r="I16" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -3076,7 +3061,7 @@
         <v>43881</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C17" s="28" t="s">
         <v>10</v>
@@ -3097,7 +3082,7 @@
         <v>600</v>
       </c>
       <c r="I17" s="28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -4123,7 +4108,7 @@
         <v>43865</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C30" s="28" t="s">
         <v>41</v>
@@ -4144,7 +4129,7 @@
         <v>1000</v>
       </c>
       <c r="I30" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
@@ -4204,7 +4189,7 @@
         <v>43865</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C31" s="28" t="s">
         <v>41</v>
@@ -4225,7 +4210,7 @@
         <v>140</v>
       </c>
       <c r="I31" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
@@ -4285,7 +4270,7 @@
         <v>43865</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C32" s="32" t="s">
         <v>41</v>
@@ -4306,7 +4291,7 @@
         <v>800</v>
       </c>
       <c r="I32" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
@@ -6286,7 +6271,7 @@
         <v>400</v>
       </c>
       <c r="G15" s="44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -6445,7 +6430,7 @@
         <v>71</v>
       </c>
       <c r="G20" s="45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -6474,8 +6459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E260431C-5552-43E0-806B-E171CCC2519A}">
   <dimension ref="A1:BL58"/>
   <sheetViews>
-    <sheetView topLeftCell="H10" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6487,7 +6472,7 @@
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="6" max="6" width="18.109375" customWidth="1"/>
     <col min="7" max="7" width="18.5546875" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.21875" customWidth="1"/>
     <col min="10" max="10" width="11.88671875" customWidth="1"/>
     <col min="11" max="11" width="11.33203125" customWidth="1"/>
@@ -6520,7 +6505,7 @@
         <v>78</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>80</v>
+        <v>151</v>
       </c>
       <c r="I1" s="9" t="s">
         <v>5</v>
@@ -6623,7 +6608,7 @@
         <v>79</v>
       </c>
       <c r="M2" s="37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -6682,7 +6667,7 @@
         <v>43899</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>10</v>
@@ -6715,7 +6700,7 @@
         <v>25</v>
       </c>
       <c r="M3" s="37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -6774,7 +6759,7 @@
         <v>43899</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>10</v>
@@ -6807,7 +6792,7 @@
         <v>27</v>
       </c>
       <c r="M4" s="37" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -6892,10 +6877,10 @@
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M5" s="37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -6980,7 +6965,7 @@
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M6" s="37"/>
       <c r="N6" s="2"/>
@@ -7040,7 +7025,7 @@
         <v>43899</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>10</v>
@@ -7073,7 +7058,7 @@
         <v>27</v>
       </c>
       <c r="M7" s="37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -7144,7 +7129,7 @@
         <v>20.7</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G8" s="13">
         <v>9.6</v>
@@ -7158,10 +7143,10 @@
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
       <c r="L8" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M8" s="37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -7232,7 +7217,7 @@
         <v>20.7</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G9" s="13">
         <v>9.6</v>
@@ -7246,10 +7231,10 @@
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
       <c r="L9" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M9" s="37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -7320,7 +7305,7 @@
         <v>20.7</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G10" s="13">
         <v>0.97199999999999998</v>
@@ -7334,10 +7319,10 @@
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M10" s="37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -7408,13 +7393,13 @@
         <v>20.7</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G11" s="13">
         <v>0.97199999999999998</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I11" s="46" t="s">
         <v>77</v>
@@ -7422,10 +7407,10 @@
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M11" s="37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -7484,7 +7469,7 @@
         <v>43899</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>10</v>
@@ -7496,7 +7481,7 @@
         <v>20.7</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G12" s="13">
         <v>0.97199999999999998</v>
@@ -7517,7 +7502,7 @@
         <v>27</v>
       </c>
       <c r="M12" s="37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -7576,7 +7561,7 @@
         <v>43899</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>10</v>
@@ -7588,7 +7573,7 @@
         <v>20.7</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G13" s="13">
         <v>0.97199999999999998</v>
@@ -7609,7 +7594,7 @@
         <v>25</v>
       </c>
       <c r="M13" s="37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -7680,7 +7665,7 @@
         <v>20.7</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G14" s="13">
         <v>0.97199999999999998</v>
@@ -7694,10 +7679,10 @@
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M14" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -7756,7 +7741,7 @@
         <v>43899</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>10</v>
@@ -7783,7 +7768,7 @@
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
       <c r="M15" s="48" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -7842,7 +7827,7 @@
         <v>43899</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>10</v>
@@ -7860,7 +7845,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I16" s="51" t="s">
         <v>16</v>
@@ -7872,10 +7857,10 @@
         <v>1000</v>
       </c>
       <c r="L16" s="52" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M16" s="50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -7960,10 +7945,10 @@
       <c r="J17" s="26"/>
       <c r="K17" s="26"/>
       <c r="L17" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M17" s="37" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
@@ -8048,10 +8033,10 @@
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="M18" s="63" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -8110,7 +8095,7 @@
         <v>43900</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>41</v>
@@ -8143,7 +8128,7 @@
         <v>47</v>
       </c>
       <c r="M19" s="37" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
@@ -8202,7 +8187,7 @@
         <v>43900</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>41</v>
@@ -8232,10 +8217,10 @@
         <v>600</v>
       </c>
       <c r="L20" s="13" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="M20" s="37" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -8294,7 +8279,7 @@
         <v>43900</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>41</v>
@@ -8324,10 +8309,10 @@
         <v>1000</v>
       </c>
       <c r="L21" s="13" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="M21" s="37" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -8412,10 +8397,10 @@
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
       <c r="L22" s="13" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="M22" s="37" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -8500,7 +8485,7 @@
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
       <c r="L23" s="13" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="M23" s="37"/>
       <c r="N23" s="2"/>
@@ -8560,7 +8545,7 @@
         <v>43900</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>41</v>
@@ -8590,10 +8575,10 @@
         <v>1000</v>
       </c>
       <c r="L24" s="13" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="M24" s="37" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -8652,7 +8637,7 @@
         <v>43900</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>41</v>
@@ -8682,10 +8667,10 @@
         <v>1000</v>
       </c>
       <c r="L25" s="13" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="M25" s="37" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
@@ -8744,7 +8729,7 @@
         <v>43900</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>41</v>
@@ -8774,10 +8759,10 @@
         <v>1000</v>
       </c>
       <c r="L26" s="13" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="M26" s="37" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
@@ -8836,7 +8821,7 @@
         <v>43900</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>41</v>
@@ -8848,7 +8833,7 @@
         <v>20.7</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="G27" s="13">
         <v>0.97199999999999998</v>
@@ -8866,10 +8851,10 @@
         <v>1000</v>
       </c>
       <c r="L27" s="13" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="M27" s="37" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -8928,7 +8913,7 @@
         <v>43900</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>41</v>
@@ -8940,7 +8925,7 @@
         <v>20.7</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="G28" s="13">
         <v>0.97199999999999998</v>
@@ -8961,7 +8946,7 @@
         <v>47</v>
       </c>
       <c r="M28" s="37" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -9032,7 +9017,7 @@
         <v>20.7</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G29" s="13">
         <v>0.97199999999999998</v>
@@ -9046,10 +9031,10 @@
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
       <c r="L29" s="13" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="M29" s="37" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -9120,7 +9105,7 @@
         <v>20.7</v>
       </c>
       <c r="F30" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G30" s="21">
         <v>0.97199999999999998</v>
@@ -9134,7 +9119,7 @@
       <c r="J30" s="21"/>
       <c r="K30" s="21"/>
       <c r="L30" s="21" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="M30" s="53"/>
       <c r="N30" s="2"/>
@@ -11048,8 +11033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7293150B-6AD7-4206-AAE6-A798C9E6EC4A}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11131,7 +11116,7 @@
         <v>76</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>80</v>
+        <v>151</v>
       </c>
       <c r="G4" s="30" t="s">
         <v>67</v>
@@ -11175,7 +11160,7 @@
         <v>1000</v>
       </c>
       <c r="J5" s="37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -11187,7 +11172,7 @@
         <v>20.7</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E6" s="28">
         <v>0.97199999999999998</v>
@@ -11205,7 +11190,7 @@
         <v>1000</v>
       </c>
       <c r="J6" s="53" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -11237,7 +11222,7 @@
         <v>71</v>
       </c>
       <c r="J7" s="37" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -11267,7 +11252,7 @@
         <v>71</v>
       </c>
       <c r="J8" s="37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -11279,7 +11264,7 @@
         <v>20.7</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E9" s="28">
         <v>0.97199999999999998</v>
@@ -11297,7 +11282,7 @@
         <v>71</v>
       </c>
       <c r="J9" s="37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -11315,7 +11300,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="F10" s="52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G10" s="54">
         <v>100</v>
@@ -11327,7 +11312,7 @@
         <v>71</v>
       </c>
       <c r="J10" s="50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -11357,7 +11342,7 @@
         <v>400</v>
       </c>
       <c r="J11" s="62" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -11387,7 +11372,7 @@
         <v>1000</v>
       </c>
       <c r="J12" s="37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
@@ -11399,7 +11384,7 @@
         <v>20.7</v>
       </c>
       <c r="D13" s="57" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E13" s="57">
         <v>9.6</v>
@@ -11417,7 +11402,7 @@
         <v>400</v>
       </c>
       <c r="J13" s="62" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -11429,7 +11414,7 @@
         <v>20.7</v>
       </c>
       <c r="D14" s="55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E14" s="55">
         <v>9.6</v>
@@ -11447,7 +11432,7 @@
         <v>1000</v>
       </c>
       <c r="J14" s="37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -11459,7 +11444,7 @@
         <v>20.7</v>
       </c>
       <c r="D15" s="57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E15" s="57">
         <v>0.97199999999999998</v>
@@ -11477,7 +11462,7 @@
         <v>400</v>
       </c>
       <c r="J15" s="62" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
@@ -11489,13 +11474,13 @@
         <v>20.7</v>
       </c>
       <c r="D16" s="59" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E16" s="59">
         <v>0.97199999999999998</v>
       </c>
       <c r="F16" s="60" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G16" s="59">
         <v>100</v>
@@ -11507,7 +11492,7 @@
         <v>1000</v>
       </c>
       <c r="J16" s="53" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
@@ -11515,7 +11500,7 @@
     <row r="17" spans="1:14" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="31" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C17" s="29">
         <v>20.7</v>
@@ -11539,7 +11524,7 @@
         <v>400</v>
       </c>
       <c r="J17" s="37" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
@@ -11569,7 +11554,7 @@
         <v>1000</v>
       </c>
       <c r="J18" s="53" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
@@ -11624,7 +11609,7 @@
         <v>76</v>
       </c>
       <c r="F23" s="30" t="s">
-        <v>80</v>
+        <v>151</v>
       </c>
       <c r="G23" s="30" t="s">
         <v>67</v>
@@ -11665,7 +11650,7 @@
         <v>800</v>
       </c>
       <c r="J24" s="37" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -11674,7 +11659,7 @@
         <v>20.7</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E25" s="28">
         <v>0.97199999999999998</v>
@@ -11692,7 +11677,7 @@
         <v>800</v>
       </c>
       <c r="J25" s="53" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
@@ -11721,7 +11706,7 @@
         <v>71</v>
       </c>
       <c r="J26" s="37" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="18" x14ac:dyDescent="0.35">
@@ -11748,7 +11733,7 @@
         <v>71</v>
       </c>
       <c r="J27" s="37" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="18" x14ac:dyDescent="0.35">
@@ -11775,7 +11760,7 @@
         <v>71</v>
       </c>
       <c r="J28" s="37" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="18" x14ac:dyDescent="0.35">
@@ -11802,7 +11787,7 @@
         <v>71</v>
       </c>
       <c r="J29" s="37" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="18" x14ac:dyDescent="0.35">
@@ -11829,7 +11814,7 @@
         <v>71</v>
       </c>
       <c r="J30" s="37" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -11838,7 +11823,7 @@
         <v>20.7</v>
       </c>
       <c r="D31" s="54" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E31" s="54">
         <v>0.97199999999999998</v>
@@ -11856,7 +11841,7 @@
         <v>71</v>
       </c>
       <c r="J31" s="37" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="18" x14ac:dyDescent="0.35">
@@ -11883,7 +11868,7 @@
         <v>400</v>
       </c>
       <c r="J32" s="62" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -11917,7 +11902,7 @@
         <v>20.7</v>
       </c>
       <c r="D34" s="55" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E34" s="55">
         <v>0.97199999999999998</v>
@@ -11935,7 +11920,7 @@
         <v>400</v>
       </c>
       <c r="J34" s="37" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -11944,7 +11929,7 @@
         <v>20.7</v>
       </c>
       <c r="D35" s="55" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E35" s="55">
         <v>0.97199999999999998</v>
@@ -11965,7 +11950,7 @@
     </row>
     <row r="36" spans="2:10" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B36" s="31" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C36" s="29">
         <v>20.7</v>
@@ -11989,7 +11974,7 @@
         <v>400</v>
       </c>
       <c r="J36" s="37" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -12016,7 +12001,7 @@
         <v>1000</v>
       </c>
       <c r="J37" s="53" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Aggiunte delle quantità per il calcolo della sez d'urto di Rutherford
</commit_message>
<xml_diff>
--- a/Caratterizzazione_THGEM.xlsx
+++ b/Caratterizzazione_THGEM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peppe\Desktop\LaTex\Report_THGEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C6500B-6334-43DE-B308-8C71B6906462}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979DAC75-D11B-4B9F-A9BE-5388E97AF38D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{ACFC7C87-C28D-4487-B063-88156E979354}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{ACFC7C87-C28D-4487-B063-88156E979354}"/>
   </bookViews>
   <sheets>
     <sheet name="alpha-crono" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="160">
   <si>
     <t>DATA</t>
   </si>
@@ -1015,6 +1015,30 @@
   </si>
   <si>
     <t>&lt;Rate_PD&gt; (Hz)</t>
+  </si>
+  <si>
+    <t>Z_p</t>
+  </si>
+  <si>
+    <t>Z_t</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>epsilon0</t>
+  </si>
+  <si>
+    <t>a^2</t>
+  </si>
+  <si>
+    <t>E (MeV)</t>
+  </si>
+  <si>
+    <t>E (J)</t>
   </si>
 </sst>
 </file>
@@ -6459,8 +6483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E260431C-5552-43E0-806B-E171CCC2519A}">
   <dimension ref="A1:BL58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11031,10 +11055,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7293150B-6AD7-4206-AAE6-A798C9E6EC4A}">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11871,7 +11895,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B33" s="64"/>
       <c r="C33" s="65">
         <v>20.7</v>
@@ -11896,7 +11920,7 @@
       </c>
       <c r="J33" s="67"/>
     </row>
-    <row r="34" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B34" s="33"/>
       <c r="C34" s="55">
         <v>20.7</v>
@@ -11923,7 +11947,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="35" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="33"/>
       <c r="C35" s="55">
         <v>20.7</v>
@@ -11948,7 +11972,7 @@
       </c>
       <c r="J35" s="61"/>
     </row>
-    <row r="36" spans="2:10" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B36" s="31" t="s">
         <v>122</v>
       </c>
@@ -11977,7 +12001,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="37" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B37" s="32"/>
       <c r="C37" s="32">
         <v>20.7</v>
@@ -12004,7 +12028,64 @@
         <v>121</v>
       </c>
     </row>
-    <row r="38" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>158</v>
+      </c>
+      <c r="B42" t="s">
+        <v>159</v>
+      </c>
+      <c r="C42" t="s">
+        <v>152</v>
+      </c>
+      <c r="D42" t="s">
+        <v>153</v>
+      </c>
+      <c r="E42" t="s">
+        <v>154</v>
+      </c>
+      <c r="F42" t="s">
+        <v>156</v>
+      </c>
+      <c r="G42" t="s">
+        <v>155</v>
+      </c>
+      <c r="H42" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>145.69999999999999</v>
+      </c>
+      <c r="B43">
+        <f>A43*10^6*1.602*10^(-19)</f>
+        <v>2.3341139999999999E-11</v>
+      </c>
+      <c r="C43">
+        <v>8</v>
+      </c>
+      <c r="D43">
+        <v>79</v>
+      </c>
+      <c r="E43">
+        <f>1.602*10^(-19)</f>
+        <v>1.602E-19</v>
+      </c>
+      <c r="F43">
+        <f>8.85*10^(-12)</f>
+        <v>8.8499999999999988E-12</v>
+      </c>
+      <c r="G43">
+        <f>C43*D43*E43^2/(8*3.1415*F43*B43)</f>
+        <v>3.1242783296891599E-15</v>
+      </c>
+      <c r="H43">
+        <f>G43^2</f>
+        <v>9.7611150813652872E-30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Creato nel file Excel un foglio chiamato Calculations
</commit_message>
<xml_diff>
--- a/Caratterizzazione_THGEM.xlsx
+++ b/Caratterizzazione_THGEM.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peppe\Desktop\LaTex\Report_THGEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979DAC75-D11B-4B9F-A9BE-5388E97AF38D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7F8F99-514E-44DE-8AF5-87CF24CDB0AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{ACFC7C87-C28D-4487-B063-88156E979354}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{ACFC7C87-C28D-4487-B063-88156E979354}"/>
   </bookViews>
   <sheets>
     <sheet name="alpha-crono" sheetId="1" r:id="rId1"/>
     <sheet name="alpha" sheetId="2" r:id="rId2"/>
     <sheet name="test_2020-03-09-crono" sheetId="4" r:id="rId3"/>
     <sheet name="test_2020-03-09" sheetId="3" r:id="rId4"/>
+    <sheet name="Calculations" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -6483,8 +6485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E260431C-5552-43E0-806B-E171CCC2519A}">
   <dimension ref="A1:BL58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11055,10 +11057,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7293150B-6AD7-4206-AAE6-A798C9E6EC4A}">
-  <dimension ref="A1:N43"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11895,7 +11897,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B33" s="64"/>
       <c r="C33" s="65">
         <v>20.7</v>
@@ -11920,7 +11922,7 @@
       </c>
       <c r="J33" s="67"/>
     </row>
-    <row r="34" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B34" s="33"/>
       <c r="C34" s="55">
         <v>20.7</v>
@@ -11947,7 +11949,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="33"/>
       <c r="C35" s="55">
         <v>20.7</v>
@@ -11972,7 +11974,7 @@
       </c>
       <c r="J35" s="61"/>
     </row>
-    <row r="36" spans="1:10" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:10" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B36" s="31" t="s">
         <v>122</v>
       </c>
@@ -12001,7 +12003,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B37" s="32"/>
       <c r="C37" s="32">
         <v>20.7</v>
@@ -12028,66 +12030,81 @@
         <v>121</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>158</v>
-      </c>
-      <c r="B42" t="s">
-        <v>159</v>
-      </c>
-      <c r="C42" t="s">
-        <v>152</v>
-      </c>
-      <c r="D42" t="s">
-        <v>153</v>
-      </c>
-      <c r="E42" t="s">
-        <v>154</v>
-      </c>
-      <c r="F42" t="s">
-        <v>156</v>
-      </c>
-      <c r="G42" t="s">
-        <v>155</v>
-      </c>
-      <c r="H42" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>145.69999999999999</v>
-      </c>
-      <c r="B43">
-        <f>A43*10^6*1.602*10^(-19)</f>
-        <v>2.3341139999999999E-11</v>
-      </c>
-      <c r="C43">
-        <v>8</v>
-      </c>
-      <c r="D43">
-        <v>79</v>
-      </c>
-      <c r="E43">
-        <f>1.602*10^(-19)</f>
-        <v>1.602E-19</v>
-      </c>
-      <c r="F43">
-        <f>8.85*10^(-12)</f>
-        <v>8.8499999999999988E-12</v>
-      </c>
-      <c r="G43">
-        <f>C43*D43*E43^2/(8*3.1415*F43*B43)</f>
-        <v>3.1242783296891599E-15</v>
-      </c>
-      <c r="H43">
-        <f>G43^2</f>
-        <v>9.7611150813652872E-30</v>
-      </c>
-    </row>
+    <row r="38" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B66FBB42-8B7D-4E2F-B67D-D60F4EF2D11F}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>145.69999999999999</v>
+      </c>
+      <c r="B2">
+        <f>A2*10^6*1.602*10^(-19)</f>
+        <v>2.3341139999999999E-11</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>79</v>
+      </c>
+      <c r="E2">
+        <f>1.602*10^(-19)</f>
+        <v>1.602E-19</v>
+      </c>
+      <c r="F2">
+        <f>8.85*10^(-12)</f>
+        <v>8.8499999999999988E-12</v>
+      </c>
+      <c r="G2">
+        <f>C2*D2*E2^2/(8*3.1415*F2*B2)</f>
+        <v>3.1242783296891599E-15</v>
+      </c>
+      <c r="H2">
+        <f>G2^2</f>
+        <v>9.7611150813652872E-30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Aggiunte al file excel due colonne: MXFC1 e rate sul tracker
</commit_message>
<xml_diff>
--- a/Caratterizzazione_THGEM.xlsx
+++ b/Caratterizzazione_THGEM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peppe\Desktop\LaTex\Report_THGEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7F8F99-514E-44DE-8AF5-87CF24CDB0AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E285CC-D4F1-48CB-AAE6-895F7FF077A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{ACFC7C87-C28D-4487-B063-88156E979354}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{ACFC7C87-C28D-4487-B063-88156E979354}"/>
   </bookViews>
   <sheets>
     <sheet name="alpha-crono" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="164">
   <si>
     <t>DATA</t>
   </si>
@@ -1041,6 +1041,18 @@
   </si>
   <si>
     <t>E (J)</t>
+  </si>
+  <si>
+    <t>MXFC1 (pA)</t>
+  </si>
+  <si>
+    <t>&lt;Rate_PD&gt; (pps)</t>
+  </si>
+  <si>
+    <t>Rate (pps)</t>
+  </si>
+  <si>
+    <t>Rate_tracker (pps)</t>
   </si>
 </sst>
 </file>
@@ -5833,7 +5845,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="K17" sqref="K17:M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6483,10 +6495,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E260431C-5552-43E0-806B-E171CCC2519A}">
-  <dimension ref="A1:BL58"/>
+  <dimension ref="A1:BN58"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6495,20 +6507,20 @@
     <col min="2" max="2" width="16.44140625" style="6" customWidth="1"/>
     <col min="3" max="3" width="12.21875" customWidth="1"/>
     <col min="4" max="4" width="10.21875" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" customWidth="1"/>
-    <col min="7" max="7" width="18.5546875" customWidth="1"/>
-    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.21875" customWidth="1"/>
-    <col min="10" max="10" width="11.88671875" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" customWidth="1"/>
-    <col min="12" max="12" width="39.21875" customWidth="1"/>
-    <col min="13" max="13" width="91" customWidth="1"/>
-    <col min="14" max="14" width="19.88671875" customWidth="1"/>
-    <col min="15" max="15" width="13.33203125" customWidth="1"/>
+    <col min="5" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" customWidth="1"/>
+    <col min="8" max="9" width="18.5546875" customWidth="1"/>
+    <col min="10" max="10" width="19.77734375" customWidth="1"/>
+    <col min="11" max="11" width="21.21875" customWidth="1"/>
+    <col min="12" max="12" width="11.88671875" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" customWidth="1"/>
+    <col min="14" max="14" width="39.21875" customWidth="1"/>
+    <col min="15" max="15" width="91" customWidth="1"/>
+    <col min="16" max="16" width="19.88671875" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:66" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -6525,31 +6537,35 @@
         <v>4</v>
       </c>
       <c r="F1" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="9" t="s">
-        <v>151</v>
-      </c>
       <c r="I1" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="O1" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -6560,8 +6576,8 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
@@ -6599,8 +6615,10 @@
       <c r="BJ1" s="1"/>
       <c r="BK1" s="1"/>
       <c r="BL1" s="1"/>
-    </row>
-    <row r="2" spans="1:64" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="BM1" s="1"/>
+      <c r="BN1" s="1"/>
+    </row>
+    <row r="2" spans="1:66" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10">
         <v>43899</v>
       </c>
@@ -6617,27 +6635,28 @@
         <v>20.7</v>
       </c>
       <c r="F2" s="13">
+        <v>870</v>
+      </c>
+      <c r="G2" s="13">
         <v>400</v>
       </c>
-      <c r="G2" s="13">
+      <c r="H2" s="13">
         <v>9.6</v>
       </c>
-      <c r="H2" s="13">
+      <c r="J2" s="13">
         <v>13.5</v>
       </c>
-      <c r="I2" s="46" t="s">
+      <c r="K2" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="M2" s="37" t="s">
+      <c r="O2" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -6648,8 +6667,8 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
@@ -6687,8 +6706,10 @@
       <c r="BJ2" s="1"/>
       <c r="BK2" s="1"/>
       <c r="BL2" s="1"/>
-    </row>
-    <row r="3" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM2" s="1"/>
+      <c r="BN2" s="1"/>
+    </row>
+    <row r="3" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="14">
         <v>43899</v>
       </c>
@@ -6705,31 +6726,32 @@
         <v>20.7</v>
       </c>
       <c r="F3" s="13">
+        <v>900</v>
+      </c>
+      <c r="G3" s="13">
         <v>400</v>
       </c>
-      <c r="G3" s="13">
+      <c r="H3" s="13">
         <v>9.6</v>
       </c>
-      <c r="H3" s="13">
+      <c r="J3" s="13">
         <v>13.4</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="K3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="13">
+      <c r="L3" s="13">
         <v>160</v>
       </c>
-      <c r="K3" s="13">
+      <c r="M3" s="13">
         <v>220</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="N3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="37" t="s">
+      <c r="O3" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
@@ -6740,8 +6762,8 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
@@ -6779,8 +6801,10 @@
       <c r="BJ3" s="1"/>
       <c r="BK3" s="1"/>
       <c r="BL3" s="1"/>
-    </row>
-    <row r="4" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM3" s="1"/>
+      <c r="BN3" s="1"/>
+    </row>
+    <row r="4" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="14">
         <v>43899</v>
       </c>
@@ -6797,31 +6821,33 @@
         <v>20.7</v>
       </c>
       <c r="F4" s="13">
+        <v>900</v>
+      </c>
+      <c r="G4" s="13">
         <v>400</v>
       </c>
-      <c r="G4" s="13">
+      <c r="H4" s="13">
         <v>9.6</v>
       </c>
-      <c r="H4" s="13">
+      <c r="I4" s="13"/>
+      <c r="J4" s="13">
         <v>13.2</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="K4" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="13">
+      <c r="L4" s="13">
         <v>200</v>
       </c>
-      <c r="K4" s="13">
+      <c r="M4" s="13">
         <v>1100</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="N4" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="37" t="s">
+      <c r="O4" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
@@ -6832,8 +6858,8 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
@@ -6871,8 +6897,10 @@
       <c r="BJ4" s="1"/>
       <c r="BK4" s="1"/>
       <c r="BL4" s="1"/>
-    </row>
-    <row r="5" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM4" s="1"/>
+      <c r="BN4" s="1"/>
+    </row>
+    <row r="5" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="14">
         <v>43899</v>
       </c>
@@ -6889,27 +6917,29 @@
         <v>20.7</v>
       </c>
       <c r="F5" s="13">
+        <v>680</v>
+      </c>
+      <c r="G5" s="13">
         <v>280</v>
       </c>
-      <c r="G5" s="13">
+      <c r="H5" s="13">
         <v>9.6</v>
       </c>
-      <c r="H5" s="13">
+      <c r="I5" s="13"/>
+      <c r="J5" s="13">
         <v>8.6</v>
       </c>
-      <c r="I5" s="46" t="s">
+      <c r="K5" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13" t="s">
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="M5" s="37" t="s">
+      <c r="O5" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
@@ -6920,8 +6950,8 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
@@ -6959,8 +6989,10 @@
       <c r="BJ5" s="1"/>
       <c r="BK5" s="1"/>
       <c r="BL5" s="1"/>
-    </row>
-    <row r="6" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM5" s="1"/>
+      <c r="BN5" s="1"/>
+    </row>
+    <row r="6" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="14">
         <v>43899</v>
       </c>
@@ -6977,25 +7009,27 @@
         <v>20.7</v>
       </c>
       <c r="F6" s="13">
+        <v>680</v>
+      </c>
+      <c r="G6" s="13">
         <v>280</v>
       </c>
-      <c r="G6" s="13">
+      <c r="H6" s="13">
         <v>9.6</v>
       </c>
-      <c r="H6" s="47">
+      <c r="I6" s="13"/>
+      <c r="J6" s="47">
         <v>9</v>
       </c>
-      <c r="I6" s="46" t="s">
+      <c r="K6" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13" t="s">
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="M6" s="37"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
+      <c r="O6" s="37"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
@@ -7006,8 +7040,8 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
@@ -7045,8 +7079,10 @@
       <c r="BJ6" s="1"/>
       <c r="BK6" s="1"/>
       <c r="BL6" s="1"/>
-    </row>
-    <row r="7" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM6" s="1"/>
+      <c r="BN6" s="1"/>
+    </row>
+    <row r="7" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="14">
         <v>43899</v>
       </c>
@@ -7063,31 +7099,33 @@
         <v>20.7</v>
       </c>
       <c r="F7" s="13">
+        <v>220</v>
+      </c>
+      <c r="G7" s="13">
         <v>100</v>
       </c>
-      <c r="G7" s="13">
+      <c r="H7" s="13">
         <v>9.6</v>
       </c>
-      <c r="H7" s="13">
+      <c r="I7" s="13"/>
+      <c r="J7" s="13">
         <v>2.5</v>
       </c>
-      <c r="I7" s="23" t="s">
+      <c r="K7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="13">
+      <c r="L7" s="13">
         <v>200</v>
       </c>
-      <c r="K7" s="13">
+      <c r="M7" s="13">
         <v>1200</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="N7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="M7" s="37" t="s">
+      <c r="O7" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
@@ -7098,8 +7136,8 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
-      <c r="Z7" s="1"/>
-      <c r="AA7" s="1"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
@@ -7137,8 +7175,10 @@
       <c r="BJ7" s="1"/>
       <c r="BK7" s="1"/>
       <c r="BL7" s="1"/>
-    </row>
-    <row r="8" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM7" s="1"/>
+      <c r="BN7" s="1"/>
+    </row>
+    <row r="8" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="14">
         <v>43899</v>
       </c>
@@ -7154,28 +7194,30 @@
       <c r="E8" s="13">
         <v>20.7</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="13">
+        <v>100</v>
+      </c>
+      <c r="G8" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="G8" s="13">
+      <c r="H8" s="13">
         <v>9.6</v>
       </c>
-      <c r="H8" s="13">
+      <c r="I8" s="13"/>
+      <c r="J8" s="13">
         <v>1.6</v>
       </c>
-      <c r="I8" s="46" t="s">
+      <c r="K8" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13" t="s">
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="M8" s="37" t="s">
+      <c r="O8" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
@@ -7186,8 +7228,8 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
-      <c r="Z8" s="1"/>
-      <c r="AA8" s="1"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
@@ -7225,8 +7267,10 @@
       <c r="BJ8" s="1"/>
       <c r="BK8" s="1"/>
       <c r="BL8" s="1"/>
-    </row>
-    <row r="9" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM8" s="1"/>
+      <c r="BN8" s="1"/>
+    </row>
+    <row r="9" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="14">
         <v>43899</v>
       </c>
@@ -7242,28 +7286,30 @@
       <c r="E9" s="13">
         <v>20.7</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="13">
+        <v>100</v>
+      </c>
+      <c r="G9" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="G9" s="13">
+      <c r="H9" s="13">
         <v>9.6</v>
       </c>
-      <c r="H9" s="13">
+      <c r="I9" s="13"/>
+      <c r="J9" s="13">
         <v>1.6</v>
       </c>
-      <c r="I9" s="46" t="s">
+      <c r="K9" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13" t="s">
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="M9" s="37" t="s">
+      <c r="O9" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
@@ -7274,8 +7320,8 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
@@ -7313,8 +7359,10 @@
       <c r="BJ9" s="1"/>
       <c r="BK9" s="1"/>
       <c r="BL9" s="1"/>
-    </row>
-    <row r="10" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM9" s="1"/>
+      <c r="BN9" s="1"/>
+    </row>
+    <row r="10" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="14">
         <v>43899</v>
       </c>
@@ -7330,28 +7378,30 @@
       <c r="E10" s="13">
         <v>20.7</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="13">
+        <v>100</v>
+      </c>
+      <c r="G10" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="G10" s="13">
+      <c r="H10" s="13">
         <v>0.97199999999999998</v>
       </c>
-      <c r="H10" s="13">
+      <c r="I10" s="13"/>
+      <c r="J10" s="13">
         <v>0.2</v>
       </c>
-      <c r="I10" s="46" t="s">
+      <c r="K10" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13" t="s">
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="M10" s="37" t="s">
+      <c r="O10" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
@@ -7362,8 +7412,8 @@
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
@@ -7401,8 +7451,10 @@
       <c r="BJ10" s="1"/>
       <c r="BK10" s="1"/>
       <c r="BL10" s="1"/>
-    </row>
-    <row r="11" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM10" s="1"/>
+      <c r="BN10" s="1"/>
+    </row>
+    <row r="11" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="14">
         <v>43899</v>
       </c>
@@ -7418,28 +7470,30 @@
       <c r="E11" s="13">
         <v>20.7</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="13">
+        <v>100</v>
+      </c>
+      <c r="G11" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="G11" s="13">
+      <c r="H11" s="13">
         <v>0.97199999999999998</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="I11" s="13"/>
+      <c r="J11" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="I11" s="46" t="s">
+      <c r="K11" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13" t="s">
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="M11" s="37" t="s">
+      <c r="O11" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
@@ -7450,8 +7504,8 @@
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
@@ -7489,8 +7543,10 @@
       <c r="BJ11" s="1"/>
       <c r="BK11" s="1"/>
       <c r="BL11" s="1"/>
-    </row>
-    <row r="12" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM11" s="1"/>
+      <c r="BN11" s="1"/>
+    </row>
+    <row r="12" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="14">
         <v>43899</v>
       </c>
@@ -7506,32 +7562,34 @@
       <c r="E12" s="13">
         <v>20.7</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="13">
+        <v>250</v>
+      </c>
+      <c r="G12" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="G12" s="13">
+      <c r="H12" s="13">
         <v>0.97199999999999998</v>
       </c>
-      <c r="H12" s="13">
+      <c r="I12" s="13"/>
+      <c r="J12" s="13">
         <v>0.3</v>
       </c>
-      <c r="I12" s="23" t="s">
+      <c r="K12" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="13">
+      <c r="L12" s="13">
         <v>200</v>
       </c>
-      <c r="K12" s="13">
+      <c r="M12" s="13">
         <v>1200</v>
       </c>
-      <c r="L12" s="13" t="s">
+      <c r="N12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="M12" s="37" t="s">
+      <c r="O12" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
@@ -7542,8 +7600,8 @@
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
@@ -7581,8 +7639,10 @@
       <c r="BJ12" s="1"/>
       <c r="BK12" s="1"/>
       <c r="BL12" s="1"/>
-    </row>
-    <row r="13" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM12" s="1"/>
+      <c r="BN12" s="1"/>
+    </row>
+    <row r="13" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="14">
         <v>43899</v>
       </c>
@@ -7598,32 +7658,34 @@
       <c r="E13" s="13">
         <v>20.7</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="13">
+        <v>250</v>
+      </c>
+      <c r="G13" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="G13" s="13">
+      <c r="H13" s="13">
         <v>0.97199999999999998</v>
       </c>
-      <c r="H13" s="13">
+      <c r="I13" s="13"/>
+      <c r="J13" s="13">
         <v>0.3</v>
       </c>
-      <c r="I13" s="22" t="s">
+      <c r="K13" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="J13" s="13">
+      <c r="L13" s="13">
         <v>170</v>
       </c>
-      <c r="K13" s="13">
+      <c r="M13" s="13">
         <v>210</v>
       </c>
-      <c r="L13" s="13" t="s">
+      <c r="N13" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="M13" s="37" t="s">
+      <c r="O13" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
@@ -7634,8 +7696,8 @@
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
-      <c r="Z13" s="1"/>
-      <c r="AA13" s="1"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
       <c r="AB13" s="1"/>
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
@@ -7673,8 +7735,10 @@
       <c r="BJ13" s="1"/>
       <c r="BK13" s="1"/>
       <c r="BL13" s="1"/>
-    </row>
-    <row r="14" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM13" s="1"/>
+      <c r="BN13" s="1"/>
+    </row>
+    <row r="14" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="14">
         <v>43899</v>
       </c>
@@ -7690,28 +7754,30 @@
       <c r="E14" s="13">
         <v>20.7</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="13">
+        <v>680</v>
+      </c>
+      <c r="G14" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="G14" s="13">
+      <c r="H14" s="13">
         <v>0.97199999999999998</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="I14" s="13"/>
+      <c r="J14" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="I14" s="46" t="s">
+      <c r="K14" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13" t="s">
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="M14" s="37" t="s">
+      <c r="O14" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
@@ -7722,8 +7788,8 @@
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
-      <c r="Z14" s="1"/>
-      <c r="AA14" s="1"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
       <c r="AB14" s="1"/>
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
@@ -7761,8 +7827,10 @@
       <c r="BJ14" s="1"/>
       <c r="BK14" s="1"/>
       <c r="BL14" s="1"/>
-    </row>
-    <row r="15" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM14" s="1"/>
+      <c r="BN14" s="1"/>
+    </row>
+    <row r="15" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="14">
         <v>43899</v>
       </c>
@@ -7778,8 +7846,8 @@
       <c r="E15" s="13">
         <v>20.7</v>
       </c>
-      <c r="F15" s="13" t="s">
-        <v>77</v>
+      <c r="F15" s="13">
+        <v>100</v>
       </c>
       <c r="G15" s="13" t="s">
         <v>77</v>
@@ -7787,17 +7855,19 @@
       <c r="H15" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="I15" s="46" t="s">
+      <c r="I15" s="13"/>
+      <c r="J15" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
+      <c r="K15" s="46" t="s">
+        <v>77</v>
+      </c>
       <c r="L15" s="13"/>
-      <c r="M15" s="48" t="s">
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
@@ -7808,8 +7878,8 @@
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
       <c r="AB15" s="1"/>
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
@@ -7847,8 +7917,10 @@
       <c r="BJ15" s="1"/>
       <c r="BK15" s="1"/>
       <c r="BL15" s="1"/>
-    </row>
-    <row r="16" spans="1:64" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="BM15" s="1"/>
+      <c r="BN15" s="1"/>
+    </row>
+    <row r="16" spans="1:66" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="49">
         <v>43899</v>
       </c>
@@ -7865,31 +7937,33 @@
         <v>20.7</v>
       </c>
       <c r="F16" s="13">
+        <v>680</v>
+      </c>
+      <c r="G16" s="13">
         <v>300</v>
       </c>
-      <c r="G16" s="13">
+      <c r="H16" s="13">
         <v>0.97199999999999998</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="I16" s="13"/>
+      <c r="J16" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="I16" s="51" t="s">
+      <c r="K16" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="J16" s="13">
+      <c r="L16" s="13">
         <v>200</v>
       </c>
-      <c r="K16" s="13">
+      <c r="M16" s="13">
         <v>1000</v>
       </c>
-      <c r="L16" s="52" t="s">
+      <c r="N16" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="M16" s="50" t="s">
+      <c r="O16" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
@@ -7900,8 +7974,8 @@
       <c r="W16" s="2"/>
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
@@ -7939,8 +8013,10 @@
       <c r="BJ16" s="1"/>
       <c r="BK16" s="1"/>
       <c r="BL16" s="1"/>
-    </row>
-    <row r="17" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM16" s="1"/>
+      <c r="BN16" s="1"/>
+    </row>
+    <row r="17" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="14">
         <v>43900</v>
       </c>
@@ -7957,27 +8033,31 @@
         <v>20.7</v>
       </c>
       <c r="F17" s="26">
+        <v>670</v>
+      </c>
+      <c r="G17" s="26">
         <v>280</v>
       </c>
-      <c r="G17" s="26">
+      <c r="H17" s="26">
         <v>9.6</v>
       </c>
-      <c r="H17" s="26" t="s">
+      <c r="I17" s="26">
+        <v>2400</v>
+      </c>
+      <c r="J17" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="I17" s="46" t="s">
+      <c r="K17" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="13" t="s">
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="M17" s="37" t="s">
+      <c r="O17" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
@@ -7988,8 +8068,8 @@
       <c r="W17" s="2"/>
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
-      <c r="Z17" s="1"/>
-      <c r="AA17" s="1"/>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
@@ -8027,8 +8107,10 @@
       <c r="BJ17" s="1"/>
       <c r="BK17" s="1"/>
       <c r="BL17" s="1"/>
-    </row>
-    <row r="18" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM17" s="1"/>
+      <c r="BN17" s="1"/>
+    </row>
+    <row r="18" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="14">
         <v>43900</v>
       </c>
@@ -8045,27 +8127,31 @@
         <v>20.7</v>
       </c>
       <c r="F18" s="13">
+        <v>670</v>
+      </c>
+      <c r="G18" s="13">
         <v>280</v>
       </c>
-      <c r="G18" s="13">
+      <c r="H18" s="13">
         <v>9.6</v>
       </c>
-      <c r="H18" s="13" t="s">
+      <c r="I18" s="13">
+        <v>2400</v>
+      </c>
+      <c r="J18" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="I18" s="13" t="s">
+      <c r="K18" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13" t="s">
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="M18" s="63" t="s">
+      <c r="O18" s="63" t="s">
         <v>126</v>
       </c>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
@@ -8076,8 +8162,8 @@
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
-      <c r="Z18" s="1"/>
-      <c r="AA18" s="1"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
@@ -8115,8 +8201,10 @@
       <c r="BJ18" s="1"/>
       <c r="BK18" s="1"/>
       <c r="BL18" s="1"/>
-    </row>
-    <row r="19" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM18" s="1"/>
+      <c r="BN18" s="1"/>
+    </row>
+    <row r="19" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="14">
         <v>43900</v>
       </c>
@@ -8133,31 +8221,35 @@
         <v>20.7</v>
       </c>
       <c r="F19" s="13">
+        <v>900</v>
+      </c>
+      <c r="G19" s="13">
         <v>400</v>
       </c>
-      <c r="G19" s="13">
+      <c r="H19" s="13">
         <v>9.6</v>
       </c>
-      <c r="H19" s="13">
+      <c r="I19" s="13">
+        <v>3400</v>
+      </c>
+      <c r="J19" s="13">
         <v>14.9</v>
       </c>
-      <c r="I19" s="22" t="s">
+      <c r="K19" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="J19" s="13">
+      <c r="L19" s="13">
         <v>170</v>
       </c>
-      <c r="K19" s="13">
+      <c r="M19" s="13">
         <v>200</v>
       </c>
-      <c r="L19" s="13" t="s">
+      <c r="N19" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="M19" s="37" t="s">
+      <c r="O19" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
@@ -8168,8 +8260,8 @@
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
-      <c r="Z19" s="1"/>
-      <c r="AA19" s="1"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
       <c r="AB19" s="1"/>
       <c r="AC19" s="1"/>
       <c r="AD19" s="1"/>
@@ -8207,8 +8299,10 @@
       <c r="BJ19" s="1"/>
       <c r="BK19" s="1"/>
       <c r="BL19" s="1"/>
-    </row>
-    <row r="20" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM19" s="1"/>
+      <c r="BN19" s="1"/>
+    </row>
+    <row r="20" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="14">
         <v>43900</v>
       </c>
@@ -8225,31 +8319,35 @@
         <v>20.7</v>
       </c>
       <c r="F20" s="13">
+        <v>900</v>
+      </c>
+      <c r="G20" s="13">
         <v>400</v>
       </c>
-      <c r="G20" s="13">
+      <c r="H20" s="13">
         <v>9.6</v>
       </c>
-      <c r="H20" s="13">
+      <c r="I20" s="13">
+        <v>3400</v>
+      </c>
+      <c r="J20" s="13">
         <v>14.8</v>
       </c>
-      <c r="I20" s="23" t="s">
+      <c r="K20" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="J20" s="13">
+      <c r="L20" s="13">
         <v>30</v>
       </c>
-      <c r="K20" s="13">
+      <c r="M20" s="13">
         <v>600</v>
       </c>
-      <c r="L20" s="13" t="s">
+      <c r="N20" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="M20" s="37" t="s">
+      <c r="O20" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
@@ -8260,8 +8358,8 @@
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
-      <c r="Z20" s="1"/>
-      <c r="AA20" s="1"/>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2"/>
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
@@ -8299,8 +8397,10 @@
       <c r="BJ20" s="1"/>
       <c r="BK20" s="1"/>
       <c r="BL20" s="1"/>
-    </row>
-    <row r="21" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM20" s="1"/>
+      <c r="BN20" s="1"/>
+    </row>
+    <row r="21" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="14">
         <v>43900</v>
       </c>
@@ -8317,31 +8417,35 @@
         <v>20.7</v>
       </c>
       <c r="F21" s="13">
+        <v>900</v>
+      </c>
+      <c r="G21" s="13">
         <v>400</v>
       </c>
-      <c r="G21" s="13">
+      <c r="H21" s="13">
         <v>9.6</v>
       </c>
-      <c r="H21" s="13">
+      <c r="I21" s="13">
+        <v>3400</v>
+      </c>
+      <c r="J21" s="13">
         <v>14.9</v>
       </c>
-      <c r="I21" s="23" t="s">
+      <c r="K21" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="J21" s="13">
+      <c r="L21" s="13">
         <v>30</v>
       </c>
-      <c r="K21" s="13">
+      <c r="M21" s="13">
         <v>1000</v>
       </c>
-      <c r="L21" s="13" t="s">
+      <c r="N21" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="M21" s="37" t="s">
+      <c r="O21" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
@@ -8352,8 +8456,8 @@
       <c r="W21" s="2"/>
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
-      <c r="Z21" s="1"/>
-      <c r="AA21" s="1"/>
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="2"/>
       <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
       <c r="AD21" s="1"/>
@@ -8391,8 +8495,10 @@
       <c r="BJ21" s="1"/>
       <c r="BK21" s="1"/>
       <c r="BL21" s="1"/>
-    </row>
-    <row r="22" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM21" s="1"/>
+      <c r="BN21" s="1"/>
+    </row>
+    <row r="22" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="14">
         <v>43900</v>
       </c>
@@ -8409,27 +8515,31 @@
         <v>20.7</v>
       </c>
       <c r="F22" s="13">
+        <v>680</v>
+      </c>
+      <c r="G22" s="13">
         <v>280</v>
       </c>
-      <c r="G22" s="13">
+      <c r="H22" s="13">
         <v>9.6</v>
       </c>
-      <c r="H22" s="13">
+      <c r="I22" s="13">
+        <v>2400</v>
+      </c>
+      <c r="J22" s="13">
         <v>8.9</v>
       </c>
-      <c r="I22" s="46" t="s">
+      <c r="K22" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13" t="s">
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="M22" s="37" t="s">
+      <c r="O22" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
@@ -8440,8 +8550,8 @@
       <c r="W22" s="2"/>
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
-      <c r="Z22" s="1"/>
-      <c r="AA22" s="1"/>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2"/>
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
@@ -8479,8 +8589,10 @@
       <c r="BJ22" s="1"/>
       <c r="BK22" s="1"/>
       <c r="BL22" s="1"/>
-    </row>
-    <row r="23" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM22" s="1"/>
+      <c r="BN22" s="1"/>
+    </row>
+    <row r="23" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A23" s="14">
         <v>43900</v>
       </c>
@@ -8497,25 +8609,29 @@
         <v>20.7</v>
       </c>
       <c r="F23" s="13">
+        <v>680</v>
+      </c>
+      <c r="G23" s="13">
         <v>280</v>
       </c>
-      <c r="G23" s="13">
+      <c r="H23" s="13">
         <v>9.6</v>
       </c>
-      <c r="H23" s="13">
+      <c r="I23" s="13">
+        <v>2400</v>
+      </c>
+      <c r="J23" s="13">
         <v>9.5</v>
       </c>
-      <c r="I23" s="46" t="s">
+      <c r="K23" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13" t="s">
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="M23" s="37"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
+      <c r="O23" s="37"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
@@ -8526,8 +8642,8 @@
       <c r="W23" s="2"/>
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
-      <c r="Z23" s="1"/>
-      <c r="AA23" s="1"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
       <c r="AB23" s="1"/>
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
@@ -8565,8 +8681,10 @@
       <c r="BJ23" s="1"/>
       <c r="BK23" s="1"/>
       <c r="BL23" s="1"/>
-    </row>
-    <row r="24" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM23" s="1"/>
+      <c r="BN23" s="1"/>
+    </row>
+    <row r="24" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" s="14">
         <v>43900</v>
       </c>
@@ -8583,31 +8701,35 @@
         <v>20.7</v>
       </c>
       <c r="F24" s="13">
+        <v>250</v>
+      </c>
+      <c r="G24" s="13">
         <v>150</v>
       </c>
-      <c r="G24" s="13">
+      <c r="H24" s="13">
         <v>9.6</v>
       </c>
-      <c r="H24" s="13">
+      <c r="I24" s="13">
+        <v>1300</v>
+      </c>
+      <c r="J24" s="13">
         <v>3.4</v>
       </c>
-      <c r="I24" s="23" t="s">
+      <c r="K24" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="J24" s="13">
+      <c r="L24" s="13">
         <v>100</v>
       </c>
-      <c r="K24" s="13">
+      <c r="M24" s="13">
         <v>1000</v>
       </c>
-      <c r="L24" s="13" t="s">
+      <c r="N24" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="M24" s="37" t="s">
+      <c r="O24" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
@@ -8618,8 +8740,8 @@
       <c r="W24" s="2"/>
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
-      <c r="Z24" s="1"/>
-      <c r="AA24" s="1"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
       <c r="AB24" s="1"/>
       <c r="AC24" s="1"/>
       <c r="AD24" s="1"/>
@@ -8657,8 +8779,10 @@
       <c r="BJ24" s="1"/>
       <c r="BK24" s="1"/>
       <c r="BL24" s="1"/>
-    </row>
-    <row r="25" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM24" s="1"/>
+      <c r="BN24" s="1"/>
+    </row>
+    <row r="25" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" s="14">
         <v>43900</v>
       </c>
@@ -8675,31 +8799,35 @@
         <v>20.7</v>
       </c>
       <c r="F25" s="13">
+        <v>110</v>
+      </c>
+      <c r="G25" s="13">
         <v>60</v>
       </c>
-      <c r="G25" s="13">
+      <c r="H25" s="13">
         <v>9.6</v>
       </c>
-      <c r="H25" s="13">
+      <c r="I25" s="13">
+        <v>510</v>
+      </c>
+      <c r="J25" s="13">
         <v>1.5</v>
       </c>
-      <c r="I25" s="23" t="s">
+      <c r="K25" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="J25" s="13">
+      <c r="L25" s="13">
         <v>400</v>
       </c>
-      <c r="K25" s="13">
+      <c r="M25" s="13">
         <v>1000</v>
       </c>
-      <c r="L25" s="13" t="s">
+      <c r="N25" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="M25" s="37" t="s">
+      <c r="O25" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
@@ -8710,8 +8838,8 @@
       <c r="W25" s="2"/>
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
-      <c r="Z25" s="1"/>
-      <c r="AA25" s="1"/>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="2"/>
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
@@ -8749,8 +8877,10 @@
       <c r="BJ25" s="1"/>
       <c r="BK25" s="1"/>
       <c r="BL25" s="1"/>
-    </row>
-    <row r="26" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM25" s="1"/>
+      <c r="BN25" s="1"/>
+    </row>
+    <row r="26" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="14">
         <v>43900</v>
       </c>
@@ -8767,31 +8897,35 @@
         <v>20.7</v>
       </c>
       <c r="F26" s="13">
+        <v>680</v>
+      </c>
+      <c r="G26" s="13">
         <v>280</v>
       </c>
-      <c r="G26" s="13">
+      <c r="H26" s="13">
         <v>0.97199999999999998</v>
       </c>
-      <c r="H26" s="13">
+      <c r="I26" s="13">
+        <v>220</v>
+      </c>
+      <c r="J26" s="13">
         <v>0.9</v>
       </c>
-      <c r="I26" s="23" t="s">
+      <c r="K26" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="J26" s="13">
+      <c r="L26" s="13">
         <v>100</v>
       </c>
-      <c r="K26" s="13">
+      <c r="M26" s="13">
         <v>1000</v>
       </c>
-      <c r="L26" s="13" t="s">
+      <c r="N26" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="M26" s="37" t="s">
+      <c r="O26" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
@@ -8802,8 +8936,8 @@
       <c r="W26" s="2"/>
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
-      <c r="Z26" s="1"/>
-      <c r="AA26" s="1"/>
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="2"/>
       <c r="AB26" s="1"/>
       <c r="AC26" s="1"/>
       <c r="AD26" s="1"/>
@@ -8841,8 +8975,10 @@
       <c r="BJ26" s="1"/>
       <c r="BK26" s="1"/>
       <c r="BL26" s="1"/>
-    </row>
-    <row r="27" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM26" s="1"/>
+      <c r="BN26" s="1"/>
+    </row>
+    <row r="27" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="14">
         <v>43900</v>
       </c>
@@ -8858,32 +8994,36 @@
       <c r="E27" s="13">
         <v>20.7</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="F27" s="13">
+        <v>250</v>
+      </c>
+      <c r="G27" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="G27" s="13">
+      <c r="H27" s="13">
         <v>0.97199999999999998</v>
       </c>
-      <c r="H27" s="13">
+      <c r="I27" s="13">
+        <v>130</v>
+      </c>
+      <c r="J27" s="13">
         <v>0.4</v>
       </c>
-      <c r="I27" s="23" t="s">
+      <c r="K27" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="J27" s="13">
+      <c r="L27" s="13">
         <v>30</v>
       </c>
-      <c r="K27" s="13">
+      <c r="M27" s="13">
         <v>1000</v>
       </c>
-      <c r="L27" s="13" t="s">
+      <c r="N27" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="M27" s="37" t="s">
+      <c r="O27" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
@@ -8894,8 +9034,8 @@
       <c r="W27" s="2"/>
       <c r="X27" s="2"/>
       <c r="Y27" s="2"/>
-      <c r="Z27" s="1"/>
-      <c r="AA27" s="1"/>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="2"/>
       <c r="AB27" s="1"/>
       <c r="AC27" s="1"/>
       <c r="AD27" s="1"/>
@@ -8933,8 +9073,10 @@
       <c r="BJ27" s="1"/>
       <c r="BK27" s="1"/>
       <c r="BL27" s="1"/>
-    </row>
-    <row r="28" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM27" s="1"/>
+      <c r="BN27" s="1"/>
+    </row>
+    <row r="28" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="14">
         <v>43900</v>
       </c>
@@ -8950,32 +9092,36 @@
       <c r="E28" s="13">
         <v>20.7</v>
       </c>
-      <c r="F28" s="13" t="s">
+      <c r="F28" s="13">
+        <v>250</v>
+      </c>
+      <c r="G28" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="G28" s="13">
+      <c r="H28" s="13">
         <v>0.97199999999999998</v>
       </c>
-      <c r="H28" s="13">
+      <c r="I28" s="13">
+        <v>130</v>
+      </c>
+      <c r="J28" s="13">
         <v>0.3</v>
       </c>
-      <c r="I28" s="22" t="s">
+      <c r="K28" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="J28" s="13">
+      <c r="L28" s="13">
         <v>170</v>
       </c>
-      <c r="K28" s="13">
+      <c r="M28" s="13">
         <v>205</v>
       </c>
-      <c r="L28" s="13" t="s">
+      <c r="N28" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="M28" s="37" t="s">
+      <c r="O28" s="37" t="s">
         <v>145</v>
       </c>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
@@ -8986,8 +9132,8 @@
       <c r="W28" s="2"/>
       <c r="X28" s="2"/>
       <c r="Y28" s="2"/>
-      <c r="Z28" s="1"/>
-      <c r="AA28" s="1"/>
+      <c r="Z28" s="2"/>
+      <c r="AA28" s="2"/>
       <c r="AB28" s="1"/>
       <c r="AC28" s="1"/>
       <c r="AD28" s="1"/>
@@ -9025,8 +9171,10 @@
       <c r="BJ28" s="1"/>
       <c r="BK28" s="1"/>
       <c r="BL28" s="1"/>
-    </row>
-    <row r="29" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM28" s="1"/>
+      <c r="BN28" s="1"/>
+    </row>
+    <row r="29" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="14">
         <v>43900</v>
       </c>
@@ -9042,28 +9190,32 @@
       <c r="E29" s="13">
         <v>20.7</v>
       </c>
-      <c r="F29" s="13" t="s">
+      <c r="F29" s="13">
         <v>110</v>
       </c>
-      <c r="G29" s="13">
+      <c r="G29" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="H29" s="13">
         <v>0.97199999999999998</v>
       </c>
-      <c r="H29" s="13">
+      <c r="I29" s="13">
+        <v>40</v>
+      </c>
+      <c r="J29" s="13">
         <v>0.2</v>
       </c>
-      <c r="I29" s="46" t="s">
+      <c r="K29" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13" t="s">
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="M29" s="37" t="s">
+      <c r="O29" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
@@ -9074,8 +9226,8 @@
       <c r="W29" s="2"/>
       <c r="X29" s="2"/>
       <c r="Y29" s="2"/>
-      <c r="Z29" s="1"/>
-      <c r="AA29" s="1"/>
+      <c r="Z29" s="2"/>
+      <c r="AA29" s="2"/>
       <c r="AB29" s="1"/>
       <c r="AC29" s="1"/>
       <c r="AD29" s="1"/>
@@ -9113,8 +9265,10 @@
       <c r="BJ29" s="1"/>
       <c r="BK29" s="1"/>
       <c r="BL29" s="1"/>
-    </row>
-    <row r="30" spans="1:64" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="BM29" s="1"/>
+      <c r="BN29" s="1"/>
+    </row>
+    <row r="30" spans="1:66" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="19">
         <v>43900</v>
       </c>
@@ -9130,26 +9284,30 @@
       <c r="E30" s="21">
         <v>20.7</v>
       </c>
-      <c r="F30" s="21" t="s">
+      <c r="F30" s="21">
         <v>110</v>
       </c>
-      <c r="G30" s="21">
+      <c r="G30" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="H30" s="21">
         <v>0.97199999999999998</v>
       </c>
-      <c r="H30" s="21">
+      <c r="I30" s="21">
+        <v>40</v>
+      </c>
+      <c r="J30" s="21">
         <v>0.2</v>
       </c>
-      <c r="I30" s="60" t="s">
+      <c r="K30" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="21" t="s">
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="M30" s="53"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
+      <c r="O30" s="53"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
@@ -9160,8 +9318,8 @@
       <c r="W30" s="2"/>
       <c r="X30" s="2"/>
       <c r="Y30" s="2"/>
-      <c r="Z30" s="1"/>
-      <c r="AA30" s="1"/>
+      <c r="Z30" s="2"/>
+      <c r="AA30" s="2"/>
       <c r="AB30" s="1"/>
       <c r="AC30" s="1"/>
       <c r="AD30" s="1"/>
@@ -9199,8 +9357,10 @@
       <c r="BJ30" s="1"/>
       <c r="BK30" s="1"/>
       <c r="BL30" s="1"/>
-    </row>
-    <row r="31" spans="1:64" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="BM30" s="1"/>
+      <c r="BN30" s="1"/>
+    </row>
+    <row r="31" spans="1:66" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A31" s="15"/>
       <c r="B31" s="16"/>
       <c r="C31" s="17"/>
@@ -9213,9 +9373,9 @@
       <c r="J31" s="17"/>
       <c r="K31" s="17"/>
       <c r="L31" s="17"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="18"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
@@ -9226,8 +9386,8 @@
       <c r="W31" s="2"/>
       <c r="X31" s="2"/>
       <c r="Y31" s="2"/>
-      <c r="Z31" s="1"/>
-      <c r="AA31" s="1"/>
+      <c r="Z31" s="2"/>
+      <c r="AA31" s="2"/>
       <c r="AB31" s="1"/>
       <c r="AC31" s="1"/>
       <c r="AD31" s="1"/>
@@ -9265,8 +9425,10 @@
       <c r="BJ31" s="1"/>
       <c r="BK31" s="1"/>
       <c r="BL31" s="1"/>
-    </row>
-    <row r="32" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM31" s="1"/>
+      <c r="BN31" s="1"/>
+    </row>
+    <row r="32" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" s="15"/>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -9279,9 +9441,9 @@
       <c r="J32" s="17"/>
       <c r="K32" s="17"/>
       <c r="L32" s="17"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="18"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
@@ -9292,8 +9454,8 @@
       <c r="W32" s="2"/>
       <c r="X32" s="2"/>
       <c r="Y32" s="2"/>
-      <c r="Z32" s="1"/>
-      <c r="AA32" s="1"/>
+      <c r="Z32" s="2"/>
+      <c r="AA32" s="2"/>
       <c r="AB32" s="1"/>
       <c r="AC32" s="1"/>
       <c r="AD32" s="1"/>
@@ -9331,8 +9493,10 @@
       <c r="BJ32" s="1"/>
       <c r="BK32" s="1"/>
       <c r="BL32" s="1"/>
-    </row>
-    <row r="33" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM32" s="1"/>
+      <c r="BN32" s="1"/>
+    </row>
+    <row r="33" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -9345,8 +9509,8 @@
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
@@ -9358,8 +9522,8 @@
       <c r="W33" s="2"/>
       <c r="X33" s="2"/>
       <c r="Y33" s="2"/>
-      <c r="Z33" s="1"/>
-      <c r="AA33" s="1"/>
+      <c r="Z33" s="2"/>
+      <c r="AA33" s="2"/>
       <c r="AB33" s="1"/>
       <c r="AC33" s="1"/>
       <c r="AD33" s="1"/>
@@ -9397,8 +9561,10 @@
       <c r="BJ33" s="1"/>
       <c r="BK33" s="1"/>
       <c r="BL33" s="1"/>
-    </row>
-    <row r="34" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM33" s="1"/>
+      <c r="BN33" s="1"/>
+    </row>
+    <row r="34" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="5"/>
       <c r="C34" s="2"/>
@@ -9424,8 +9590,8 @@
       <c r="W34" s="2"/>
       <c r="X34" s="2"/>
       <c r="Y34" s="2"/>
-      <c r="Z34" s="1"/>
-      <c r="AA34" s="1"/>
+      <c r="Z34" s="2"/>
+      <c r="AA34" s="2"/>
       <c r="AB34" s="1"/>
       <c r="AC34" s="1"/>
       <c r="AD34" s="1"/>
@@ -9463,8 +9629,10 @@
       <c r="BJ34" s="1"/>
       <c r="BK34" s="1"/>
       <c r="BL34" s="1"/>
-    </row>
-    <row r="35" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM34" s="1"/>
+      <c r="BN34" s="1"/>
+    </row>
+    <row r="35" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="5"/>
       <c r="C35" s="2"/>
@@ -9490,8 +9658,8 @@
       <c r="W35" s="2"/>
       <c r="X35" s="2"/>
       <c r="Y35" s="2"/>
-      <c r="Z35" s="1"/>
-      <c r="AA35" s="1"/>
+      <c r="Z35" s="2"/>
+      <c r="AA35" s="2"/>
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
       <c r="AD35" s="1"/>
@@ -9529,8 +9697,10 @@
       <c r="BJ35" s="1"/>
       <c r="BK35" s="1"/>
       <c r="BL35" s="1"/>
-    </row>
-    <row r="36" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM35" s="1"/>
+      <c r="BN35" s="1"/>
+    </row>
+    <row r="36" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="5"/>
       <c r="C36" s="2"/>
@@ -9556,8 +9726,8 @@
       <c r="W36" s="2"/>
       <c r="X36" s="2"/>
       <c r="Y36" s="2"/>
-      <c r="Z36" s="1"/>
-      <c r="AA36" s="1"/>
+      <c r="Z36" s="2"/>
+      <c r="AA36" s="2"/>
       <c r="AB36" s="1"/>
       <c r="AC36" s="1"/>
       <c r="AD36" s="1"/>
@@ -9595,8 +9765,10 @@
       <c r="BJ36" s="1"/>
       <c r="BK36" s="1"/>
       <c r="BL36" s="1"/>
-    </row>
-    <row r="37" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM36" s="1"/>
+      <c r="BN36" s="1"/>
+    </row>
+    <row r="37" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="5"/>
       <c r="C37" s="2"/>
@@ -9622,8 +9794,8 @@
       <c r="W37" s="2"/>
       <c r="X37" s="2"/>
       <c r="Y37" s="2"/>
-      <c r="Z37" s="1"/>
-      <c r="AA37" s="1"/>
+      <c r="Z37" s="2"/>
+      <c r="AA37" s="2"/>
       <c r="AB37" s="1"/>
       <c r="AC37" s="1"/>
       <c r="AD37" s="1"/>
@@ -9661,8 +9833,10 @@
       <c r="BJ37" s="1"/>
       <c r="BK37" s="1"/>
       <c r="BL37" s="1"/>
-    </row>
-    <row r="38" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM37" s="1"/>
+      <c r="BN37" s="1"/>
+    </row>
+    <row r="38" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
       <c r="B38" s="5"/>
       <c r="C38" s="2"/>
@@ -9688,8 +9862,8 @@
       <c r="W38" s="2"/>
       <c r="X38" s="2"/>
       <c r="Y38" s="2"/>
-      <c r="Z38" s="1"/>
-      <c r="AA38" s="1"/>
+      <c r="Z38" s="2"/>
+      <c r="AA38" s="2"/>
       <c r="AB38" s="1"/>
       <c r="AC38" s="1"/>
       <c r="AD38" s="1"/>
@@ -9727,8 +9901,10 @@
       <c r="BJ38" s="1"/>
       <c r="BK38" s="1"/>
       <c r="BL38" s="1"/>
-    </row>
-    <row r="39" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM38" s="1"/>
+      <c r="BN38" s="1"/>
+    </row>
+    <row r="39" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
       <c r="B39" s="5"/>
       <c r="C39" s="2"/>
@@ -9754,8 +9930,8 @@
       <c r="W39" s="2"/>
       <c r="X39" s="2"/>
       <c r="Y39" s="2"/>
-      <c r="Z39" s="1"/>
-      <c r="AA39" s="1"/>
+      <c r="Z39" s="2"/>
+      <c r="AA39" s="2"/>
       <c r="AB39" s="1"/>
       <c r="AC39" s="1"/>
       <c r="AD39" s="1"/>
@@ -9793,8 +9969,10 @@
       <c r="BJ39" s="1"/>
       <c r="BK39" s="1"/>
       <c r="BL39" s="1"/>
-    </row>
-    <row r="40" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM39" s="1"/>
+      <c r="BN39" s="1"/>
+    </row>
+    <row r="40" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
       <c r="B40" s="5"/>
       <c r="C40" s="2"/>
@@ -9820,8 +9998,8 @@
       <c r="W40" s="2"/>
       <c r="X40" s="2"/>
       <c r="Y40" s="2"/>
-      <c r="Z40" s="1"/>
-      <c r="AA40" s="1"/>
+      <c r="Z40" s="2"/>
+      <c r="AA40" s="2"/>
       <c r="AB40" s="1"/>
       <c r="AC40" s="1"/>
       <c r="AD40" s="1"/>
@@ -9859,8 +10037,10 @@
       <c r="BJ40" s="1"/>
       <c r="BK40" s="1"/>
       <c r="BL40" s="1"/>
-    </row>
-    <row r="41" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM40" s="1"/>
+      <c r="BN40" s="1"/>
+    </row>
+    <row r="41" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
       <c r="B41" s="5"/>
       <c r="C41" s="2"/>
@@ -9886,8 +10066,8 @@
       <c r="W41" s="2"/>
       <c r="X41" s="2"/>
       <c r="Y41" s="2"/>
-      <c r="Z41" s="1"/>
-      <c r="AA41" s="1"/>
+      <c r="Z41" s="2"/>
+      <c r="AA41" s="2"/>
       <c r="AB41" s="1"/>
       <c r="AC41" s="1"/>
       <c r="AD41" s="1"/>
@@ -9925,8 +10105,10 @@
       <c r="BJ41" s="1"/>
       <c r="BK41" s="1"/>
       <c r="BL41" s="1"/>
-    </row>
-    <row r="42" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM41" s="1"/>
+      <c r="BN41" s="1"/>
+    </row>
+    <row r="42" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
       <c r="B42" s="5"/>
       <c r="C42" s="2"/>
@@ -9952,8 +10134,8 @@
       <c r="W42" s="2"/>
       <c r="X42" s="2"/>
       <c r="Y42" s="2"/>
-      <c r="Z42" s="1"/>
-      <c r="AA42" s="1"/>
+      <c r="Z42" s="2"/>
+      <c r="AA42" s="2"/>
       <c r="AB42" s="1"/>
       <c r="AC42" s="1"/>
       <c r="AD42" s="1"/>
@@ -9991,8 +10173,10 @@
       <c r="BJ42" s="1"/>
       <c r="BK42" s="1"/>
       <c r="BL42" s="1"/>
-    </row>
-    <row r="43" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM42" s="1"/>
+      <c r="BN42" s="1"/>
+    </row>
+    <row r="43" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="5"/>
       <c r="C43" s="2"/>
@@ -10018,8 +10202,8 @@
       <c r="W43" s="2"/>
       <c r="X43" s="2"/>
       <c r="Y43" s="2"/>
-      <c r="Z43" s="1"/>
-      <c r="AA43" s="1"/>
+      <c r="Z43" s="2"/>
+      <c r="AA43" s="2"/>
       <c r="AB43" s="1"/>
       <c r="AC43" s="1"/>
       <c r="AD43" s="1"/>
@@ -10057,8 +10241,10 @@
       <c r="BJ43" s="1"/>
       <c r="BK43" s="1"/>
       <c r="BL43" s="1"/>
-    </row>
-    <row r="44" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM43" s="1"/>
+      <c r="BN43" s="1"/>
+    </row>
+    <row r="44" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A44" s="3"/>
       <c r="B44" s="5"/>
       <c r="C44" s="2"/>
@@ -10084,8 +10270,8 @@
       <c r="W44" s="2"/>
       <c r="X44" s="2"/>
       <c r="Y44" s="2"/>
-      <c r="Z44" s="1"/>
-      <c r="AA44" s="1"/>
+      <c r="Z44" s="2"/>
+      <c r="AA44" s="2"/>
       <c r="AB44" s="1"/>
       <c r="AC44" s="1"/>
       <c r="AD44" s="1"/>
@@ -10123,8 +10309,10 @@
       <c r="BJ44" s="1"/>
       <c r="BK44" s="1"/>
       <c r="BL44" s="1"/>
-    </row>
-    <row r="45" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM44" s="1"/>
+      <c r="BN44" s="1"/>
+    </row>
+    <row r="45" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" s="3"/>
       <c r="B45" s="5"/>
       <c r="C45" s="2"/>
@@ -10150,8 +10338,8 @@
       <c r="W45" s="2"/>
       <c r="X45" s="2"/>
       <c r="Y45" s="2"/>
-      <c r="Z45" s="1"/>
-      <c r="AA45" s="1"/>
+      <c r="Z45" s="2"/>
+      <c r="AA45" s="2"/>
       <c r="AB45" s="1"/>
       <c r="AC45" s="1"/>
       <c r="AD45" s="1"/>
@@ -10189,8 +10377,10 @@
       <c r="BJ45" s="1"/>
       <c r="BK45" s="1"/>
       <c r="BL45" s="1"/>
-    </row>
-    <row r="46" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM45" s="1"/>
+      <c r="BN45" s="1"/>
+    </row>
+    <row r="46" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" s="3"/>
       <c r="B46" s="5"/>
       <c r="C46" s="2"/>
@@ -10216,8 +10406,8 @@
       <c r="W46" s="2"/>
       <c r="X46" s="2"/>
       <c r="Y46" s="2"/>
-      <c r="Z46" s="1"/>
-      <c r="AA46" s="1"/>
+      <c r="Z46" s="2"/>
+      <c r="AA46" s="2"/>
       <c r="AB46" s="1"/>
       <c r="AC46" s="1"/>
       <c r="AD46" s="1"/>
@@ -10255,8 +10445,10 @@
       <c r="BJ46" s="1"/>
       <c r="BK46" s="1"/>
       <c r="BL46" s="1"/>
-    </row>
-    <row r="47" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM46" s="1"/>
+      <c r="BN46" s="1"/>
+    </row>
+    <row r="47" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
       <c r="B47" s="5"/>
       <c r="C47" s="2"/>
@@ -10282,8 +10474,8 @@
       <c r="W47" s="2"/>
       <c r="X47" s="2"/>
       <c r="Y47" s="2"/>
-      <c r="Z47" s="1"/>
-      <c r="AA47" s="1"/>
+      <c r="Z47" s="2"/>
+      <c r="AA47" s="2"/>
       <c r="AB47" s="1"/>
       <c r="AC47" s="1"/>
       <c r="AD47" s="1"/>
@@ -10321,8 +10513,10 @@
       <c r="BJ47" s="1"/>
       <c r="BK47" s="1"/>
       <c r="BL47" s="1"/>
-    </row>
-    <row r="48" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM47" s="1"/>
+      <c r="BN47" s="1"/>
+    </row>
+    <row r="48" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A48" s="3"/>
       <c r="B48" s="5"/>
       <c r="C48" s="2"/>
@@ -10348,8 +10542,8 @@
       <c r="W48" s="2"/>
       <c r="X48" s="2"/>
       <c r="Y48" s="2"/>
-      <c r="Z48" s="1"/>
-      <c r="AA48" s="1"/>
+      <c r="Z48" s="2"/>
+      <c r="AA48" s="2"/>
       <c r="AB48" s="1"/>
       <c r="AC48" s="1"/>
       <c r="AD48" s="1"/>
@@ -10387,8 +10581,10 @@
       <c r="BJ48" s="1"/>
       <c r="BK48" s="1"/>
       <c r="BL48" s="1"/>
-    </row>
-    <row r="49" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM48" s="1"/>
+      <c r="BN48" s="1"/>
+    </row>
+    <row r="49" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A49" s="3"/>
       <c r="B49" s="5"/>
       <c r="C49" s="2"/>
@@ -10414,8 +10610,8 @@
       <c r="W49" s="2"/>
       <c r="X49" s="2"/>
       <c r="Y49" s="2"/>
-      <c r="Z49" s="1"/>
-      <c r="AA49" s="1"/>
+      <c r="Z49" s="2"/>
+      <c r="AA49" s="2"/>
       <c r="AB49" s="1"/>
       <c r="AC49" s="1"/>
       <c r="AD49" s="1"/>
@@ -10453,8 +10649,10 @@
       <c r="BJ49" s="1"/>
       <c r="BK49" s="1"/>
       <c r="BL49" s="1"/>
-    </row>
-    <row r="50" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM49" s="1"/>
+      <c r="BN49" s="1"/>
+    </row>
+    <row r="50" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A50" s="3"/>
       <c r="B50" s="5"/>
       <c r="C50" s="2"/>
@@ -10480,8 +10678,8 @@
       <c r="W50" s="2"/>
       <c r="X50" s="2"/>
       <c r="Y50" s="2"/>
-      <c r="Z50" s="1"/>
-      <c r="AA50" s="1"/>
+      <c r="Z50" s="2"/>
+      <c r="AA50" s="2"/>
       <c r="AB50" s="1"/>
       <c r="AC50" s="1"/>
       <c r="AD50" s="1"/>
@@ -10519,8 +10717,10 @@
       <c r="BJ50" s="1"/>
       <c r="BK50" s="1"/>
       <c r="BL50" s="1"/>
-    </row>
-    <row r="51" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM50" s="1"/>
+      <c r="BN50" s="1"/>
+    </row>
+    <row r="51" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A51" s="3"/>
       <c r="B51" s="5"/>
       <c r="C51" s="2"/>
@@ -10546,8 +10746,8 @@
       <c r="W51" s="2"/>
       <c r="X51" s="2"/>
       <c r="Y51" s="2"/>
-      <c r="Z51" s="1"/>
-      <c r="AA51" s="1"/>
+      <c r="Z51" s="2"/>
+      <c r="AA51" s="2"/>
       <c r="AB51" s="1"/>
       <c r="AC51" s="1"/>
       <c r="AD51" s="1"/>
@@ -10585,8 +10785,10 @@
       <c r="BJ51" s="1"/>
       <c r="BK51" s="1"/>
       <c r="BL51" s="1"/>
-    </row>
-    <row r="52" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM51" s="1"/>
+      <c r="BN51" s="1"/>
+    </row>
+    <row r="52" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
       <c r="B52" s="5"/>
       <c r="C52" s="2"/>
@@ -10612,8 +10814,8 @@
       <c r="W52" s="2"/>
       <c r="X52" s="2"/>
       <c r="Y52" s="2"/>
-      <c r="Z52" s="1"/>
-      <c r="AA52" s="1"/>
+      <c r="Z52" s="2"/>
+      <c r="AA52" s="2"/>
       <c r="AB52" s="1"/>
       <c r="AC52" s="1"/>
       <c r="AD52" s="1"/>
@@ -10651,8 +10853,10 @@
       <c r="BJ52" s="1"/>
       <c r="BK52" s="1"/>
       <c r="BL52" s="1"/>
-    </row>
-    <row r="53" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM52" s="1"/>
+      <c r="BN52" s="1"/>
+    </row>
+    <row r="53" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A53" s="3"/>
       <c r="B53" s="5"/>
       <c r="C53" s="2"/>
@@ -10678,8 +10882,8 @@
       <c r="W53" s="2"/>
       <c r="X53" s="2"/>
       <c r="Y53" s="2"/>
-      <c r="Z53" s="1"/>
-      <c r="AA53" s="1"/>
+      <c r="Z53" s="2"/>
+      <c r="AA53" s="2"/>
       <c r="AB53" s="1"/>
       <c r="AC53" s="1"/>
       <c r="AD53" s="1"/>
@@ -10717,8 +10921,10 @@
       <c r="BJ53" s="1"/>
       <c r="BK53" s="1"/>
       <c r="BL53" s="1"/>
-    </row>
-    <row r="54" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM53" s="1"/>
+      <c r="BN53" s="1"/>
+    </row>
+    <row r="54" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A54" s="3"/>
       <c r="B54" s="5"/>
       <c r="C54" s="2"/>
@@ -10744,8 +10950,8 @@
       <c r="W54" s="2"/>
       <c r="X54" s="2"/>
       <c r="Y54" s="2"/>
-      <c r="Z54" s="1"/>
-      <c r="AA54" s="1"/>
+      <c r="Z54" s="2"/>
+      <c r="AA54" s="2"/>
       <c r="AB54" s="1"/>
       <c r="AC54" s="1"/>
       <c r="AD54" s="1"/>
@@ -10783,8 +10989,10 @@
       <c r="BJ54" s="1"/>
       <c r="BK54" s="1"/>
       <c r="BL54" s="1"/>
-    </row>
-    <row r="55" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM54" s="1"/>
+      <c r="BN54" s="1"/>
+    </row>
+    <row r="55" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A55" s="3"/>
       <c r="B55" s="5"/>
       <c r="C55" s="2"/>
@@ -10810,8 +11018,8 @@
       <c r="W55" s="2"/>
       <c r="X55" s="2"/>
       <c r="Y55" s="2"/>
-      <c r="Z55" s="1"/>
-      <c r="AA55" s="1"/>
+      <c r="Z55" s="2"/>
+      <c r="AA55" s="2"/>
       <c r="AB55" s="1"/>
       <c r="AC55" s="1"/>
       <c r="AD55" s="1"/>
@@ -10849,8 +11057,10 @@
       <c r="BJ55" s="1"/>
       <c r="BK55" s="1"/>
       <c r="BL55" s="1"/>
-    </row>
-    <row r="56" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM55" s="1"/>
+      <c r="BN55" s="1"/>
+    </row>
+    <row r="56" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A56" s="3"/>
       <c r="B56" s="5"/>
       <c r="C56" s="2"/>
@@ -10876,8 +11086,8 @@
       <c r="W56" s="2"/>
       <c r="X56" s="2"/>
       <c r="Y56" s="2"/>
-      <c r="Z56" s="1"/>
-      <c r="AA56" s="1"/>
+      <c r="Z56" s="2"/>
+      <c r="AA56" s="2"/>
       <c r="AB56" s="1"/>
       <c r="AC56" s="1"/>
       <c r="AD56" s="1"/>
@@ -10915,8 +11125,10 @@
       <c r="BJ56" s="1"/>
       <c r="BK56" s="1"/>
       <c r="BL56" s="1"/>
-    </row>
-    <row r="57" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM56" s="1"/>
+      <c r="BN56" s="1"/>
+    </row>
+    <row r="57" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A57" s="3"/>
       <c r="B57" s="5"/>
       <c r="C57" s="2"/>
@@ -10942,8 +11154,8 @@
       <c r="W57" s="2"/>
       <c r="X57" s="2"/>
       <c r="Y57" s="2"/>
-      <c r="Z57" s="1"/>
-      <c r="AA57" s="1"/>
+      <c r="Z57" s="2"/>
+      <c r="AA57" s="2"/>
       <c r="AB57" s="1"/>
       <c r="AC57" s="1"/>
       <c r="AD57" s="1"/>
@@ -10981,8 +11193,10 @@
       <c r="BJ57" s="1"/>
       <c r="BK57" s="1"/>
       <c r="BL57" s="1"/>
-    </row>
-    <row r="58" spans="1:64" ht="18" x14ac:dyDescent="0.35">
+      <c r="BM57" s="1"/>
+      <c r="BN57" s="1"/>
+    </row>
+    <row r="58" spans="1:66" ht="18" x14ac:dyDescent="0.35">
       <c r="A58" s="3"/>
       <c r="B58" s="5"/>
       <c r="C58" s="2"/>
@@ -11008,8 +11222,8 @@
       <c r="W58" s="2"/>
       <c r="X58" s="2"/>
       <c r="Y58" s="2"/>
-      <c r="Z58" s="1"/>
-      <c r="AA58" s="1"/>
+      <c r="Z58" s="2"/>
+      <c r="AA58" s="2"/>
       <c r="AB58" s="1"/>
       <c r="AC58" s="1"/>
       <c r="AD58" s="1"/>
@@ -11047,6 +11261,8 @@
       <c r="BJ58" s="1"/>
       <c r="BK58" s="1"/>
       <c r="BL58" s="1"/>
+      <c r="BM58" s="1"/>
+      <c r="BN58" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -11057,33 +11273,36 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7293150B-6AD7-4206-AAE6-A798C9E6EC4A}">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" customWidth="1"/>
     <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5546875" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="6" width="20.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" customWidth="1"/>
-    <col min="8" max="8" width="13.77734375" customWidth="1"/>
-    <col min="9" max="9" width="15.44140625" customWidth="1"/>
-    <col min="10" max="10" width="92.21875" customWidth="1"/>
-    <col min="12" max="12" width="10.88671875" customWidth="1"/>
-    <col min="13" max="13" width="23.44140625" customWidth="1"/>
-    <col min="14" max="14" width="11.77734375" customWidth="1"/>
-    <col min="15" max="15" width="14.88671875" customWidth="1"/>
-    <col min="16" max="16" width="13.33203125" customWidth="1"/>
-    <col min="17" max="17" width="14.77734375" customWidth="1"/>
-    <col min="18" max="18" width="9" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.44140625" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.21875" customWidth="1"/>
+    <col min="10" max="10" width="13.77734375" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" customWidth="1"/>
+    <col min="12" max="12" width="92.21875" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" customWidth="1"/>
+    <col min="15" max="15" width="23.44140625" customWidth="1"/>
+    <col min="16" max="16" width="11.77734375" customWidth="1"/>
+    <col min="17" max="17" width="14.88671875" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" customWidth="1"/>
+    <col min="19" max="19" width="14.77734375" customWidth="1"/>
+    <col min="20" max="20" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -11098,8 +11317,10 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A2" s="2"/>
       <c r="B2" s="27" t="s">
         <v>66</v>
@@ -11114,8 +11335,10 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -11128,38 +11351,46 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:16" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="30" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="E4" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="F4" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="G4" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="H4" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="I4" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="H4" s="30" t="s">
+      <c r="J4" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="K4" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="30" t="s">
+      <c r="L4" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:16" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="31" t="s">
         <v>13</v>
@@ -11168,60 +11399,68 @@
         <v>20.7</v>
       </c>
       <c r="D5" s="29">
+        <v>900</v>
+      </c>
+      <c r="E5" s="29">
         <v>400</v>
       </c>
-      <c r="E5" s="29">
+      <c r="F5" s="29">
         <v>9.6</v>
       </c>
-      <c r="F5" s="29">
+      <c r="G5" s="29"/>
+      <c r="H5" s="29">
         <v>13.4</v>
       </c>
-      <c r="G5" s="29">
+      <c r="I5" s="29">
         <v>100</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="J5" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="I5" s="29">
+      <c r="K5" s="29">
         <v>1000</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="L5" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2"/>
       <c r="B6" s="28"/>
       <c r="C6" s="28">
         <v>20.7</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="28">
+        <v>250</v>
+      </c>
+      <c r="E6" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="E6" s="28">
+      <c r="F6" s="28">
         <v>0.97199999999999998</v>
       </c>
-      <c r="F6" s="28">
+      <c r="G6" s="28"/>
+      <c r="H6" s="28">
         <v>0.3</v>
       </c>
-      <c r="G6" s="28">
+      <c r="I6" s="28">
         <v>100</v>
       </c>
-      <c r="H6" s="28" t="s">
+      <c r="J6" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="I6" s="28">
+      <c r="K6" s="28">
         <v>1000</v>
       </c>
-      <c r="J6" s="53" t="s">
+      <c r="L6" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:16" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="31" t="s">
         <v>16</v>
@@ -11230,300 +11469,340 @@
         <v>20.7</v>
       </c>
       <c r="D7" s="29">
+        <v>900</v>
+      </c>
+      <c r="E7" s="29">
         <v>400</v>
       </c>
-      <c r="E7" s="29">
+      <c r="F7" s="29">
         <v>9.6</v>
       </c>
-      <c r="F7" s="29">
+      <c r="G7" s="29"/>
+      <c r="H7" s="29">
         <v>13.2</v>
       </c>
-      <c r="G7" s="29">
+      <c r="I7" s="29">
         <v>100</v>
       </c>
-      <c r="H7" s="29">
+      <c r="J7" s="29">
         <v>205</v>
       </c>
-      <c r="I7" s="29" t="s">
+      <c r="K7" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="J7" s="37" t="s">
+      <c r="L7" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="28"/>
       <c r="C8" s="28">
         <v>20.7</v>
       </c>
       <c r="D8" s="28">
+        <v>220</v>
+      </c>
+      <c r="E8" s="28">
         <v>100</v>
       </c>
-      <c r="E8" s="28">
+      <c r="F8" s="28">
         <v>9.6</v>
       </c>
-      <c r="F8" s="28">
+      <c r="G8" s="28"/>
+      <c r="H8" s="28">
         <v>2.5</v>
       </c>
-      <c r="G8" s="28">
+      <c r="I8" s="28">
         <v>100</v>
       </c>
-      <c r="H8" s="28">
+      <c r="J8" s="28">
         <v>205</v>
       </c>
-      <c r="I8" s="28" t="s">
+      <c r="K8" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="J8" s="37" t="s">
+      <c r="L8" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="28"/>
       <c r="C9" s="28">
         <v>20.7</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="28">
+        <v>250</v>
+      </c>
+      <c r="E9" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="E9" s="28">
+      <c r="F9" s="28">
         <v>0.97199999999999998</v>
       </c>
-      <c r="F9" s="28">
+      <c r="G9" s="28"/>
+      <c r="H9" s="28">
         <v>0.3</v>
       </c>
-      <c r="G9" s="28">
+      <c r="I9" s="28">
         <v>100</v>
       </c>
-      <c r="H9" s="28">
+      <c r="J9" s="28">
         <v>205</v>
       </c>
-      <c r="I9" s="28" t="s">
+      <c r="K9" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="J9" s="37" t="s">
+      <c r="L9" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2"/>
       <c r="B10" s="54"/>
       <c r="C10" s="54">
         <v>20.7</v>
       </c>
       <c r="D10" s="54">
+        <v>680</v>
+      </c>
+      <c r="E10" s="54">
         <v>300</v>
       </c>
-      <c r="E10" s="54">
+      <c r="F10" s="54">
         <v>0.97199999999999998</v>
       </c>
-      <c r="F10" s="52" t="s">
+      <c r="G10" s="54"/>
+      <c r="H10" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="G10" s="54">
+      <c r="I10" s="54">
         <v>100</v>
       </c>
-      <c r="H10" s="54">
+      <c r="J10" s="54">
         <v>205</v>
       </c>
-      <c r="I10" s="54" t="s">
+      <c r="K10" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="J10" s="50" t="s">
+      <c r="L10" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-    </row>
-    <row r="11" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="56"/>
       <c r="C11" s="55">
         <v>20.7</v>
       </c>
       <c r="D11" s="55">
+        <v>680</v>
+      </c>
+      <c r="E11" s="55">
         <v>280</v>
       </c>
-      <c r="E11" s="55">
+      <c r="F11" s="55">
         <v>9.6</v>
       </c>
-      <c r="F11" s="46">
+      <c r="G11" s="55"/>
+      <c r="H11" s="46">
         <v>8.6</v>
       </c>
-      <c r="G11" s="55">
+      <c r="I11" s="55">
         <v>100</v>
       </c>
-      <c r="H11" s="55">
+      <c r="J11" s="55">
         <v>205</v>
       </c>
-      <c r="I11" s="55">
+      <c r="K11" s="55">
         <v>400</v>
       </c>
-      <c r="J11" s="62" t="s">
+      <c r="L11" s="62" t="s">
         <v>120</v>
       </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="2"/>
       <c r="B12" s="33"/>
       <c r="C12" s="55">
         <v>20.7</v>
       </c>
       <c r="D12" s="55">
+        <v>680</v>
+      </c>
+      <c r="E12" s="55">
         <v>280</v>
       </c>
-      <c r="E12" s="55">
+      <c r="F12" s="55">
         <v>9.6</v>
       </c>
-      <c r="F12" s="46">
+      <c r="G12" s="55"/>
+      <c r="H12" s="46">
         <v>8.6</v>
       </c>
-      <c r="G12" s="55">
+      <c r="I12" s="55">
         <v>100</v>
       </c>
-      <c r="H12" s="55">
+      <c r="J12" s="55">
         <v>205</v>
       </c>
-      <c r="I12" s="55">
+      <c r="K12" s="55">
         <v>1000</v>
       </c>
-      <c r="J12" s="37" t="s">
+      <c r="L12" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-    </row>
-    <row r="13" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="56"/>
       <c r="C13" s="57">
         <v>20.7</v>
       </c>
-      <c r="D13" s="57" t="s">
+      <c r="D13" s="57">
+        <v>100</v>
+      </c>
+      <c r="E13" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="57">
+      <c r="F13" s="57">
         <v>9.6</v>
       </c>
-      <c r="F13" s="58">
+      <c r="G13" s="57"/>
+      <c r="H13" s="58">
         <v>1.6</v>
       </c>
-      <c r="G13" s="57">
+      <c r="I13" s="57">
         <v>100</v>
       </c>
-      <c r="H13" s="57">
+      <c r="J13" s="57">
         <v>205</v>
       </c>
-      <c r="I13" s="57">
+      <c r="K13" s="57">
         <v>400</v>
       </c>
-      <c r="J13" s="62" t="s">
+      <c r="L13" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2"/>
       <c r="B14" s="33"/>
       <c r="C14" s="55">
         <v>20.7</v>
       </c>
-      <c r="D14" s="55" t="s">
+      <c r="D14" s="55">
+        <v>100</v>
+      </c>
+      <c r="E14" s="55" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="55">
+      <c r="F14" s="55">
         <v>9.6</v>
       </c>
-      <c r="F14" s="46">
+      <c r="G14" s="55"/>
+      <c r="H14" s="46">
         <v>1.6</v>
       </c>
-      <c r="G14" s="55">
+      <c r="I14" s="55">
         <v>100</v>
       </c>
-      <c r="H14" s="55">
+      <c r="J14" s="55">
         <v>205</v>
       </c>
-      <c r="I14" s="55">
+      <c r="K14" s="55">
         <v>1000</v>
       </c>
-      <c r="J14" s="37" t="s">
+      <c r="L14" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="56"/>
       <c r="C15" s="57">
         <v>20.7</v>
       </c>
-      <c r="D15" s="57" t="s">
+      <c r="D15" s="57">
+        <v>100</v>
+      </c>
+      <c r="E15" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="E15" s="57">
+      <c r="F15" s="57">
         <v>0.97199999999999998</v>
       </c>
-      <c r="F15" s="58">
+      <c r="G15" s="57"/>
+      <c r="H15" s="58">
         <v>0.2</v>
       </c>
-      <c r="G15" s="57">
+      <c r="I15" s="57">
         <v>100</v>
       </c>
-      <c r="H15" s="57">
+      <c r="J15" s="57">
         <v>205</v>
       </c>
-      <c r="I15" s="57">
+      <c r="K15" s="57">
         <v>400</v>
       </c>
-      <c r="J15" s="62" t="s">
+      <c r="L15" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="2"/>
       <c r="B16" s="35"/>
       <c r="C16" s="59">
         <v>20.7</v>
       </c>
-      <c r="D16" s="59" t="s">
+      <c r="D16" s="59">
+        <v>100</v>
+      </c>
+      <c r="E16" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="E16" s="59">
+      <c r="F16" s="59">
         <v>0.97199999999999998</v>
       </c>
-      <c r="F16" s="60" t="s">
+      <c r="G16" s="59"/>
+      <c r="H16" s="60" t="s">
         <v>107</v>
       </c>
-      <c r="G16" s="59">
+      <c r="I16" s="59">
         <v>100</v>
       </c>
-      <c r="H16" s="59">
+      <c r="J16" s="59">
         <v>205</v>
       </c>
-      <c r="I16" s="59">
+      <c r="K16" s="59">
         <v>1000</v>
       </c>
-      <c r="J16" s="53" t="s">
+      <c r="L16" s="53" t="s">
         <v>121</v>
       </c>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="1:14" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:16" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="31" t="s">
         <v>122</v>
@@ -11540,22 +11819,26 @@
       <c r="F17" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="G17" s="29">
+      <c r="G17" s="29"/>
+      <c r="H17" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="I17" s="29">
         <v>100</v>
       </c>
-      <c r="H17" s="29">
+      <c r="J17" s="29">
         <v>205</v>
       </c>
-      <c r="I17" s="29">
+      <c r="K17" s="29">
         <v>400</v>
       </c>
-      <c r="J17" s="37" t="s">
+      <c r="L17" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-    </row>
-    <row r="18" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2"/>
       <c r="B18" s="32"/>
       <c r="C18" s="32">
@@ -11570,42 +11853,46 @@
       <c r="F18" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="G18" s="32">
+      <c r="G18" s="32"/>
+      <c r="H18" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="I18" s="32">
         <v>100</v>
       </c>
-      <c r="H18" s="32">
+      <c r="J18" s="32">
         <v>205</v>
       </c>
-      <c r="I18" s="32">
+      <c r="K18" s="32">
         <v>1000</v>
       </c>
-      <c r="J18" s="53" t="s">
+      <c r="L18" s="53" t="s">
         <v>121</v>
       </c>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
-    </row>
-    <row r="19" spans="1:14" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+    </row>
+    <row r="19" spans="1:16" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
-    </row>
-    <row r="20" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+    </row>
+    <row r="20" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
-    </row>
-    <row r="21" spans="1:14" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+    </row>
+    <row r="21" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B21" s="27" t="s">
         <v>72</v>
       </c>
@@ -11614,43 +11901,53 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:14" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:16" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="2"/>
       <c r="C23" s="30" t="s">
         <v>4</v>
       </c>
       <c r="D23" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="E23" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="E23" s="30" t="s">
+      <c r="F23" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="F23" s="30" t="s">
+      <c r="G23" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="H23" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="G23" s="30" t="s">
+      <c r="I23" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="H23" s="30" t="s">
+      <c r="J23" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="I23" s="30" t="s">
+      <c r="K23" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="J23" s="30" t="s">
+      <c r="L23" s="30" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B24" s="31" t="s">
         <v>13</v>
       </c>
@@ -11658,55 +11955,67 @@
         <v>20.7</v>
       </c>
       <c r="D24" s="29">
+        <v>900</v>
+      </c>
+      <c r="E24" s="29">
         <v>400</v>
       </c>
-      <c r="E24" s="29">
+      <c r="F24" s="29">
         <v>9.6</v>
       </c>
-      <c r="F24" s="29">
+      <c r="G24" s="29">
+        <v>3400</v>
+      </c>
+      <c r="H24" s="29">
         <v>14.9</v>
       </c>
-      <c r="G24" s="29">
+      <c r="I24" s="29">
         <v>50</v>
       </c>
-      <c r="H24" s="29" t="s">
+      <c r="J24" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="I24" s="29">
+      <c r="K24" s="29">
         <v>800</v>
       </c>
-      <c r="J24" s="37" t="s">
+      <c r="L24" s="37" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B25" s="28"/>
       <c r="C25" s="28">
         <v>20.7</v>
       </c>
-      <c r="D25" s="28" t="s">
+      <c r="D25" s="28">
+        <v>250</v>
+      </c>
+      <c r="E25" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="E25" s="28">
+      <c r="F25" s="28">
         <v>0.97199999999999998</v>
       </c>
-      <c r="F25" s="28">
+      <c r="G25" s="28">
+        <v>130</v>
+      </c>
+      <c r="H25" s="28">
         <v>0.3</v>
       </c>
-      <c r="G25" s="28">
+      <c r="I25" s="28">
         <v>50</v>
       </c>
-      <c r="H25" s="28" t="s">
+      <c r="J25" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="I25" s="28">
+      <c r="K25" s="28">
         <v>800</v>
       </c>
-      <c r="J25" s="53" t="s">
+      <c r="L25" s="53" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B26" s="31" t="s">
         <v>16</v>
       </c>
@@ -11714,267 +12023,327 @@
         <v>20.7</v>
       </c>
       <c r="D26" s="29">
+        <v>900</v>
+      </c>
+      <c r="E26" s="29">
         <v>400</v>
       </c>
-      <c r="E26" s="29">
+      <c r="F26" s="29">
         <v>9.6</v>
       </c>
-      <c r="F26" s="29">
+      <c r="G26" s="29">
+        <v>3400</v>
+      </c>
+      <c r="H26" s="29">
         <v>14.8</v>
       </c>
-      <c r="G26" s="29">
+      <c r="I26" s="29">
         <v>50</v>
       </c>
-      <c r="H26" s="29">
+      <c r="J26" s="29">
         <v>195</v>
       </c>
-      <c r="I26" s="29" t="s">
+      <c r="K26" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="J26" s="37" t="s">
+      <c r="L26" s="37" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="B27" s="28"/>
       <c r="C27" s="28">
         <v>20.7</v>
       </c>
       <c r="D27" s="28">
+        <v>900</v>
+      </c>
+      <c r="E27" s="28">
         <v>400</v>
       </c>
-      <c r="E27" s="28">
+      <c r="F27" s="28">
         <v>9.6</v>
       </c>
-      <c r="F27" s="28">
+      <c r="G27" s="28">
+        <v>3400</v>
+      </c>
+      <c r="H27" s="28">
         <v>14.9</v>
       </c>
-      <c r="G27" s="28">
+      <c r="I27" s="28">
         <v>50</v>
       </c>
-      <c r="H27" s="28">
+      <c r="J27" s="28">
         <v>190</v>
       </c>
-      <c r="I27" s="28" t="s">
+      <c r="K27" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="J27" s="37" t="s">
+      <c r="L27" s="37" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="B28" s="28"/>
       <c r="C28" s="28">
         <v>20.7</v>
       </c>
       <c r="D28" s="28">
+        <v>250</v>
+      </c>
+      <c r="E28" s="28">
         <v>150</v>
       </c>
-      <c r="E28" s="28">
+      <c r="F28" s="28">
         <v>9.6</v>
       </c>
-      <c r="F28" s="28">
+      <c r="G28" s="28">
+        <v>1300</v>
+      </c>
+      <c r="H28" s="28">
         <v>3.4</v>
       </c>
-      <c r="G28" s="28">
+      <c r="I28" s="28">
         <v>50</v>
       </c>
-      <c r="H28" s="28">
+      <c r="J28" s="28">
         <v>190</v>
       </c>
-      <c r="I28" s="28" t="s">
+      <c r="K28" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="J28" s="37" t="s">
+      <c r="L28" s="37" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="B29" s="28"/>
       <c r="C29" s="28">
         <v>20.7</v>
       </c>
       <c r="D29" s="28">
+        <v>110</v>
+      </c>
+      <c r="E29" s="28">
         <v>60</v>
       </c>
-      <c r="E29" s="28">
+      <c r="F29" s="28">
         <v>9.6</v>
       </c>
-      <c r="F29" s="28">
+      <c r="G29" s="28">
+        <v>510</v>
+      </c>
+      <c r="H29" s="28">
         <v>1.5</v>
       </c>
-      <c r="G29" s="28">
+      <c r="I29" s="28">
         <v>50</v>
       </c>
-      <c r="H29" s="28">
+      <c r="J29" s="28">
         <v>190</v>
       </c>
-      <c r="I29" s="28" t="s">
+      <c r="K29" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="J29" s="37" t="s">
+      <c r="L29" s="37" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="B30" s="28"/>
       <c r="C30" s="28">
         <v>20.7</v>
       </c>
       <c r="D30" s="28">
+        <v>680</v>
+      </c>
+      <c r="E30" s="28">
         <v>280</v>
       </c>
-      <c r="E30" s="28">
+      <c r="F30" s="28">
         <v>0.97199999999999998</v>
       </c>
-      <c r="F30" s="28">
+      <c r="G30" s="28">
+        <v>220</v>
+      </c>
+      <c r="H30" s="28">
         <v>0.9</v>
       </c>
-      <c r="G30" s="28">
+      <c r="I30" s="28">
         <v>50</v>
       </c>
-      <c r="H30" s="28">
+      <c r="J30" s="28">
         <v>190</v>
       </c>
-      <c r="I30" s="28" t="s">
+      <c r="K30" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="J30" s="37" t="s">
+      <c r="L30" s="37" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B31" s="54"/>
       <c r="C31" s="54">
         <v>20.7</v>
       </c>
-      <c r="D31" s="54" t="s">
+      <c r="D31" s="54">
+        <v>250</v>
+      </c>
+      <c r="E31" s="54" t="s">
         <v>147</v>
       </c>
-      <c r="E31" s="54">
+      <c r="F31" s="54">
         <v>0.97199999999999998</v>
       </c>
-      <c r="F31" s="52">
+      <c r="G31" s="54">
+        <v>130</v>
+      </c>
+      <c r="H31" s="52">
         <v>0.4</v>
       </c>
-      <c r="G31" s="54">
+      <c r="I31" s="54">
         <v>50</v>
       </c>
-      <c r="H31" s="54">
+      <c r="J31" s="54">
         <v>190</v>
       </c>
-      <c r="I31" s="54" t="s">
+      <c r="K31" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="J31" s="37" t="s">
+      <c r="L31" s="37" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="B32" s="56"/>
       <c r="C32" s="55">
         <v>20.7</v>
       </c>
       <c r="D32" s="55">
+        <v>680</v>
+      </c>
+      <c r="E32" s="55">
         <v>280</v>
       </c>
-      <c r="E32" s="55">
+      <c r="F32" s="55">
         <v>9.6</v>
       </c>
-      <c r="F32" s="46">
+      <c r="G32" s="55">
+        <v>2400</v>
+      </c>
+      <c r="H32" s="46">
         <v>8.9</v>
       </c>
-      <c r="G32" s="55">
+      <c r="I32" s="55">
         <v>50</v>
       </c>
-      <c r="H32" s="55">
+      <c r="J32" s="55">
         <v>190</v>
       </c>
-      <c r="I32" s="55">
+      <c r="K32" s="55">
         <v>400</v>
       </c>
-      <c r="J32" s="62" t="s">
+      <c r="L32" s="62" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B33" s="64"/>
       <c r="C33" s="65">
         <v>20.7</v>
       </c>
       <c r="D33" s="65">
+        <v>680</v>
+      </c>
+      <c r="E33" s="65">
         <v>280</v>
       </c>
-      <c r="E33" s="65">
+      <c r="F33" s="65">
         <v>9.6</v>
       </c>
-      <c r="F33" s="66">
+      <c r="G33" s="65">
+        <v>2400</v>
+      </c>
+      <c r="H33" s="66">
         <v>9.5</v>
       </c>
-      <c r="G33" s="65">
+      <c r="I33" s="65">
         <v>50</v>
       </c>
-      <c r="H33" s="65">
+      <c r="J33" s="65">
         <v>190</v>
       </c>
-      <c r="I33" s="65">
+      <c r="K33" s="65">
         <v>1000</v>
       </c>
-      <c r="J33" s="67"/>
-    </row>
-    <row r="34" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="L33" s="67"/>
+    </row>
+    <row r="34" spans="2:12" ht="18" x14ac:dyDescent="0.35">
       <c r="B34" s="33"/>
       <c r="C34" s="55">
         <v>20.7</v>
       </c>
-      <c r="D34" s="55" t="s">
+      <c r="D34" s="55">
         <v>110</v>
       </c>
-      <c r="E34" s="55">
+      <c r="E34" s="55" t="s">
+        <v>110</v>
+      </c>
+      <c r="F34" s="55">
         <v>0.97199999999999998</v>
       </c>
-      <c r="F34" s="46">
+      <c r="G34" s="55">
+        <v>40</v>
+      </c>
+      <c r="H34" s="46">
         <v>0.2</v>
       </c>
-      <c r="G34" s="55">
+      <c r="I34" s="55">
         <v>50</v>
       </c>
-      <c r="H34" s="55">
+      <c r="J34" s="55">
         <v>190</v>
       </c>
-      <c r="I34" s="55">
+      <c r="K34" s="55">
         <v>400</v>
       </c>
-      <c r="J34" s="37" t="s">
+      <c r="L34" s="37" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="35" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="33"/>
       <c r="C35" s="55">
         <v>20.7</v>
       </c>
-      <c r="D35" s="55" t="s">
+      <c r="D35" s="55">
         <v>110</v>
       </c>
-      <c r="E35" s="55">
+      <c r="E35" s="55" t="s">
+        <v>110</v>
+      </c>
+      <c r="F35" s="55">
         <v>0.97199999999999998</v>
       </c>
-      <c r="F35" s="46">
+      <c r="G35" s="55">
+        <v>40</v>
+      </c>
+      <c r="H35" s="46">
         <v>0.2</v>
       </c>
-      <c r="G35" s="55">
+      <c r="I35" s="55">
         <v>50</v>
       </c>
-      <c r="H35" s="55">
+      <c r="J35" s="55">
         <v>190</v>
       </c>
-      <c r="I35" s="55">
+      <c r="K35" s="55">
         <v>1000</v>
       </c>
-      <c r="J35" s="61"/>
-    </row>
-    <row r="36" spans="2:10" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="L35" s="61"/>
+    </row>
+    <row r="36" spans="2:12" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B36" s="31" t="s">
         <v>122</v>
       </c>
@@ -11990,20 +12359,26 @@
       <c r="F36" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="G36" s="29">
+      <c r="G36" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="H36" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="I36" s="29">
         <v>50</v>
       </c>
-      <c r="H36" s="29">
+      <c r="J36" s="29">
         <v>190</v>
       </c>
-      <c r="I36" s="29">
+      <c r="K36" s="29">
         <v>400</v>
       </c>
-      <c r="J36" s="37" t="s">
+      <c r="L36" s="37" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="37" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B37" s="32"/>
       <c r="C37" s="32">
         <v>20.7</v>
@@ -12017,20 +12392,26 @@
       <c r="F37" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="G37" s="32">
+      <c r="G37" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="H37" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="I37" s="32">
         <v>50</v>
       </c>
-      <c r="H37" s="32">
+      <c r="J37" s="32">
         <v>190</v>
       </c>
-      <c r="I37" s="32">
+      <c r="K37" s="32">
         <v>1000</v>
       </c>
-      <c r="J37" s="53" t="s">
+      <c r="L37" s="53" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="38" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -12041,7 +12422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B66FBB42-8B7D-4E2F-B67D-D60F4EF2D11F}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Aggiunti i grafici della corrente anodica in funzione del rate, con barra di errore. Modificata la macro plotTable_Rate.C in modo che stampi l'errore del 10% sulla corrente anodica. Modificato il .gitignore così da non tracciare il file temporaneo .~lock.Caratterizzazione_THGEM.xlsx#.
</commit_message>
<xml_diff>
--- a/Caratterizzazione_THGEM.xlsx
+++ b/Caratterizzazione_THGEM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ireneciraldo/Desktop/graphics_testbeam_mar20_fullthgem/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peppe\Desktop\LaTex\Report_THGEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7AE97C-681C-5843-83B7-1B21E14A8098}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0206D0A0-2EE7-4E10-B764-4105C5DC9DDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" activeTab="2" xr2:uid="{ACFC7C87-C28D-4487-B063-88156E979354}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{ACFC7C87-C28D-4487-B063-88156E979354}"/>
   </bookViews>
   <sheets>
     <sheet name="alpha-crono" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,18 @@
     <sheet name="test_2020-03-09" sheetId="3" r:id="rId4"/>
     <sheet name="Calculations" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1046,10 +1054,10 @@
     <t>Rate_tracker (pps)</t>
   </si>
   <si>
-    <t>Ibeam (pA) calculated from MXFC1</t>
-  </si>
-  <si>
     <t>Ibeam (pA) from FC</t>
+  </si>
+  <si>
+    <t>Ibeam (pA) calc from MXFC1</t>
   </si>
 </sst>
 </file>
@@ -1280,7 +1288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1466,9 +1474,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1790,22 +1795,22 @@
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" customWidth="1"/>
-    <col min="6" max="6" width="21.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" customWidth="1"/>
-    <col min="9" max="9" width="33.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" customWidth="1"/>
+    <col min="9" max="9" width="33.77734375" customWidth="1"/>
     <col min="10" max="11" width="12" customWidth="1"/>
     <col min="12" max="12" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:61" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1886,7 +1891,7 @@
       <c r="BH1" s="1"/>
       <c r="BI1" s="1"/>
     </row>
-    <row r="2" spans="1:61" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:61" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10">
         <v>43802</v>
       </c>
@@ -1967,7 +1972,7 @@
       <c r="BH2" s="1"/>
       <c r="BI2" s="1"/>
     </row>
-    <row r="3" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="14">
         <v>43803</v>
       </c>
@@ -2048,7 +2053,7 @@
       <c r="BH3" s="1"/>
       <c r="BI3" s="1"/>
     </row>
-    <row r="4" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="14">
         <v>43803</v>
       </c>
@@ -2129,7 +2134,7 @@
       <c r="BH4" s="1"/>
       <c r="BI4" s="1"/>
     </row>
-    <row r="5" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="14">
         <v>43803</v>
       </c>
@@ -2210,7 +2215,7 @@
       <c r="BH5" s="1"/>
       <c r="BI5" s="1"/>
     </row>
-    <row r="6" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="14">
         <v>43803</v>
       </c>
@@ -2291,7 +2296,7 @@
       <c r="BH6" s="1"/>
       <c r="BI6" s="1"/>
     </row>
-    <row r="7" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="14">
         <v>43804</v>
       </c>
@@ -2372,7 +2377,7 @@
       <c r="BH7" s="1"/>
       <c r="BI7" s="1"/>
     </row>
-    <row r="8" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="14">
         <v>43805</v>
       </c>
@@ -2453,7 +2458,7 @@
       <c r="BH8" s="1"/>
       <c r="BI8" s="1"/>
     </row>
-    <row r="9" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="14">
         <v>43805</v>
       </c>
@@ -2534,7 +2539,7 @@
       <c r="BH9" s="1"/>
       <c r="BI9" s="1"/>
     </row>
-    <row r="10" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="14">
         <v>43808</v>
       </c>
@@ -2615,7 +2620,7 @@
       <c r="BH10" s="1"/>
       <c r="BI10" s="1"/>
     </row>
-    <row r="11" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="14">
         <v>43808</v>
       </c>
@@ -2696,7 +2701,7 @@
       <c r="BH11" s="1"/>
       <c r="BI11" s="1"/>
     </row>
-    <row r="12" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="14">
         <v>43808</v>
       </c>
@@ -2777,7 +2782,7 @@
       <c r="BH12" s="1"/>
       <c r="BI12" s="1"/>
     </row>
-    <row r="13" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="14">
         <v>43808</v>
       </c>
@@ -2858,7 +2863,7 @@
       <c r="BH13" s="1"/>
       <c r="BI13" s="1"/>
     </row>
-    <row r="14" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="14">
         <v>43808</v>
       </c>
@@ -2939,7 +2944,7 @@
       <c r="BH14" s="1"/>
       <c r="BI14" s="1"/>
     </row>
-    <row r="15" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="14">
         <v>43808</v>
       </c>
@@ -3020,7 +3025,7 @@
       <c r="BH15" s="1"/>
       <c r="BI15" s="1"/>
     </row>
-    <row r="16" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>43881</v>
       </c>
@@ -3101,7 +3106,7 @@
       <c r="BH16" s="1"/>
       <c r="BI16" s="1"/>
     </row>
-    <row r="17" spans="1:61" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:61" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <v>43881</v>
       </c>
@@ -3182,7 +3187,7 @@
       <c r="BH17" s="1"/>
       <c r="BI17" s="1"/>
     </row>
-    <row r="18" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="24">
         <v>43810</v>
       </c>
@@ -3263,7 +3268,7 @@
       <c r="BH18" s="1"/>
       <c r="BI18" s="1"/>
     </row>
-    <row r="19" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="14">
         <v>43810</v>
       </c>
@@ -3338,7 +3343,7 @@
       <c r="BH19" s="1"/>
       <c r="BI19" s="1"/>
     </row>
-    <row r="20" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="14">
         <v>43810</v>
       </c>
@@ -3419,7 +3424,7 @@
       <c r="BH20" s="1"/>
       <c r="BI20" s="1"/>
     </row>
-    <row r="21" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="14">
         <v>43816</v>
       </c>
@@ -3500,7 +3505,7 @@
       <c r="BH21" s="1"/>
       <c r="BI21" s="1"/>
     </row>
-    <row r="22" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="14">
         <v>43816</v>
       </c>
@@ -3581,7 +3586,7 @@
       <c r="BH22" s="1"/>
       <c r="BI22" s="1"/>
     </row>
-    <row r="23" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A23" s="14">
         <v>43817</v>
       </c>
@@ -3662,7 +3667,7 @@
       <c r="BH23" s="1"/>
       <c r="BI23" s="1"/>
     </row>
-    <row r="24" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" s="14">
         <v>43817</v>
       </c>
@@ -3743,7 +3748,7 @@
       <c r="BH24" s="1"/>
       <c r="BI24" s="1"/>
     </row>
-    <row r="25" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" s="14">
         <v>43837</v>
       </c>
@@ -3824,7 +3829,7 @@
       <c r="BH25" s="1"/>
       <c r="BI25" s="1"/>
     </row>
-    <row r="26" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="14">
         <v>43837</v>
       </c>
@@ -3905,7 +3910,7 @@
       <c r="BH26" s="1"/>
       <c r="BI26" s="1"/>
     </row>
-    <row r="27" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="14">
         <v>43837</v>
       </c>
@@ -3986,7 +3991,7 @@
       <c r="BH27" s="1"/>
       <c r="BI27" s="1"/>
     </row>
-    <row r="28" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="14">
         <v>43837</v>
       </c>
@@ -4067,7 +4072,7 @@
       <c r="BH28" s="1"/>
       <c r="BI28" s="1"/>
     </row>
-    <row r="29" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="14">
         <v>43837</v>
       </c>
@@ -4148,7 +4153,7 @@
       <c r="BH29" s="1"/>
       <c r="BI29" s="1"/>
     </row>
-    <row r="30" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A30" s="14">
         <v>43865</v>
       </c>
@@ -4229,7 +4234,7 @@
       <c r="BH30" s="1"/>
       <c r="BI30" s="1"/>
     </row>
-    <row r="31" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="14">
         <v>43865</v>
       </c>
@@ -4310,7 +4315,7 @@
       <c r="BH31" s="1"/>
       <c r="BI31" s="1"/>
     </row>
-    <row r="32" spans="1:61" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:61" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="19">
         <v>43865</v>
       </c>
@@ -4391,7 +4396,7 @@
       <c r="BH32" s="1"/>
       <c r="BI32" s="1"/>
     </row>
-    <row r="33" spans="1:61" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:61" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -4454,7 +4459,7 @@
       <c r="BH33" s="1"/>
       <c r="BI33" s="1"/>
     </row>
-    <row r="34" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -4517,7 +4522,7 @@
       <c r="BH34" s="1"/>
       <c r="BI34" s="1"/>
     </row>
-    <row r="35" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -4580,7 +4585,7 @@
       <c r="BH35" s="1"/>
       <c r="BI35" s="1"/>
     </row>
-    <row r="36" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -4643,7 +4648,7 @@
       <c r="BH36" s="1"/>
       <c r="BI36" s="1"/>
     </row>
-    <row r="37" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -4706,7 +4711,7 @@
       <c r="BH37" s="1"/>
       <c r="BI37" s="1"/>
     </row>
-    <row r="38" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -4769,7 +4774,7 @@
       <c r="BH38" s="1"/>
       <c r="BI38" s="1"/>
     </row>
-    <row r="39" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -4832,7 +4837,7 @@
       <c r="BH39" s="1"/>
       <c r="BI39" s="1"/>
     </row>
-    <row r="40" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -4895,7 +4900,7 @@
       <c r="BH40" s="1"/>
       <c r="BI40" s="1"/>
     </row>
-    <row r="41" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -4958,7 +4963,7 @@
       <c r="BH41" s="1"/>
       <c r="BI41" s="1"/>
     </row>
-    <row r="42" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -5021,7 +5026,7 @@
       <c r="BH42" s="1"/>
       <c r="BI42" s="1"/>
     </row>
-    <row r="43" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -5084,7 +5089,7 @@
       <c r="BH43" s="1"/>
       <c r="BI43" s="1"/>
     </row>
-    <row r="44" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A44" s="3"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -5147,7 +5152,7 @@
       <c r="BH44" s="1"/>
       <c r="BI44" s="1"/>
     </row>
-    <row r="45" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" s="3"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -5210,7 +5215,7 @@
       <c r="BH45" s="1"/>
       <c r="BI45" s="1"/>
     </row>
-    <row r="46" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" s="3"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -5273,7 +5278,7 @@
       <c r="BH46" s="1"/>
       <c r="BI46" s="1"/>
     </row>
-    <row r="47" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -5336,7 +5341,7 @@
       <c r="BH47" s="1"/>
       <c r="BI47" s="1"/>
     </row>
-    <row r="48" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A48" s="3"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -5399,7 +5404,7 @@
       <c r="BH48" s="1"/>
       <c r="BI48" s="1"/>
     </row>
-    <row r="49" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A49" s="3"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -5462,7 +5467,7 @@
       <c r="BH49" s="1"/>
       <c r="BI49" s="1"/>
     </row>
-    <row r="50" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A50" s="3"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -5525,7 +5530,7 @@
       <c r="BH50" s="1"/>
       <c r="BI50" s="1"/>
     </row>
-    <row r="51" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A51" s="3"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -5588,7 +5593,7 @@
       <c r="BH51" s="1"/>
       <c r="BI51" s="1"/>
     </row>
-    <row r="52" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -5651,7 +5656,7 @@
       <c r="BH52" s="1"/>
       <c r="BI52" s="1"/>
     </row>
-    <row r="53" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A53" s="3"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -5714,7 +5719,7 @@
       <c r="BH53" s="1"/>
       <c r="BI53" s="1"/>
     </row>
-    <row r="54" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A54" s="3"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -5777,7 +5782,7 @@
       <c r="BH54" s="1"/>
       <c r="BI54" s="1"/>
     </row>
-    <row r="55" spans="1:61" ht="19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:61" ht="18" x14ac:dyDescent="0.35">
       <c r="A55" s="3"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -5855,24 +5860,24 @@
       <selection activeCell="K17" sqref="K17:M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" customWidth="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1"/>
     <col min="7" max="7" width="36.33203125" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" customWidth="1"/>
-    <col min="10" max="10" width="23.5" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" customWidth="1"/>
-    <col min="12" max="12" width="14.83203125" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" customWidth="1"/>
+    <col min="12" max="12" width="14.77734375" customWidth="1"/>
     <col min="13" max="13" width="13.33203125" customWidth="1"/>
-    <col min="14" max="14" width="14.83203125" customWidth="1"/>
+    <col min="14" max="14" width="14.77734375" customWidth="1"/>
     <col min="15" max="15" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -5885,7 +5890,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:15" ht="26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A2" s="2"/>
       <c r="B2" s="27" t="s">
         <v>66</v>
@@ -5905,7 +5910,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -5921,7 +5926,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:15" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="30" t="s">
@@ -5958,7 +5963,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="31" t="s">
         <v>70</v>
@@ -5995,7 +6000,7 @@
       </c>
       <c r="O5" s="34"/>
     </row>
-    <row r="6" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="28"/>
       <c r="C6" s="28">
@@ -6028,7 +6033,7 @@
       </c>
       <c r="O6" s="33"/>
     </row>
-    <row r="7" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="28"/>
       <c r="C7" s="28">
@@ -6061,7 +6066,7 @@
       </c>
       <c r="O7" s="33"/>
     </row>
-    <row r="8" spans="1:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2"/>
       <c r="B8" s="28"/>
       <c r="C8" s="28">
@@ -6094,7 +6099,7 @@
       </c>
       <c r="O8" s="35"/>
     </row>
-    <row r="9" spans="1:15" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="28"/>
       <c r="C9" s="28">
@@ -6131,7 +6136,7 @@
       </c>
       <c r="O9" s="34"/>
     </row>
-    <row r="10" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="28"/>
       <c r="C10" s="28">
@@ -6166,7 +6171,7 @@
       </c>
       <c r="O10" s="33"/>
     </row>
-    <row r="11" spans="1:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2"/>
       <c r="B11" s="28"/>
       <c r="C11" s="28">
@@ -6199,7 +6204,7 @@
       </c>
       <c r="O11" s="33"/>
     </row>
-    <row r="12" spans="1:15" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="31" t="s">
         <v>13</v>
@@ -6234,7 +6239,7 @@
       </c>
       <c r="O12" s="33"/>
     </row>
-    <row r="13" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="28"/>
       <c r="C13" s="28">
@@ -6267,7 +6272,7 @@
       </c>
       <c r="O13" s="33"/>
     </row>
-    <row r="14" spans="1:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2"/>
       <c r="B14" s="28"/>
       <c r="C14" s="28">
@@ -6300,7 +6305,7 @@
       </c>
       <c r="O14" s="33"/>
     </row>
-    <row r="15" spans="1:15" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="2"/>
       <c r="B15" s="35"/>
       <c r="C15" s="28">
@@ -6337,7 +6342,7 @@
       </c>
       <c r="O15" s="34"/>
     </row>
-    <row r="16" spans="1:15" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="31" t="s">
         <v>16</v>
@@ -6372,7 +6377,7 @@
       </c>
       <c r="O16" s="33"/>
     </row>
-    <row r="17" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="28"/>
       <c r="C17" s="28">
@@ -6405,7 +6410,7 @@
       </c>
       <c r="O17" s="33"/>
     </row>
-    <row r="18" spans="1:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2"/>
       <c r="B18" s="28"/>
       <c r="C18" s="28">
@@ -6438,7 +6443,7 @@
       </c>
       <c r="O18" s="35"/>
     </row>
-    <row r="19" spans="1:15" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="28"/>
       <c r="C19" s="28">
@@ -6459,7 +6464,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="2"/>
       <c r="B20" s="32"/>
       <c r="C20" s="32">
@@ -6482,7 +6487,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:15" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -6504,30 +6509,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E260431C-5552-43E0-806B-E171CCC2519A}">
   <dimension ref="A1:BO58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="16.5" style="6" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
     <col min="5" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="8" width="18.1640625" customWidth="1"/>
-    <col min="9" max="10" width="18.5" customWidth="1"/>
-    <col min="11" max="11" width="19.83203125" customWidth="1"/>
-    <col min="12" max="12" width="21.1640625" customWidth="1"/>
-    <col min="13" max="13" width="11.83203125" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.5546875" customWidth="1"/>
+    <col min="9" max="10" width="18.44140625" customWidth="1"/>
+    <col min="11" max="11" width="19.77734375" customWidth="1"/>
+    <col min="12" max="12" width="21.109375" customWidth="1"/>
+    <col min="13" max="13" width="11.77734375" customWidth="1"/>
     <col min="14" max="14" width="11.33203125" customWidth="1"/>
-    <col min="15" max="15" width="39.1640625" customWidth="1"/>
+    <col min="15" max="15" width="39.109375" customWidth="1"/>
     <col min="16" max="16" width="91" customWidth="1"/>
-    <col min="17" max="17" width="19.83203125" customWidth="1"/>
+    <col min="17" max="17" width="19.77734375" customWidth="1"/>
     <col min="18" max="18" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:67" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -6546,11 +6552,11 @@
       <c r="F1" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="G1" s="68" t="s">
+      <c r="G1" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="H1" s="68" t="s">
-        <v>164</v>
       </c>
       <c r="I1" s="9" t="s">
         <v>78</v>
@@ -6628,7 +6634,7 @@
       <c r="BN1" s="1"/>
       <c r="BO1" s="1"/>
     </row>
-    <row r="2" spans="1:67" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:67" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10">
         <v>43899</v>
       </c>
@@ -6723,7 +6729,7 @@
       <c r="BN2" s="1"/>
       <c r="BO2" s="1"/>
     </row>
-    <row r="3" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="14">
         <v>43899</v>
       </c>
@@ -6822,7 +6828,7 @@
       <c r="BN3" s="1"/>
       <c r="BO3" s="1"/>
     </row>
-    <row r="4" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="14">
         <v>43899</v>
       </c>
@@ -6921,7 +6927,7 @@
       <c r="BN4" s="1"/>
       <c r="BO4" s="1"/>
     </row>
-    <row r="5" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="14">
         <v>43899</v>
       </c>
@@ -7016,7 +7022,7 @@
       <c r="BN5" s="1"/>
       <c r="BO5" s="1"/>
     </row>
-    <row r="6" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="14">
         <v>43899</v>
       </c>
@@ -7109,7 +7115,7 @@
       <c r="BN6" s="1"/>
       <c r="BO6" s="1"/>
     </row>
-    <row r="7" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="14">
         <v>43899</v>
       </c>
@@ -7208,7 +7214,7 @@
       <c r="BN7" s="1"/>
       <c r="BO7" s="1"/>
     </row>
-    <row r="8" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="14">
         <v>43899</v>
       </c>
@@ -7303,7 +7309,7 @@
       <c r="BN8" s="1"/>
       <c r="BO8" s="1"/>
     </row>
-    <row r="9" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="14">
         <v>43899</v>
       </c>
@@ -7398,7 +7404,7 @@
       <c r="BN9" s="1"/>
       <c r="BO9" s="1"/>
     </row>
-    <row r="10" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="14">
         <v>43899</v>
       </c>
@@ -7495,7 +7501,7 @@
       <c r="BN10" s="1"/>
       <c r="BO10" s="1"/>
     </row>
-    <row r="11" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="14">
         <v>43899</v>
       </c>
@@ -7592,7 +7598,7 @@
       <c r="BN11" s="1"/>
       <c r="BO11" s="1"/>
     </row>
-    <row r="12" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="14">
         <v>43899</v>
       </c>
@@ -7693,7 +7699,7 @@
       <c r="BN12" s="1"/>
       <c r="BO12" s="1"/>
     </row>
-    <row r="13" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="14">
         <v>43899</v>
       </c>
@@ -7794,7 +7800,7 @@
       <c r="BN13" s="1"/>
       <c r="BO13" s="1"/>
     </row>
-    <row r="14" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="14">
         <v>43899</v>
       </c>
@@ -7889,7 +7895,7 @@
       <c r="BN14" s="1"/>
       <c r="BO14" s="1"/>
     </row>
-    <row r="15" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="14">
         <v>43899</v>
       </c>
@@ -7982,7 +7988,7 @@
       <c r="BN15" s="1"/>
       <c r="BO15" s="1"/>
     </row>
-    <row r="16" spans="1:67" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:67" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="49">
         <v>43899</v>
       </c>
@@ -8081,7 +8087,7 @@
       <c r="BN16" s="1"/>
       <c r="BO16" s="1"/>
     </row>
-    <row r="17" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="14">
         <v>43900</v>
       </c>
@@ -8176,7 +8182,7 @@
       <c r="BN17" s="1"/>
       <c r="BO17" s="1"/>
     </row>
-    <row r="18" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="14">
         <v>43900</v>
       </c>
@@ -8271,7 +8277,7 @@
       <c r="BN18" s="1"/>
       <c r="BO18" s="1"/>
     </row>
-    <row r="19" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="14">
         <v>43900</v>
       </c>
@@ -8370,7 +8376,7 @@
       <c r="BN19" s="1"/>
       <c r="BO19" s="1"/>
     </row>
-    <row r="20" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="14">
         <v>43900</v>
       </c>
@@ -8469,7 +8475,7 @@
       <c r="BN20" s="1"/>
       <c r="BO20" s="1"/>
     </row>
-    <row r="21" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="14">
         <v>43900</v>
       </c>
@@ -8568,7 +8574,7 @@
       <c r="BN21" s="1"/>
       <c r="BO21" s="1"/>
     </row>
-    <row r="22" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="14">
         <v>43900</v>
       </c>
@@ -8663,7 +8669,7 @@
       <c r="BN22" s="1"/>
       <c r="BO22" s="1"/>
     </row>
-    <row r="23" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A23" s="14">
         <v>43900</v>
       </c>
@@ -8756,7 +8762,7 @@
       <c r="BN23" s="1"/>
       <c r="BO23" s="1"/>
     </row>
-    <row r="24" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" s="14">
         <v>43900</v>
       </c>
@@ -8855,7 +8861,7 @@
       <c r="BN24" s="1"/>
       <c r="BO24" s="1"/>
     </row>
-    <row r="25" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" s="14">
         <v>43900</v>
       </c>
@@ -8954,7 +8960,7 @@
       <c r="BN25" s="1"/>
       <c r="BO25" s="1"/>
     </row>
-    <row r="26" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="14">
         <v>43900</v>
       </c>
@@ -9053,7 +9059,7 @@
       <c r="BN26" s="1"/>
       <c r="BO26" s="1"/>
     </row>
-    <row r="27" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="14">
         <v>43900</v>
       </c>
@@ -9152,7 +9158,7 @@
       <c r="BN27" s="1"/>
       <c r="BO27" s="1"/>
     </row>
-    <row r="28" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="14">
         <v>43900</v>
       </c>
@@ -9251,7 +9257,7 @@
       <c r="BN28" s="1"/>
       <c r="BO28" s="1"/>
     </row>
-    <row r="29" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="14">
         <v>43900</v>
       </c>
@@ -9273,7 +9279,9 @@
       <c r="G29" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="H29" s="13"/>
+      <c r="H29" s="13">
+        <v>50</v>
+      </c>
       <c r="I29" s="13">
         <v>0.97199999999999998</v>
       </c>
@@ -9346,7 +9354,7 @@
       <c r="BN29" s="1"/>
       <c r="BO29" s="1"/>
     </row>
-    <row r="30" spans="1:67" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:67" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="19">
         <v>43900</v>
       </c>
@@ -9368,7 +9376,9 @@
       <c r="G30" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="H30" s="21"/>
+      <c r="H30" s="21">
+        <v>50</v>
+      </c>
       <c r="I30" s="21">
         <v>0.97199999999999998</v>
       </c>
@@ -9439,7 +9449,7 @@
       <c r="BN30" s="1"/>
       <c r="BO30" s="1"/>
     </row>
-    <row r="31" spans="1:67" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:67" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A31" s="15"/>
       <c r="B31" s="16"/>
       <c r="C31" s="17"/>
@@ -9508,7 +9518,7 @@
       <c r="BN31" s="1"/>
       <c r="BO31" s="1"/>
     </row>
-    <row r="32" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" s="15"/>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -9577,7 +9587,7 @@
       <c r="BN32" s="1"/>
       <c r="BO32" s="1"/>
     </row>
-    <row r="33" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -9646,7 +9656,7 @@
       <c r="BN33" s="1"/>
       <c r="BO33" s="1"/>
     </row>
-    <row r="34" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="5"/>
       <c r="C34" s="2"/>
@@ -9715,7 +9725,7 @@
       <c r="BN34" s="1"/>
       <c r="BO34" s="1"/>
     </row>
-    <row r="35" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="5"/>
       <c r="C35" s="2"/>
@@ -9784,7 +9794,7 @@
       <c r="BN35" s="1"/>
       <c r="BO35" s="1"/>
     </row>
-    <row r="36" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="5"/>
       <c r="C36" s="2"/>
@@ -9853,7 +9863,7 @@
       <c r="BN36" s="1"/>
       <c r="BO36" s="1"/>
     </row>
-    <row r="37" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="5"/>
       <c r="C37" s="2"/>
@@ -9922,7 +9932,7 @@
       <c r="BN37" s="1"/>
       <c r="BO37" s="1"/>
     </row>
-    <row r="38" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
       <c r="B38" s="5"/>
       <c r="C38" s="2"/>
@@ -9991,7 +10001,7 @@
       <c r="BN38" s="1"/>
       <c r="BO38" s="1"/>
     </row>
-    <row r="39" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
       <c r="B39" s="5"/>
       <c r="C39" s="2"/>
@@ -10060,7 +10070,7 @@
       <c r="BN39" s="1"/>
       <c r="BO39" s="1"/>
     </row>
-    <row r="40" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
       <c r="B40" s="5"/>
       <c r="C40" s="2"/>
@@ -10129,7 +10139,7 @@
       <c r="BN40" s="1"/>
       <c r="BO40" s="1"/>
     </row>
-    <row r="41" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
       <c r="B41" s="5"/>
       <c r="C41" s="2"/>
@@ -10198,7 +10208,7 @@
       <c r="BN41" s="1"/>
       <c r="BO41" s="1"/>
     </row>
-    <row r="42" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
       <c r="B42" s="5"/>
       <c r="C42" s="2"/>
@@ -10267,7 +10277,7 @@
       <c r="BN42" s="1"/>
       <c r="BO42" s="1"/>
     </row>
-    <row r="43" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="5"/>
       <c r="C43" s="2"/>
@@ -10336,7 +10346,7 @@
       <c r="BN43" s="1"/>
       <c r="BO43" s="1"/>
     </row>
-    <row r="44" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A44" s="3"/>
       <c r="B44" s="5"/>
       <c r="C44" s="2"/>
@@ -10405,7 +10415,7 @@
       <c r="BN44" s="1"/>
       <c r="BO44" s="1"/>
     </row>
-    <row r="45" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" s="3"/>
       <c r="B45" s="5"/>
       <c r="C45" s="2"/>
@@ -10474,7 +10484,7 @@
       <c r="BN45" s="1"/>
       <c r="BO45" s="1"/>
     </row>
-    <row r="46" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" s="3"/>
       <c r="B46" s="5"/>
       <c r="C46" s="2"/>
@@ -10543,7 +10553,7 @@
       <c r="BN46" s="1"/>
       <c r="BO46" s="1"/>
     </row>
-    <row r="47" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
       <c r="B47" s="5"/>
       <c r="C47" s="2"/>
@@ -10612,7 +10622,7 @@
       <c r="BN47" s="1"/>
       <c r="BO47" s="1"/>
     </row>
-    <row r="48" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A48" s="3"/>
       <c r="B48" s="5"/>
       <c r="C48" s="2"/>
@@ -10681,7 +10691,7 @@
       <c r="BN48" s="1"/>
       <c r="BO48" s="1"/>
     </row>
-    <row r="49" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A49" s="3"/>
       <c r="B49" s="5"/>
       <c r="C49" s="2"/>
@@ -10750,7 +10760,7 @@
       <c r="BN49" s="1"/>
       <c r="BO49" s="1"/>
     </row>
-    <row r="50" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A50" s="3"/>
       <c r="B50" s="5"/>
       <c r="C50" s="2"/>
@@ -10819,7 +10829,7 @@
       <c r="BN50" s="1"/>
       <c r="BO50" s="1"/>
     </row>
-    <row r="51" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A51" s="3"/>
       <c r="B51" s="5"/>
       <c r="C51" s="2"/>
@@ -10888,7 +10898,7 @@
       <c r="BN51" s="1"/>
       <c r="BO51" s="1"/>
     </row>
-    <row r="52" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
       <c r="B52" s="5"/>
       <c r="C52" s="2"/>
@@ -10957,7 +10967,7 @@
       <c r="BN52" s="1"/>
       <c r="BO52" s="1"/>
     </row>
-    <row r="53" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A53" s="3"/>
       <c r="B53" s="5"/>
       <c r="C53" s="2"/>
@@ -11026,7 +11036,7 @@
       <c r="BN53" s="1"/>
       <c r="BO53" s="1"/>
     </row>
-    <row r="54" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A54" s="3"/>
       <c r="B54" s="5"/>
       <c r="C54" s="2"/>
@@ -11095,7 +11105,7 @@
       <c r="BN54" s="1"/>
       <c r="BO54" s="1"/>
     </row>
-    <row r="55" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A55" s="3"/>
       <c r="B55" s="5"/>
       <c r="C55" s="2"/>
@@ -11164,7 +11174,7 @@
       <c r="BN55" s="1"/>
       <c r="BO55" s="1"/>
     </row>
-    <row r="56" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A56" s="3"/>
       <c r="B56" s="5"/>
       <c r="C56" s="2"/>
@@ -11233,7 +11243,7 @@
       <c r="BN56" s="1"/>
       <c r="BO56" s="1"/>
     </row>
-    <row r="57" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A57" s="3"/>
       <c r="B57" s="5"/>
       <c r="C57" s="2"/>
@@ -11302,7 +11312,7 @@
       <c r="BN57" s="1"/>
       <c r="BO57" s="1"/>
     </row>
-    <row r="58" spans="1:67" ht="19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:67" ht="18" x14ac:dyDescent="0.35">
       <c r="A58" s="3"/>
       <c r="B58" s="5"/>
       <c r="C58" s="2"/>
@@ -11386,30 +11396,30 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" customWidth="1"/>
-    <col min="7" max="7" width="22.5" customWidth="1"/>
+    <col min="7" max="7" width="22.44140625" customWidth="1"/>
     <col min="8" max="8" width="20.6640625" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" customWidth="1"/>
-    <col min="10" max="10" width="13.83203125" customWidth="1"/>
-    <col min="11" max="11" width="15.5" customWidth="1"/>
-    <col min="12" max="12" width="92.1640625" customWidth="1"/>
-    <col min="14" max="14" width="10.83203125" customWidth="1"/>
-    <col min="15" max="15" width="23.5" customWidth="1"/>
-    <col min="16" max="16" width="11.83203125" customWidth="1"/>
-    <col min="17" max="17" width="14.83203125" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.77734375" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" customWidth="1"/>
+    <col min="12" max="12" width="92.109375" customWidth="1"/>
+    <col min="14" max="14" width="10.77734375" customWidth="1"/>
+    <col min="15" max="15" width="23.44140625" customWidth="1"/>
+    <col min="16" max="16" width="11.77734375" customWidth="1"/>
+    <col min="17" max="17" width="14.77734375" customWidth="1"/>
     <col min="18" max="18" width="13.33203125" customWidth="1"/>
-    <col min="19" max="19" width="14.83203125" customWidth="1"/>
+    <col min="19" max="19" width="14.77734375" customWidth="1"/>
     <col min="20" max="20" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -11427,7 +11437,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" ht="26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A2" s="2"/>
       <c r="B2" s="27" t="s">
         <v>66</v>
@@ -11445,7 +11455,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -11461,7 +11471,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:16" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="30" t="s">
@@ -11497,7 +11507,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:16" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="31" t="s">
         <v>13</v>
@@ -11533,7 +11543,7 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="1:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2"/>
       <c r="B6" s="28"/>
       <c r="C6" s="28">
@@ -11567,7 +11577,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="1:16" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="31" t="s">
         <v>16</v>
@@ -11603,7 +11613,7 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="28"/>
       <c r="C8" s="28">
@@ -11637,7 +11647,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="28"/>
       <c r="C9" s="28">
@@ -11671,7 +11681,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2"/>
       <c r="B10" s="54"/>
       <c r="C10" s="54">
@@ -11705,7 +11715,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="56"/>
       <c r="C11" s="55">
@@ -11739,7 +11749,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="2"/>
       <c r="B12" s="33"/>
       <c r="C12" s="55">
@@ -11773,7 +11783,7 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="56"/>
       <c r="C13" s="57">
@@ -11807,7 +11817,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2"/>
       <c r="B14" s="33"/>
       <c r="C14" s="55">
@@ -11841,7 +11851,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="56"/>
       <c r="C15" s="57">
@@ -11875,7 +11885,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="2"/>
       <c r="B16" s="35"/>
       <c r="C16" s="59">
@@ -11909,7 +11919,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="1:16" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="31" t="s">
         <v>122</v>
@@ -11945,7 +11955,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="1:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2"/>
       <c r="B18" s="32"/>
       <c r="C18" s="32">
@@ -11981,7 +11991,7 @@
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
     </row>
-    <row r="19" spans="1:16" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
@@ -11990,7 +12000,7 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
     </row>
-    <row r="20" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -11999,7 +12009,7 @@
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
     </row>
-    <row r="21" spans="1:16" ht="26" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B21" s="27" t="s">
         <v>72</v>
       </c>
@@ -12011,7 +12021,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -12021,7 +12031,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:16" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="2"/>
       <c r="C23" s="30" t="s">
         <v>4</v>
@@ -12054,7 +12064,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B24" s="31" t="s">
         <v>13</v>
       </c>
@@ -12089,7 +12099,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B25" s="28"/>
       <c r="C25" s="28">
         <v>20.7</v>
@@ -12122,7 +12132,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B26" s="31" t="s">
         <v>16</v>
       </c>
@@ -12157,7 +12167,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="B27" s="28"/>
       <c r="C27" s="28">
         <v>20.7</v>
@@ -12190,7 +12200,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="B28" s="28"/>
       <c r="C28" s="28">
         <v>20.7</v>
@@ -12223,7 +12233,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="B29" s="28"/>
       <c r="C29" s="28">
         <v>20.7</v>
@@ -12256,7 +12266,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="B30" s="28"/>
       <c r="C30" s="28">
         <v>20.7</v>
@@ -12289,7 +12299,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B31" s="54"/>
       <c r="C31" s="54">
         <v>20.7</v>
@@ -12322,7 +12332,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="B32" s="56"/>
       <c r="C32" s="55">
         <v>20.7</v>
@@ -12355,7 +12365,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="2:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B33" s="64"/>
       <c r="C33" s="65">
         <v>20.7</v>
@@ -12386,7 +12396,7 @@
       </c>
       <c r="L33" s="67"/>
     </row>
-    <row r="34" spans="2:12" ht="19" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12" ht="18" x14ac:dyDescent="0.35">
       <c r="B34" s="33"/>
       <c r="C34" s="55">
         <v>20.7</v>
@@ -12419,7 +12429,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="35" spans="2:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="33"/>
       <c r="C35" s="55">
         <v>20.7</v>
@@ -12450,7 +12460,7 @@
       </c>
       <c r="L35" s="61"/>
     </row>
-    <row r="36" spans="2:12" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B36" s="31" t="s">
         <v>122</v>
       </c>
@@ -12485,7 +12495,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="37" spans="2:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B37" s="32"/>
       <c r="C37" s="32">
         <v>20.7</v>
@@ -12518,7 +12528,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="38" spans="2:12" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -12533,14 +12543,14 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>158</v>
       </c>
@@ -12566,7 +12576,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>145.69999999999999</v>
       </c>

</xml_diff>

<commit_message>
Aggiunto al file Excel il calcolo del rate di sorgente e fascio e il calcolo del gain
</commit_message>
<xml_diff>
--- a/Caratterizzazione_THGEM.xlsx
+++ b/Caratterizzazione_THGEM.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peppe\Desktop\LaTex\Report_THGEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F1990F-FDCA-4281-9964-4010DFAB0249}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF779330-599F-463A-8214-2FC4884C3A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{ACFC7C87-C28D-4487-B063-88156E979354}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{ACFC7C87-C28D-4487-B063-88156E979354}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
     <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
+    <sheet name="2° test con fascio" sheetId="3" r:id="rId3"/>
+    <sheet name="Rate sorgente" sheetId="5" r:id="rId4"/>
+    <sheet name="Calcolo gain" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="132">
   <si>
     <t>DATA</t>
   </si>
@@ -655,6 +658,144 @@
   <si>
     <t>Vind=50        VTG=160</t>
   </si>
+  <si>
+    <t>G = gain</t>
+  </si>
+  <si>
+    <t>Ian = corrente anodo</t>
+  </si>
+  <si>
+    <t>Iprim = corrente part primarie</t>
+  </si>
+  <si>
+    <t>ne = num elettr</t>
+  </si>
+  <si>
+    <t>R = rate</t>
+  </si>
+  <si>
+    <t>c = fatt convers elettr-Coulomb</t>
+  </si>
+  <si>
+    <t>G = Ian/Iprim = Ian/(ne*R*c)</t>
+  </si>
+  <si>
+    <t>Iprim = ne*R*c</t>
+  </si>
+  <si>
+    <t>MXFC1 (pA)</t>
+  </si>
+  <si>
+    <t>TeBeFC (pA)</t>
+  </si>
+  <si>
+    <t>I_est (pA)</t>
+  </si>
+  <si>
+    <t>Target thick. (mg/cm2)</t>
+  </si>
+  <si>
+    <t>Rate_phdiode (pps)</t>
+  </si>
+  <si>
+    <t>NR</t>
+  </si>
+  <si>
+    <t>Target thick. (atoms/cm2)</t>
+  </si>
+  <si>
+    <t>M_at Au197 (amu)</t>
+  </si>
+  <si>
+    <t>M_at Au197 (g)</t>
+  </si>
+  <si>
+    <t>Flux (ppA)</t>
+  </si>
+  <si>
+    <t>Carica elettr. (C)</t>
+  </si>
+  <si>
+    <t>Elettr. in 1 C</t>
+  </si>
+  <si>
+    <t>Elettr. in 1 pC</t>
+  </si>
+  <si>
+    <t>dist target-rivel (cm)</t>
+  </si>
+  <si>
+    <t>Area (cm2)</t>
+  </si>
+  <si>
+    <t>Omega</t>
+  </si>
+  <si>
+    <t>Rate = Flux*Target thick*Ruth diff cross section*Omega</t>
+  </si>
+  <si>
+    <t>Ruth diff cross section a 30° nel LAB (mb/sr) LISE</t>
+  </si>
+  <si>
+    <t>Ruth diff cross section a 30° nel LAB (cm2/sr) LISE</t>
+  </si>
+  <si>
+    <t>c = Elettr. in 1 C</t>
+  </si>
+  <si>
+    <t>Perdita energia ( MeV)</t>
+  </si>
+  <si>
+    <t>Energia ionizz isobutano (eV)</t>
+  </si>
+  <si>
+    <t>ne</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Ian (nA)</t>
+  </si>
+  <si>
+    <t>R (pps)</t>
+  </si>
+  <si>
+    <t>Ian (pps)</t>
+  </si>
+  <si>
+    <t>Rate_calc TeBeFC (pps)</t>
+  </si>
+  <si>
+    <t>Rate_calc MXFC1 (pps)</t>
+  </si>
+  <si>
+    <t>Flux MXFC1 (pps)</t>
+  </si>
+  <si>
+    <t>Flux TeBeFC (pps)</t>
+  </si>
+  <si>
+    <t>Attività sorgente (kBq)</t>
+  </si>
+  <si>
+    <t>Distanza sorg-diaframma (mm)</t>
+  </si>
+  <si>
+    <t>Raggio diaframma (mm)</t>
+  </si>
+  <si>
+    <t>Attività sorg (decad/s)</t>
+  </si>
+  <si>
+    <t>Semi-apertura cono (rad)</t>
+  </si>
+  <si>
+    <t>Omega cono (sr)</t>
+  </si>
+  <si>
+    <t>Rate (pps)</t>
+  </si>
 </sst>
 </file>
 
@@ -663,7 +804,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -719,6 +860,21 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -746,7 +902,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -828,11 +984,198 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -943,6 +1286,99 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5326,7 +5762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838DA34D-F765-43A5-B43B-778E7D45A2A4}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -5974,4 +6410,2486 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13CF5F27-5E79-4739-BBEA-C2285C06A699}">
+  <dimension ref="A1:S35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" customWidth="1"/>
+    <col min="8" max="8" width="24.21875" customWidth="1"/>
+    <col min="9" max="9" width="21.44140625" customWidth="1"/>
+    <col min="10" max="10" width="22.44140625" customWidth="1"/>
+    <col min="11" max="11" width="23.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" s="49" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="K1" s="50" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="51">
+        <v>900</v>
+      </c>
+      <c r="B2" s="47">
+        <v>400</v>
+      </c>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47">
+        <f>B2/8</f>
+        <v>50</v>
+      </c>
+      <c r="E2" s="56">
+        <f>D2*$E$14</f>
+        <v>312109862.67166042</v>
+      </c>
+      <c r="F2" s="56">
+        <f>(A2/8)*$E$14</f>
+        <v>702247191.01123595</v>
+      </c>
+      <c r="G2" s="47">
+        <v>9.6</v>
+      </c>
+      <c r="H2" s="47">
+        <f>(G2/1000)/$B$14</f>
+        <v>2.9360473829113475E+19</v>
+      </c>
+      <c r="I2" s="62">
+        <f>E2*H2*$C$21*$C$25</f>
+        <v>3215.0003336359177</v>
+      </c>
+      <c r="J2" s="62">
+        <f>F2*H2*$C$21*$C$25</f>
+        <v>7233.7507506808142</v>
+      </c>
+      <c r="K2" s="52">
+        <v>13.4</v>
+      </c>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="51">
+        <v>680</v>
+      </c>
+      <c r="B3" s="47">
+        <v>280</v>
+      </c>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47">
+        <f t="shared" ref="D3:D10" si="0">B3/8</f>
+        <v>35</v>
+      </c>
+      <c r="E3" s="56">
+        <f t="shared" ref="E3:E10" si="1">D3*$E$14</f>
+        <v>218476903.87016231</v>
+      </c>
+      <c r="F3" s="56">
+        <f t="shared" ref="F3:F10" si="2">(A3/8)*$E$14</f>
+        <v>530586766.54182273</v>
+      </c>
+      <c r="G3" s="47">
+        <v>9.6</v>
+      </c>
+      <c r="H3" s="47">
+        <f t="shared" ref="H3:H10" si="3">(G3/1000)/$B$14</f>
+        <v>2.9360473829113475E+19</v>
+      </c>
+      <c r="I3" s="62">
+        <f t="shared" ref="I3:I10" si="4">E3*H3*$C$21*$C$25</f>
+        <v>2250.5002335451427</v>
+      </c>
+      <c r="J3" s="62">
+        <f t="shared" ref="J3:J10" si="5">F3*H3*$C$21*$C$25</f>
+        <v>5465.5005671810595</v>
+      </c>
+      <c r="K3" s="52">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43"/>
+      <c r="S3" s="43"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="51">
+        <v>220</v>
+      </c>
+      <c r="B4" s="47">
+        <v>100</v>
+      </c>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+      <c r="E4" s="56">
+        <f t="shared" si="1"/>
+        <v>78027465.667915106</v>
+      </c>
+      <c r="F4" s="56">
+        <f t="shared" si="2"/>
+        <v>171660424.46941325</v>
+      </c>
+      <c r="G4" s="47">
+        <v>9.6</v>
+      </c>
+      <c r="H4" s="47">
+        <f t="shared" si="3"/>
+        <v>2.9360473829113475E+19</v>
+      </c>
+      <c r="I4" s="62">
+        <f t="shared" si="4"/>
+        <v>803.75008340897944</v>
+      </c>
+      <c r="J4" s="62">
+        <f t="shared" si="5"/>
+        <v>1768.2501834997547</v>
+      </c>
+      <c r="K4" s="52">
+        <v>2.5</v>
+      </c>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="43"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="51">
+        <v>100</v>
+      </c>
+      <c r="B5" s="47">
+        <v>60</v>
+      </c>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="E5" s="56">
+        <f t="shared" si="1"/>
+        <v>46816479.400749065</v>
+      </c>
+      <c r="F5" s="56">
+        <f t="shared" si="2"/>
+        <v>78027465.667915106</v>
+      </c>
+      <c r="G5" s="47">
+        <v>9.6</v>
+      </c>
+      <c r="H5" s="47">
+        <f t="shared" si="3"/>
+        <v>2.9360473829113475E+19</v>
+      </c>
+      <c r="I5" s="62">
+        <f t="shared" si="4"/>
+        <v>482.25005004538758</v>
+      </c>
+      <c r="J5" s="62">
+        <f t="shared" si="5"/>
+        <v>803.75008340897944</v>
+      </c>
+      <c r="K5" s="52">
+        <v>1.6</v>
+      </c>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="43"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="51">
+        <v>100</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="47">
+        <v>45</v>
+      </c>
+      <c r="D6" s="47">
+        <f>C6/8</f>
+        <v>5.625</v>
+      </c>
+      <c r="E6" s="56">
+        <f t="shared" si="1"/>
+        <v>35112359.550561801</v>
+      </c>
+      <c r="F6" s="56">
+        <f t="shared" si="2"/>
+        <v>78027465.667915106</v>
+      </c>
+      <c r="G6" s="47">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="H6" s="47">
+        <f t="shared" si="3"/>
+        <v>2.9727479751977395E+18</v>
+      </c>
+      <c r="I6" s="62">
+        <f t="shared" si="4"/>
+        <v>36.620863175321624</v>
+      </c>
+      <c r="J6" s="62">
+        <f t="shared" si="5"/>
+        <v>81.379695945159156</v>
+      </c>
+      <c r="K6" s="52">
+        <v>0.2</v>
+      </c>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="43"/>
+      <c r="S6" s="43"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="51">
+        <v>250</v>
+      </c>
+      <c r="B7" s="47" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="47">
+        <v>110</v>
+      </c>
+      <c r="D7" s="47">
+        <f>C7/8</f>
+        <v>13.75</v>
+      </c>
+      <c r="E7" s="56">
+        <f t="shared" si="1"/>
+        <v>85830212.234706625</v>
+      </c>
+      <c r="F7" s="56">
+        <f t="shared" si="2"/>
+        <v>195068664.16978776</v>
+      </c>
+      <c r="G7" s="47">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="H7" s="47">
+        <f t="shared" si="3"/>
+        <v>2.9727479751977395E+18</v>
+      </c>
+      <c r="I7" s="62">
+        <f t="shared" si="4"/>
+        <v>89.517665539675093</v>
+      </c>
+      <c r="J7" s="62">
+        <f t="shared" si="5"/>
+        <v>203.44923986289791</v>
+      </c>
+      <c r="K7" s="52">
+        <v>0.3</v>
+      </c>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="43"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="43"/>
+      <c r="R7" s="43"/>
+      <c r="S7" s="43"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="51">
+        <v>680</v>
+      </c>
+      <c r="B8" s="47">
+        <v>300</v>
+      </c>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47">
+        <f t="shared" si="0"/>
+        <v>37.5</v>
+      </c>
+      <c r="E8" s="56">
+        <f t="shared" si="1"/>
+        <v>234082397.00374535</v>
+      </c>
+      <c r="F8" s="56">
+        <f t="shared" si="2"/>
+        <v>530586766.54182273</v>
+      </c>
+      <c r="G8" s="47">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="H8" s="47">
+        <f t="shared" si="3"/>
+        <v>2.9727479751977395E+18</v>
+      </c>
+      <c r="I8" s="62">
+        <f t="shared" si="4"/>
+        <v>244.13908783547751</v>
+      </c>
+      <c r="J8" s="62">
+        <f t="shared" si="5"/>
+        <v>553.38193242708235</v>
+      </c>
+      <c r="K8" s="52">
+        <v>1</v>
+      </c>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="43"/>
+      <c r="P8" s="43"/>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="43"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="51">
+        <v>250</v>
+      </c>
+      <c r="B9" s="47">
+        <v>150</v>
+      </c>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47">
+        <f t="shared" si="0"/>
+        <v>18.75</v>
+      </c>
+      <c r="E9" s="56">
+        <f t="shared" si="1"/>
+        <v>117041198.50187267</v>
+      </c>
+      <c r="F9" s="56">
+        <f t="shared" si="2"/>
+        <v>195068664.16978776</v>
+      </c>
+      <c r="G9" s="47">
+        <v>9.6</v>
+      </c>
+      <c r="H9" s="47">
+        <f t="shared" si="3"/>
+        <v>2.9360473829113475E+19</v>
+      </c>
+      <c r="I9" s="62">
+        <f t="shared" si="4"/>
+        <v>1205.625125113469</v>
+      </c>
+      <c r="J9" s="62">
+        <f t="shared" si="5"/>
+        <v>2009.3752085224485</v>
+      </c>
+      <c r="K9" s="52">
+        <v>3.4</v>
+      </c>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="43"/>
+      <c r="P9" s="43"/>
+      <c r="Q9" s="43"/>
+      <c r="R9" s="43"/>
+      <c r="S9" s="43"/>
+    </row>
+    <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="53">
+        <v>250</v>
+      </c>
+      <c r="B10" s="54">
+        <v>160</v>
+      </c>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E10" s="57">
+        <f t="shared" si="1"/>
+        <v>124843945.06866418</v>
+      </c>
+      <c r="F10" s="57">
+        <f t="shared" si="2"/>
+        <v>195068664.16978776</v>
+      </c>
+      <c r="G10" s="54">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="H10" s="54">
+        <f t="shared" si="3"/>
+        <v>2.9727479751977395E+18</v>
+      </c>
+      <c r="I10" s="70">
+        <f t="shared" si="4"/>
+        <v>130.20751351225468</v>
+      </c>
+      <c r="J10" s="70">
+        <f t="shared" si="5"/>
+        <v>203.44923986289791</v>
+      </c>
+      <c r="K10" s="55">
+        <v>0.3</v>
+      </c>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="43"/>
+      <c r="S10" s="43"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="43"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="43"/>
+      <c r="S11" s="43"/>
+    </row>
+    <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="43"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="43"/>
+      <c r="S12" s="43"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="48" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" s="69" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="72"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="43"/>
+      <c r="R13" s="43"/>
+      <c r="S13" s="43"/>
+    </row>
+    <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="53">
+        <v>196.97</v>
+      </c>
+      <c r="B14" s="54">
+        <f>A14*1.66*10^(-24)</f>
+        <v>3.2697020000000002E-22</v>
+      </c>
+      <c r="C14" s="54">
+        <f>1.602*10^(-19)</f>
+        <v>1.602E-19</v>
+      </c>
+      <c r="D14" s="54">
+        <f>1/C14</f>
+        <v>6.2421972534332088E+18</v>
+      </c>
+      <c r="E14" s="55">
+        <f>D14/10^(12)</f>
+        <v>6242197.2534332089</v>
+      </c>
+      <c r="F14" s="45"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="43"/>
+      <c r="S14" s="43"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="43"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="43"/>
+      <c r="O15" s="43"/>
+      <c r="P15" s="43"/>
+      <c r="Q15" s="43"/>
+      <c r="R15" s="43"/>
+      <c r="S15" s="43"/>
+    </row>
+    <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="43"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="43"/>
+      <c r="M16" s="43"/>
+      <c r="N16" s="43"/>
+      <c r="O16" s="43"/>
+      <c r="P16" s="43"/>
+      <c r="Q16" s="43"/>
+      <c r="R16" s="43"/>
+      <c r="S16" s="43"/>
+    </row>
+    <row r="17" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="58" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" s="59"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="43"/>
+      <c r="O17" s="43"/>
+      <c r="P17" s="43"/>
+      <c r="Q17" s="43"/>
+      <c r="R17" s="43"/>
+      <c r="S17" s="43"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="61"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="43"/>
+      <c r="M18" s="43"/>
+      <c r="N18" s="43"/>
+      <c r="O18" s="43"/>
+      <c r="P18" s="43"/>
+      <c r="Q18" s="43"/>
+      <c r="R18" s="43"/>
+      <c r="S18" s="43"/>
+    </row>
+    <row r="19" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="43"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="43"/>
+      <c r="O19" s="43"/>
+      <c r="P19" s="43"/>
+      <c r="Q19" s="43"/>
+      <c r="R19" s="43"/>
+      <c r="S19" s="43"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="63" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" s="64"/>
+      <c r="C20" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" s="64"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="43"/>
+      <c r="P20" s="43"/>
+      <c r="Q20" s="43"/>
+      <c r="R20" s="43"/>
+      <c r="S20" s="43"/>
+    </row>
+    <row r="21" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="66">
+        <f>5.98*10^3</f>
+        <v>5980</v>
+      </c>
+      <c r="B21" s="67"/>
+      <c r="C21" s="67">
+        <f>A21*10^(-27)</f>
+        <v>5.98E-24</v>
+      </c>
+      <c r="D21" s="67"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="43"/>
+      <c r="O21" s="43"/>
+      <c r="P21" s="43"/>
+      <c r="Q21" s="43"/>
+      <c r="R21" s="43"/>
+      <c r="S21" s="43"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" s="45"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="43"/>
+      <c r="P22" s="43"/>
+      <c r="Q22" s="43"/>
+      <c r="R22" s="43"/>
+      <c r="S22" s="43"/>
+    </row>
+    <row r="23" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="43"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="43"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="43"/>
+      <c r="O23" s="43"/>
+      <c r="P23" s="43"/>
+      <c r="Q23" s="43"/>
+      <c r="R23" s="43"/>
+      <c r="S23" s="43"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" s="48" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" s="49" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
+      <c r="K24" s="43"/>
+      <c r="L24" s="43"/>
+      <c r="M24" s="43"/>
+      <c r="N24" s="43"/>
+      <c r="O24" s="43"/>
+      <c r="P24" s="43"/>
+      <c r="Q24" s="43"/>
+      <c r="R24" s="43"/>
+      <c r="S24" s="43"/>
+    </row>
+    <row r="25" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="53">
+        <v>47</v>
+      </c>
+      <c r="B25" s="54">
+        <f>10.8*12</f>
+        <v>129.60000000000002</v>
+      </c>
+      <c r="C25" s="55">
+        <f>B25/A25^2</f>
+        <v>5.8669081032141253E-2</v>
+      </c>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="43"/>
+      <c r="O25" s="43"/>
+      <c r="P25" s="43"/>
+      <c r="Q25" s="43"/>
+      <c r="R25" s="43"/>
+      <c r="S25" s="43"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A26" s="43"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="43"/>
+      <c r="S26" s="43"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A27" s="43"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="43"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="43"/>
+      <c r="O27" s="43"/>
+      <c r="P27" s="43"/>
+      <c r="Q27" s="43"/>
+      <c r="R27" s="43"/>
+      <c r="S27" s="43"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A28" s="43"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="43"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="43"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="43"/>
+      <c r="P28" s="43"/>
+      <c r="Q28" s="43"/>
+      <c r="R28" s="43"/>
+      <c r="S28" s="43"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A29" s="43"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="43"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="43"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="43"/>
+      <c r="P29" s="43"/>
+      <c r="Q29" s="43"/>
+      <c r="R29" s="43"/>
+      <c r="S29" s="43"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A30" s="43"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="43"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="43"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="43"/>
+      <c r="P30" s="43"/>
+      <c r="Q30" s="43"/>
+      <c r="R30" s="43"/>
+      <c r="S30" s="43"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A31" s="43"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="43"/>
+      <c r="K31" s="43"/>
+      <c r="L31" s="43"/>
+      <c r="M31" s="43"/>
+      <c r="N31" s="43"/>
+      <c r="O31" s="43"/>
+      <c r="P31" s="43"/>
+      <c r="Q31" s="43"/>
+      <c r="R31" s="43"/>
+      <c r="S31" s="43"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A32" s="43"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="43"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="43"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="43"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="43"/>
+      <c r="P32" s="43"/>
+      <c r="Q32" s="43"/>
+      <c r="R32" s="43"/>
+      <c r="S32" s="43"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A33" s="43"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="43"/>
+      <c r="L33" s="43"/>
+      <c r="M33" s="43"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="43"/>
+      <c r="P33" s="43"/>
+      <c r="Q33" s="43"/>
+      <c r="R33" s="43"/>
+      <c r="S33" s="43"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A34" s="43"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="43"/>
+      <c r="K34" s="43"/>
+      <c r="L34" s="43"/>
+      <c r="M34" s="43"/>
+      <c r="N34" s="43"/>
+      <c r="O34" s="43"/>
+      <c r="P34" s="43"/>
+      <c r="Q34" s="43"/>
+      <c r="R34" s="43"/>
+      <c r="S34" s="43"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A35" s="43"/>
+      <c r="B35" s="43"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="43"/>
+      <c r="K35" s="43"/>
+      <c r="L35" s="43"/>
+      <c r="M35" s="43"/>
+      <c r="N35" s="43"/>
+      <c r="O35" s="43"/>
+      <c r="P35" s="43"/>
+      <c r="Q35" s="43"/>
+      <c r="R35" s="43"/>
+      <c r="S35" s="43"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C512A73-7FF1-4E2F-9CF1-BB7BA243F606}">
+  <dimension ref="A1:X28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" customWidth="1"/>
+    <col min="6" max="6" width="22.5546875" customWidth="1"/>
+    <col min="7" max="7" width="21.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A1" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A2" s="47">
+        <v>55</v>
+      </c>
+      <c r="B2" s="47">
+        <f>A2*1000</f>
+        <v>55000</v>
+      </c>
+      <c r="C2" s="47">
+        <v>25.5</v>
+      </c>
+      <c r="D2" s="47">
+        <f>6.5/2</f>
+        <v>3.25</v>
+      </c>
+      <c r="E2" s="47">
+        <f>ATAN(D2/C2)</f>
+        <v>0.12676753510136199</v>
+      </c>
+      <c r="F2" s="47">
+        <f>2*PI()*(1-COS(E2))</f>
+        <v>5.0417846718221082E-2</v>
+      </c>
+      <c r="G2" s="47">
+        <f>B2*F2/(4*PI())</f>
+        <v>220.66686194449539</v>
+      </c>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="43"/>
+      <c r="V2" s="43"/>
+      <c r="W2" s="43"/>
+      <c r="X2" s="43"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="43"/>
+      <c r="V3" s="43"/>
+      <c r="W3" s="43"/>
+      <c r="X3" s="43"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="43"/>
+      <c r="T4" s="43"/>
+      <c r="U4" s="43"/>
+      <c r="V4" s="43"/>
+      <c r="W4" s="43"/>
+      <c r="X4" s="43"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A5" s="43"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="43"/>
+      <c r="T5" s="43"/>
+      <c r="U5" s="43"/>
+      <c r="V5" s="43"/>
+      <c r="W5" s="43"/>
+      <c r="X5" s="43"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A6" s="43"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="43"/>
+      <c r="S6" s="43"/>
+      <c r="T6" s="43"/>
+      <c r="U6" s="43"/>
+      <c r="V6" s="43"/>
+      <c r="W6" s="43"/>
+      <c r="X6" s="43"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A7" s="43"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="43"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="43"/>
+      <c r="R7" s="43"/>
+      <c r="S7" s="43"/>
+      <c r="T7" s="43"/>
+      <c r="U7" s="43"/>
+      <c r="V7" s="43"/>
+      <c r="W7" s="43"/>
+      <c r="X7" s="43"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A8" s="43"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="43"/>
+      <c r="P8" s="43"/>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="43"/>
+      <c r="T8" s="43"/>
+      <c r="U8" s="43"/>
+      <c r="V8" s="43"/>
+      <c r="W8" s="43"/>
+      <c r="X8" s="43"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A9" s="43"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="43"/>
+      <c r="P9" s="43"/>
+      <c r="Q9" s="43"/>
+      <c r="R9" s="43"/>
+      <c r="S9" s="43"/>
+      <c r="T9" s="43"/>
+      <c r="U9" s="43"/>
+      <c r="V9" s="43"/>
+      <c r="W9" s="43"/>
+      <c r="X9" s="43"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A10" s="43"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="43"/>
+      <c r="S10" s="43"/>
+      <c r="T10" s="43"/>
+      <c r="U10" s="43"/>
+      <c r="V10" s="43"/>
+      <c r="W10" s="43"/>
+      <c r="X10" s="43"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A11" s="43"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="43"/>
+      <c r="S11" s="43"/>
+      <c r="T11" s="43"/>
+      <c r="U11" s="43"/>
+      <c r="V11" s="43"/>
+      <c r="W11" s="43"/>
+      <c r="X11" s="43"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A12" s="43"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="43"/>
+      <c r="S12" s="43"/>
+      <c r="T12" s="43"/>
+      <c r="U12" s="43"/>
+      <c r="V12" s="43"/>
+      <c r="W12" s="43"/>
+      <c r="X12" s="43"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A13" s="43"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="43"/>
+      <c r="R13" s="43"/>
+      <c r="S13" s="43"/>
+      <c r="T13" s="43"/>
+      <c r="U13" s="43"/>
+      <c r="V13" s="43"/>
+      <c r="W13" s="43"/>
+      <c r="X13" s="43"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A14" s="43"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="43"/>
+      <c r="S14" s="43"/>
+      <c r="T14" s="43"/>
+      <c r="U14" s="43"/>
+      <c r="V14" s="43"/>
+      <c r="W14" s="43"/>
+      <c r="X14" s="43"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A15" s="43"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="43"/>
+      <c r="O15" s="43"/>
+      <c r="P15" s="43"/>
+      <c r="Q15" s="43"/>
+      <c r="R15" s="43"/>
+      <c r="S15" s="43"/>
+      <c r="T15" s="43"/>
+      <c r="U15" s="43"/>
+      <c r="V15" s="43"/>
+      <c r="W15" s="43"/>
+      <c r="X15" s="43"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A16" s="43"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="43"/>
+      <c r="M16" s="43"/>
+      <c r="N16" s="43"/>
+      <c r="O16" s="43"/>
+      <c r="P16" s="43"/>
+      <c r="Q16" s="43"/>
+      <c r="R16" s="43"/>
+      <c r="S16" s="43"/>
+      <c r="T16" s="43"/>
+      <c r="U16" s="43"/>
+      <c r="V16" s="43"/>
+      <c r="W16" s="43"/>
+      <c r="X16" s="43"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A17" s="43"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="43"/>
+      <c r="O17" s="43"/>
+      <c r="P17" s="43"/>
+      <c r="Q17" s="43"/>
+      <c r="R17" s="43"/>
+      <c r="S17" s="43"/>
+      <c r="T17" s="43"/>
+      <c r="U17" s="43"/>
+      <c r="V17" s="43"/>
+      <c r="W17" s="43"/>
+      <c r="X17" s="43"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A18" s="43"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="43"/>
+      <c r="M18" s="43"/>
+      <c r="N18" s="43"/>
+      <c r="O18" s="43"/>
+      <c r="P18" s="43"/>
+      <c r="Q18" s="43"/>
+      <c r="R18" s="43"/>
+      <c r="S18" s="43"/>
+      <c r="T18" s="43"/>
+      <c r="U18" s="43"/>
+      <c r="V18" s="43"/>
+      <c r="W18" s="43"/>
+      <c r="X18" s="43"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A19" s="43"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="43"/>
+      <c r="O19" s="43"/>
+      <c r="P19" s="43"/>
+      <c r="Q19" s="43"/>
+      <c r="R19" s="43"/>
+      <c r="S19" s="43"/>
+      <c r="T19" s="43"/>
+      <c r="U19" s="43"/>
+      <c r="V19" s="43"/>
+      <c r="W19" s="43"/>
+      <c r="X19" s="43"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A20" s="43"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="43"/>
+      <c r="P20" s="43"/>
+      <c r="Q20" s="43"/>
+      <c r="R20" s="43"/>
+      <c r="S20" s="43"/>
+      <c r="T20" s="43"/>
+      <c r="U20" s="43"/>
+      <c r="V20" s="43"/>
+      <c r="W20" s="43"/>
+      <c r="X20" s="43"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A21" s="43"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="43"/>
+      <c r="O21" s="43"/>
+      <c r="P21" s="43"/>
+      <c r="Q21" s="43"/>
+      <c r="R21" s="43"/>
+      <c r="S21" s="43"/>
+      <c r="T21" s="43"/>
+      <c r="U21" s="43"/>
+      <c r="V21" s="43"/>
+      <c r="W21" s="43"/>
+      <c r="X21" s="43"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A22" s="43"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="43"/>
+      <c r="P22" s="43"/>
+      <c r="Q22" s="43"/>
+      <c r="R22" s="43"/>
+      <c r="S22" s="43"/>
+      <c r="T22" s="43"/>
+      <c r="U22" s="43"/>
+      <c r="V22" s="43"/>
+      <c r="W22" s="43"/>
+      <c r="X22" s="43"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A23" s="43"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="43"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="43"/>
+      <c r="O23" s="43"/>
+      <c r="P23" s="43"/>
+      <c r="Q23" s="43"/>
+      <c r="R23" s="43"/>
+      <c r="S23" s="43"/>
+      <c r="T23" s="43"/>
+      <c r="U23" s="43"/>
+      <c r="V23" s="43"/>
+      <c r="W23" s="43"/>
+      <c r="X23" s="43"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A24" s="43"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
+      <c r="K24" s="43"/>
+      <c r="L24" s="43"/>
+      <c r="M24" s="43"/>
+      <c r="N24" s="43"/>
+      <c r="O24" s="43"/>
+      <c r="P24" s="43"/>
+      <c r="Q24" s="43"/>
+      <c r="R24" s="43"/>
+      <c r="S24" s="43"/>
+      <c r="T24" s="43"/>
+      <c r="U24" s="43"/>
+      <c r="V24" s="43"/>
+      <c r="W24" s="43"/>
+      <c r="X24" s="43"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A25" s="43"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="43"/>
+      <c r="O25" s="43"/>
+      <c r="P25" s="43"/>
+      <c r="Q25" s="43"/>
+      <c r="R25" s="43"/>
+      <c r="S25" s="43"/>
+      <c r="T25" s="43"/>
+      <c r="U25" s="43"/>
+      <c r="V25" s="43"/>
+      <c r="W25" s="43"/>
+      <c r="X25" s="43"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A26" s="43"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="43"/>
+      <c r="S26" s="43"/>
+      <c r="T26" s="43"/>
+      <c r="U26" s="43"/>
+      <c r="V26" s="43"/>
+      <c r="W26" s="43"/>
+      <c r="X26" s="43"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A27" s="43"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="43"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="43"/>
+      <c r="O27" s="43"/>
+      <c r="P27" s="43"/>
+      <c r="Q27" s="43"/>
+      <c r="R27" s="43"/>
+      <c r="S27" s="43"/>
+      <c r="T27" s="43"/>
+      <c r="U27" s="43"/>
+      <c r="V27" s="43"/>
+      <c r="W27" s="43"/>
+      <c r="X27" s="43"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A28" s="43"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="43"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="43"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="43"/>
+      <c r="P28" s="43"/>
+      <c r="Q28" s="43"/>
+      <c r="R28" s="43"/>
+      <c r="S28" s="43"/>
+      <c r="T28" s="43"/>
+      <c r="U28" s="43"/>
+      <c r="V28" s="43"/>
+      <c r="W28" s="43"/>
+      <c r="X28" s="43"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62375537-B4AB-4D3C-B99B-4547CB7785F8}">
+  <dimension ref="A1:P29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" customWidth="1"/>
+    <col min="3" max="3" width="27.5546875" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" customWidth="1"/>
+    <col min="6" max="6" width="26.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+    </row>
+    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="43"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+    </row>
+    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="45"/>
+      <c r="B3" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+    </row>
+    <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+    </row>
+    <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="43"/>
+      <c r="B5" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="43"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
+    </row>
+    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="43"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="43"/>
+      <c r="P7" s="43"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="43"/>
+      <c r="D8" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="43"/>
+      <c r="P8" s="43"/>
+    </row>
+    <row r="9" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="54">
+        <f>1.602*10^(-19)</f>
+        <v>1.602E-19</v>
+      </c>
+      <c r="B9" s="54">
+        <f>1/A9</f>
+        <v>6.2421972534332088E+18</v>
+      </c>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E9" s="43">
+        <v>23.4</v>
+      </c>
+      <c r="F9" s="43">
+        <f>(D9*10^6)/E9</f>
+        <v>47008.547008547008</v>
+      </c>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="43"/>
+      <c r="P9" s="43"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="43"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="43"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="43"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="43">
+        <v>50</v>
+      </c>
+      <c r="B13" s="43">
+        <f>A13*10^(-9)*$B$9</f>
+        <v>312109862671.66046</v>
+      </c>
+      <c r="C13" s="43">
+        <v>3215</v>
+      </c>
+      <c r="D13" s="71">
+        <f>B13/(F9*C13)</f>
+        <v>2065.1408982092053</v>
+      </c>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="43"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="43">
+        <v>50</v>
+      </c>
+      <c r="B14" s="43">
+        <f>A14*10^(-9)*$B$9</f>
+        <v>312109862671.66046</v>
+      </c>
+      <c r="C14" s="43">
+        <v>7233</v>
+      </c>
+      <c r="D14" s="71">
+        <f>B14/($F$9*C14)</f>
+        <v>917.93557137323319</v>
+      </c>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="43"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="43">
+        <v>220</v>
+      </c>
+      <c r="D15" s="71">
+        <f>B15/($F$9*C15)</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="43"/>
+      <c r="O15" s="43"/>
+      <c r="P15" s="43"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="43"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="43"/>
+      <c r="M16" s="43"/>
+      <c r="N16" s="43"/>
+      <c r="O16" s="43"/>
+      <c r="P16" s="43"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="43"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="43"/>
+      <c r="O17" s="43"/>
+      <c r="P17" s="43"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="43"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="43"/>
+      <c r="M18" s="43"/>
+      <c r="N18" s="43"/>
+      <c r="O18" s="43"/>
+      <c r="P18" s="43"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="43"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="43"/>
+      <c r="O19" s="43"/>
+      <c r="P19" s="43"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="43"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="43"/>
+      <c r="P20" s="43"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="43"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="43"/>
+      <c r="O21" s="43"/>
+      <c r="P21" s="43"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="43"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="43"/>
+      <c r="P22" s="43"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="43"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="43"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="43"/>
+      <c r="O23" s="43"/>
+      <c r="P23" s="43"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="43"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
+      <c r="K24" s="43"/>
+      <c r="L24" s="43"/>
+      <c r="M24" s="43"/>
+      <c r="N24" s="43"/>
+      <c r="O24" s="43"/>
+      <c r="P24" s="43"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="43"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="43"/>
+      <c r="O25" s="43"/>
+      <c r="P25" s="43"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="43"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="43"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="43"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="43"/>
+      <c r="O27" s="43"/>
+      <c r="P27" s="43"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="43"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="43"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="43"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="43"/>
+      <c r="P28" s="43"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="43"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="43"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="43"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="43"/>
+      <c r="P29" s="43"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>